<commit_message>
Se modifico de formato a la columna fecha
</commit_message>
<xml_diff>
--- a/data/ep_mes_2025.xlsx
+++ b/data/ep_mes_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6. Código\seguimiento_presupuestal_unsch_streamlit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723E0625-AB78-4A07-AA5F-40E0C967A69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911742ED-A3BB-4DD9-8DA6-2A7A778B2913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -882,8 +882,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1166,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,7 +1256,7 @@
       <c r="Y1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1335,7 +1336,7 @@
       <c r="Y2">
         <v>6603.52</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="1">
         <v>45677.679732025463</v>
       </c>
     </row>
@@ -1415,7 +1416,7 @@
       <c r="Y3">
         <v>-1343.89</v>
       </c>
-      <c r="Z3">
+      <c r="Z3" s="1">
         <v>45677.679732025463</v>
       </c>
     </row>
@@ -1495,7 +1496,7 @@
       <c r="Y4">
         <v>320</v>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="1">
         <v>45680.692369212964</v>
       </c>
     </row>
@@ -1575,7 +1576,7 @@
       <c r="Y5">
         <v>224</v>
       </c>
-      <c r="Z5">
+      <c r="Z5" s="1">
         <v>45688.687467557873</v>
       </c>
     </row>
@@ -1655,7 +1656,7 @@
       <c r="Y6">
         <v>-4</v>
       </c>
-      <c r="Z6">
+      <c r="Z6" s="1">
         <v>45688.687467557873</v>
       </c>
     </row>
@@ -1735,7 +1736,7 @@
       <c r="Y7">
         <v>320</v>
       </c>
-      <c r="Z7">
+      <c r="Z7" s="1">
         <v>45681.638071909721</v>
       </c>
     </row>
@@ -1815,7 +1816,7 @@
       <c r="Y8">
         <v>320</v>
       </c>
-      <c r="Z8">
+      <c r="Z8" s="1">
         <v>45681.638227083335</v>
       </c>
     </row>
@@ -1895,7 +1896,7 @@
       <c r="Y9">
         <v>-39</v>
       </c>
-      <c r="Z9">
+      <c r="Z9" s="1">
         <v>45681.638227083335</v>
       </c>
     </row>
@@ -1975,7 +1976,7 @@
       <c r="Y10">
         <v>224</v>
       </c>
-      <c r="Z10">
+      <c r="Z10" s="1">
         <v>45688.687400381947</v>
       </c>
     </row>
@@ -2055,7 +2056,7 @@
       <c r="Y11">
         <v>320</v>
       </c>
-      <c r="Z11">
+      <c r="Z11" s="1">
         <v>45681.638293171294</v>
       </c>
     </row>
@@ -2135,7 +2136,7 @@
       <c r="Y12">
         <v>-29</v>
       </c>
-      <c r="Z12">
+      <c r="Z12" s="1">
         <v>45681.638293171294</v>
       </c>
     </row>
@@ -2215,7 +2216,7 @@
       <c r="Y13">
         <v>224</v>
       </c>
-      <c r="Z13">
+      <c r="Z13" s="1">
         <v>45688.661467789352</v>
       </c>
     </row>
@@ -2295,7 +2296,7 @@
       <c r="Y14">
         <v>200</v>
       </c>
-      <c r="Z14">
+      <c r="Z14" s="1">
         <v>45698.605144363428</v>
       </c>
     </row>
@@ -2375,7 +2376,7 @@
       <c r="Y15">
         <v>640</v>
       </c>
-      <c r="Z15">
+      <c r="Z15" s="1">
         <v>45698.605144363428</v>
       </c>
     </row>
@@ -2455,7 +2456,7 @@
       <c r="Y16">
         <v>380</v>
       </c>
-      <c r="Z16">
+      <c r="Z16" s="1">
         <v>45700.41507318287</v>
       </c>
     </row>
@@ -2535,7 +2536,7 @@
       <c r="Y17">
         <v>200</v>
       </c>
-      <c r="Z17">
+      <c r="Z17" s="1">
         <v>45700.477851886571</v>
       </c>
     </row>
@@ -2615,7 +2616,7 @@
       <c r="Y18">
         <v>320</v>
       </c>
-      <c r="Z18">
+      <c r="Z18" s="1">
         <v>45700.477851886571</v>
       </c>
     </row>
@@ -2695,7 +2696,7 @@
       <c r="Y19">
         <v>200</v>
       </c>
-      <c r="Z19">
+      <c r="Z19" s="1">
         <v>45715.366732488423</v>
       </c>
     </row>
@@ -2775,7 +2776,7 @@
       <c r="Y20">
         <v>280</v>
       </c>
-      <c r="Z20">
+      <c r="Z20" s="1">
         <v>45715.366732488423</v>
       </c>
     </row>
@@ -2855,7 +2856,7 @@
       <c r="Y21">
         <v>200</v>
       </c>
-      <c r="Z21">
+      <c r="Z21" s="1">
         <v>45702.463211840281</v>
       </c>
     </row>
@@ -2935,7 +2936,7 @@
       <c r="Y22">
         <v>200</v>
       </c>
-      <c r="Z22">
+      <c r="Z22" s="1">
         <v>45702.463400613429</v>
       </c>
     </row>
@@ -3015,7 +3016,7 @@
       <c r="Y23">
         <v>12000</v>
       </c>
-      <c r="Z23">
+      <c r="Z23" s="1">
         <v>45702.463463194443</v>
       </c>
     </row>
@@ -3095,7 +3096,7 @@
       <c r="Y24">
         <v>380</v>
       </c>
-      <c r="Z24">
+      <c r="Z24" s="1">
         <v>45707.61117916667</v>
       </c>
     </row>
@@ -3175,7 +3176,7 @@
       <c r="Y25">
         <v>640</v>
       </c>
-      <c r="Z25">
+      <c r="Z25" s="1">
         <v>45707.656110914351</v>
       </c>
     </row>
@@ -3255,7 +3256,7 @@
       <c r="Y26">
         <v>250</v>
       </c>
-      <c r="Z26">
+      <c r="Z26" s="1">
         <v>45715.365797569444</v>
       </c>
     </row>
@@ -3335,7 +3336,7 @@
       <c r="Y27">
         <v>320</v>
       </c>
-      <c r="Z27">
+      <c r="Z27" s="1">
         <v>45715.365797569444</v>
       </c>
     </row>
@@ -3415,7 +3416,7 @@
       <c r="Y28">
         <v>250</v>
       </c>
-      <c r="Z28">
+      <c r="Z28" s="1">
         <v>45715.366664236113</v>
       </c>
     </row>
@@ -3495,7 +3496,7 @@
       <c r="Y29">
         <v>280</v>
       </c>
-      <c r="Z29">
+      <c r="Z29" s="1">
         <v>45715.366664236113</v>
       </c>
     </row>
@@ -3575,7 +3576,7 @@
       <c r="Y30">
         <v>35000</v>
       </c>
-      <c r="Z30">
+      <c r="Z30" s="1">
         <v>45687.748541666668</v>
       </c>
     </row>
@@ -3655,7 +3656,7 @@
       <c r="Y31">
         <v>83477.2</v>
       </c>
-      <c r="Z31">
+      <c r="Z31" s="1">
         <v>45692.523941203704</v>
       </c>
     </row>
@@ -3735,7 +3736,7 @@
       <c r="Y32">
         <v>58787.4</v>
       </c>
-      <c r="Z32">
+      <c r="Z32" s="1">
         <v>45686.51876230324</v>
       </c>
     </row>
@@ -3815,7 +3816,7 @@
       <c r="Y33">
         <v>79898.7</v>
       </c>
-      <c r="Z33">
+      <c r="Z33" s="1">
         <v>45706.496361724538</v>
       </c>
     </row>
@@ -3895,7 +3896,7 @@
       <c r="Y34">
         <v>1158.17</v>
       </c>
-      <c r="Z34">
+      <c r="Z34" s="1">
         <v>45688.513609062502</v>
       </c>
     </row>
@@ -3975,7 +3976,7 @@
       <c r="Y35">
         <v>2144.77</v>
       </c>
-      <c r="Z35">
+      <c r="Z35" s="1">
         <v>45688.513609062502</v>
       </c>
     </row>
@@ -4055,7 +4056,7 @@
       <c r="Y36">
         <v>1045.57</v>
       </c>
-      <c r="Z36">
+      <c r="Z36" s="1">
         <v>45688.513609062502</v>
       </c>
     </row>
@@ -4135,7 +4136,7 @@
       <c r="Y37">
         <v>2000</v>
       </c>
-      <c r="Z37">
+      <c r="Z37" s="1">
         <v>45701.461469560185</v>
       </c>
     </row>
@@ -4215,7 +4216,7 @@
       <c r="Y38">
         <v>2500</v>
       </c>
-      <c r="Z38">
+      <c r="Z38" s="1">
         <v>45701.457183645834</v>
       </c>
     </row>
@@ -4295,7 +4296,7 @@
       <c r="Y39">
         <v>2000</v>
       </c>
-      <c r="Z39">
+      <c r="Z39" s="1">
         <v>45701.628672222221</v>
       </c>
     </row>
@@ -4375,7 +4376,7 @@
       <c r="Y40">
         <v>3500</v>
       </c>
-      <c r="Z40">
+      <c r="Z40" s="1">
         <v>45701.645267476852</v>
       </c>
     </row>
@@ -4455,7 +4456,7 @@
       <c r="Y41">
         <v>1800</v>
       </c>
-      <c r="Z41">
+      <c r="Z41" s="1">
         <v>45707.371597604164</v>
       </c>
     </row>
@@ -4535,7 +4536,7 @@
       <c r="Y42">
         <v>2500</v>
       </c>
-      <c r="Z42">
+      <c r="Z42" s="1">
         <v>45701.469520833336</v>
       </c>
     </row>
@@ -4615,7 +4616,7 @@
       <c r="Y43">
         <v>6000</v>
       </c>
-      <c r="Z43">
+      <c r="Z43" s="1">
         <v>45701.640783414354</v>
       </c>
     </row>
@@ -4695,7 +4696,7 @@
       <c r="Y44">
         <v>6000</v>
       </c>
-      <c r="Z44">
+      <c r="Z44" s="1">
         <v>45701.634319097226</v>
       </c>
     </row>
@@ -4775,7 +4776,7 @@
       <c r="Y45">
         <v>6000</v>
       </c>
-      <c r="Z45">
+      <c r="Z45" s="1">
         <v>45702.527147488428</v>
       </c>
     </row>
@@ -4855,7 +4856,7 @@
       <c r="Y46">
         <v>6000</v>
       </c>
-      <c r="Z46">
+      <c r="Z46" s="1">
         <v>45702.525631053242</v>
       </c>
     </row>
@@ -4935,7 +4936,7 @@
       <c r="Y47">
         <v>2500</v>
       </c>
-      <c r="Z47">
+      <c r="Z47" s="1">
         <v>45701.631847106481</v>
       </c>
     </row>
@@ -5015,7 +5016,7 @@
       <c r="Y48">
         <v>2400</v>
       </c>
-      <c r="Z48">
+      <c r="Z48" s="1">
         <v>45699.588922835646</v>
       </c>
     </row>
@@ -5095,7 +5096,7 @@
       <c r="Y49">
         <v>2500</v>
       </c>
-      <c r="Z49">
+      <c r="Z49" s="1">
         <v>45699.693505439813</v>
       </c>
     </row>
@@ -5175,7 +5176,7 @@
       <c r="Y50">
         <v>2500</v>
       </c>
-      <c r="Z50">
+      <c r="Z50" s="1">
         <v>45699.692172650466</v>
       </c>
     </row>
@@ -5255,7 +5256,7 @@
       <c r="Y51">
         <v>2200</v>
       </c>
-      <c r="Z51">
+      <c r="Z51" s="1">
         <v>45699.690588576392</v>
       </c>
     </row>
@@ -5335,7 +5336,7 @@
       <c r="Y52">
         <v>4500</v>
       </c>
-      <c r="Z52">
+      <c r="Z52" s="1">
         <v>45701.637598877314</v>
       </c>
     </row>
@@ -5415,7 +5416,7 @@
       <c r="Y53">
         <v>2500</v>
       </c>
-      <c r="Z53">
+      <c r="Z53" s="1">
         <v>45699.696334143518</v>
       </c>
     </row>
@@ -5495,7 +5496,7 @@
       <c r="Y54">
         <v>1250</v>
       </c>
-      <c r="Z54">
+      <c r="Z54" s="1">
         <v>45707.63599490741</v>
       </c>
     </row>
@@ -5575,7 +5576,7 @@
       <c r="Y55">
         <v>2200</v>
       </c>
-      <c r="Z55">
+      <c r="Z55" s="1">
         <v>45699.540004513889</v>
       </c>
     </row>
@@ -5655,7 +5656,7 @@
       <c r="Y56">
         <v>2000</v>
       </c>
-      <c r="Z56">
+      <c r="Z56" s="1">
         <v>45712.713480208331</v>
       </c>
     </row>
@@ -5735,7 +5736,7 @@
       <c r="Y57">
         <v>2500</v>
       </c>
-      <c r="Z57">
+      <c r="Z57" s="1">
         <v>45712.709774456016</v>
       </c>
     </row>
@@ -5815,7 +5816,7 @@
       <c r="Y58">
         <v>1500</v>
       </c>
-      <c r="Z58">
+      <c r="Z58" s="1">
         <v>45715.433138854169</v>
       </c>
     </row>
@@ -5895,7 +5896,7 @@
       <c r="Y59">
         <v>2000</v>
       </c>
-      <c r="Z59">
+      <c r="Z59" s="1">
         <v>45716.696389895835</v>
       </c>
     </row>
@@ -5975,7 +5976,7 @@
       <c r="Y60">
         <v>2800</v>
       </c>
-      <c r="Z60">
+      <c r="Z60" s="1">
         <v>45708.642616898149</v>
       </c>
     </row>
@@ -6055,7 +6056,7 @@
       <c r="Y61">
         <v>2500</v>
       </c>
-      <c r="Z61">
+      <c r="Z61" s="1">
         <v>45708.63907607639</v>
       </c>
     </row>
@@ -6135,7 +6136,7 @@
       <c r="Y62">
         <v>500</v>
       </c>
-      <c r="Z62">
+      <c r="Z62" s="1">
         <v>45712.708242210647</v>
       </c>
     </row>
@@ -6215,7 +6216,7 @@
       <c r="Y63">
         <v>400</v>
       </c>
-      <c r="Z63">
+      <c r="Z63" s="1">
         <v>45716.695539618057</v>
       </c>
     </row>
@@ -6295,7 +6296,7 @@
       <c r="Y64">
         <v>2000</v>
       </c>
-      <c r="Z64">
+      <c r="Z64" s="1">
         <v>45700.662263541664</v>
       </c>
     </row>
@@ -6375,7 +6376,7 @@
       <c r="Y65">
         <v>2000</v>
       </c>
-      <c r="Z65">
+      <c r="Z65" s="1">
         <v>45700.662263541664</v>
       </c>
     </row>
@@ -6455,7 +6456,7 @@
       <c r="Y66">
         <v>2000</v>
       </c>
-      <c r="Z66">
+      <c r="Z66" s="1">
         <v>45700.663486226855</v>
       </c>
     </row>
@@ -6535,7 +6536,7 @@
       <c r="Y67">
         <v>2000</v>
       </c>
-      <c r="Z67">
+      <c r="Z67" s="1">
         <v>45700.663486226855</v>
       </c>
     </row>
@@ -6615,7 +6616,7 @@
       <c r="Y68">
         <v>2000</v>
       </c>
-      <c r="Z68">
+      <c r="Z68" s="1">
         <v>45700.661114201386</v>
       </c>
     </row>
@@ -6695,7 +6696,7 @@
       <c r="Y69">
         <v>2000</v>
       </c>
-      <c r="Z69">
+      <c r="Z69" s="1">
         <v>45700.661114201386</v>
       </c>
     </row>
@@ -6775,7 +6776,7 @@
       <c r="Y70">
         <v>2000</v>
       </c>
-      <c r="Z70">
+      <c r="Z70" s="1">
         <v>45700.652947372684</v>
       </c>
     </row>
@@ -6855,7 +6856,7 @@
       <c r="Y71">
         <v>2000</v>
       </c>
-      <c r="Z71">
+      <c r="Z71" s="1">
         <v>45700.652947372684</v>
       </c>
     </row>
@@ -6935,7 +6936,7 @@
       <c r="Y72">
         <v>2000</v>
       </c>
-      <c r="Z72">
+      <c r="Z72" s="1">
         <v>45700.654281944444</v>
       </c>
     </row>
@@ -7015,7 +7016,7 @@
       <c r="Y73">
         <v>2000</v>
       </c>
-      <c r="Z73">
+      <c r="Z73" s="1">
         <v>45700.654281944444</v>
       </c>
     </row>
@@ -7095,7 +7096,7 @@
       <c r="Y74">
         <v>2000</v>
       </c>
-      <c r="Z74">
+      <c r="Z74" s="1">
         <v>45702.509515891201</v>
       </c>
     </row>
@@ -7175,7 +7176,7 @@
       <c r="Y75">
         <v>2000</v>
       </c>
-      <c r="Z75">
+      <c r="Z75" s="1">
         <v>45702.509515891201</v>
       </c>
     </row>
@@ -7255,7 +7256,7 @@
       <c r="Y76">
         <v>2000</v>
       </c>
-      <c r="Z76">
+      <c r="Z76" s="1">
         <v>45700.659497835652</v>
       </c>
     </row>
@@ -7335,7 +7336,7 @@
       <c r="Y77">
         <v>2000</v>
       </c>
-      <c r="Z77">
+      <c r="Z77" s="1">
         <v>45700.659497835652</v>
       </c>
     </row>
@@ -7415,7 +7416,7 @@
       <c r="Y78">
         <v>2000</v>
       </c>
-      <c r="Z78">
+      <c r="Z78" s="1">
         <v>45700.651365474536</v>
       </c>
     </row>
@@ -7495,7 +7496,7 @@
       <c r="Y79">
         <v>2000</v>
       </c>
-      <c r="Z79">
+      <c r="Z79" s="1">
         <v>45700.651365474536</v>
       </c>
     </row>
@@ -7575,7 +7576,7 @@
       <c r="Y80">
         <v>2000</v>
       </c>
-      <c r="Z80">
+      <c r="Z80" s="1">
         <v>45702.520452280092</v>
       </c>
     </row>
@@ -7655,7 +7656,7 @@
       <c r="Y81">
         <v>2000</v>
       </c>
-      <c r="Z81">
+      <c r="Z81" s="1">
         <v>45702.520452280092</v>
       </c>
     </row>
@@ -7735,7 +7736,7 @@
       <c r="Y82">
         <v>2000</v>
       </c>
-      <c r="Z82">
+      <c r="Z82" s="1">
         <v>45700.658020451388</v>
       </c>
     </row>
@@ -7815,7 +7816,7 @@
       <c r="Y83">
         <v>2000</v>
       </c>
-      <c r="Z83">
+      <c r="Z83" s="1">
         <v>45700.658020451388</v>
       </c>
     </row>
@@ -7895,7 +7896,7 @@
       <c r="Y84">
         <v>2500</v>
       </c>
-      <c r="Z84">
+      <c r="Z84" s="1">
         <v>45699.695142824072</v>
       </c>
     </row>
@@ -7975,7 +7976,7 @@
       <c r="Y85">
         <v>2000</v>
       </c>
-      <c r="Z85">
+      <c r="Z85" s="1">
         <v>45700.655673067129</v>
       </c>
     </row>
@@ -8055,7 +8056,7 @@
       <c r="Y86">
         <v>2000</v>
       </c>
-      <c r="Z86">
+      <c r="Z86" s="1">
         <v>45700.655673067129</v>
       </c>
     </row>
@@ -8135,7 +8136,7 @@
       <c r="Y87">
         <v>533.33000000000004</v>
       </c>
-      <c r="Z87">
+      <c r="Z87" s="1">
         <v>45715.621550729164</v>
       </c>
     </row>
@@ -8215,7 +8216,7 @@
       <c r="Y88">
         <v>2500</v>
       </c>
-      <c r="Z88">
+      <c r="Z88" s="1">
         <v>45712.705184687497</v>
       </c>
     </row>
@@ -8295,7 +8296,7 @@
       <c r="Y89">
         <v>2200</v>
       </c>
-      <c r="Z89">
+      <c r="Z89" s="1">
         <v>45712.710528275464</v>
       </c>
     </row>
@@ -8375,7 +8376,7 @@
       <c r="Y90">
         <v>2800</v>
       </c>
-      <c r="Z90">
+      <c r="Z90" s="1">
         <v>45712.715031793981</v>
       </c>
     </row>
@@ -8455,7 +8456,7 @@
       <c r="Y91">
         <v>1496</v>
       </c>
-      <c r="Z91">
+      <c r="Z91" s="1">
         <v>45715.423745601853</v>
       </c>
     </row>
@@ -8535,7 +8536,7 @@
       <c r="Y92">
         <v>7464.6</v>
       </c>
-      <c r="Z92">
+      <c r="Z92" s="1">
         <v>45692.523941203704</v>
       </c>
     </row>
@@ -8615,7 +8616,7 @@
       <c r="Y93">
         <v>2000</v>
       </c>
-      <c r="Z93">
+      <c r="Z93" s="1">
         <v>45706.432341238426</v>
       </c>
     </row>
@@ -8695,7 +8696,7 @@
       <c r="Y94">
         <v>150</v>
       </c>
-      <c r="Z94">
+      <c r="Z94" s="1">
         <v>45712.714414930553</v>
       </c>
     </row>
@@ -8775,7 +8776,7 @@
       <c r="Y95">
         <v>1700</v>
       </c>
-      <c r="Z95">
+      <c r="Z95" s="1">
         <v>45715.431714895836</v>
       </c>
     </row>
@@ -8855,7 +8856,7 @@
       <c r="Y96">
         <v>2000</v>
       </c>
-      <c r="Z96">
+      <c r="Z96" s="1">
         <v>45699.697784062497</v>
       </c>
     </row>
@@ -8935,7 +8936,7 @@
       <c r="Y97">
         <v>2000</v>
       </c>
-      <c r="Z97">
+      <c r="Z97" s="1">
         <v>45699.697784062497</v>
       </c>
     </row>
@@ -9015,7 +9016,7 @@
       <c r="Y98">
         <v>2800</v>
       </c>
-      <c r="Z98">
+      <c r="Z98" s="1">
         <v>45715.627838229164</v>
       </c>
     </row>
@@ -9095,7 +9096,7 @@
       <c r="Y99">
         <v>2800</v>
       </c>
-      <c r="Z99">
+      <c r="Z99" s="1">
         <v>45715.634292673611</v>
       </c>
     </row>
@@ -9175,7 +9176,7 @@
       <c r="Y100">
         <v>2800</v>
       </c>
-      <c r="Z100">
+      <c r="Z100" s="1">
         <v>45715.619089155094</v>
       </c>
     </row>
@@ -9255,7 +9256,7 @@
       <c r="Y101">
         <v>2800</v>
       </c>
-      <c r="Z101">
+      <c r="Z101" s="1">
         <v>45715.620652199075</v>
       </c>
     </row>
@@ -9335,7 +9336,7 @@
       <c r="Y102">
         <v>2800</v>
       </c>
-      <c r="Z102">
+      <c r="Z102" s="1">
         <v>45715.617958136572</v>
       </c>
     </row>
@@ -9415,7 +9416,7 @@
       <c r="Y103">
         <v>2800</v>
       </c>
-      <c r="Z103">
+      <c r="Z103" s="1">
         <v>45715.61500150463</v>
       </c>
     </row>
@@ -9495,7 +9496,7 @@
       <c r="Y104">
         <v>2800</v>
       </c>
-      <c r="Z104">
+      <c r="Z104" s="1">
         <v>45712.703846261575</v>
       </c>
     </row>
@@ -9575,7 +9576,7 @@
       <c r="Y105">
         <v>2200</v>
       </c>
-      <c r="Z105">
+      <c r="Z105" s="1">
         <v>45713.632253668984</v>
       </c>
     </row>
@@ -9655,7 +9656,7 @@
       <c r="Y106">
         <v>2000</v>
       </c>
-      <c r="Z106">
+      <c r="Z106" s="1">
         <v>45702.524119178241</v>
       </c>
     </row>
@@ -9735,7 +9736,7 @@
       <c r="Y107">
         <v>2500</v>
       </c>
-      <c r="Z107">
+      <c r="Z107" s="1">
         <v>45707.475378506948</v>
       </c>
     </row>
@@ -9815,7 +9816,7 @@
       <c r="Y108">
         <v>46457.53</v>
       </c>
-      <c r="Z108">
+      <c r="Z108" s="1">
         <v>45712.702018206015</v>
       </c>
     </row>
@@ -9895,7 +9896,7 @@
       <c r="Y109">
         <v>46457.53</v>
       </c>
-      <c r="Z109">
+      <c r="Z109" s="1">
         <v>45712.703188888889</v>
       </c>
     </row>
@@ -9975,7 +9976,7 @@
       <c r="Y110">
         <v>312</v>
       </c>
-      <c r="Z110">
+      <c r="Z110" s="1">
         <v>45707.443961111108</v>
       </c>
     </row>
@@ -10055,7 +10056,7 @@
       <c r="Y111">
         <v>2200</v>
       </c>
-      <c r="Z111">
+      <c r="Z111" s="1">
         <v>45716.397964699077</v>
       </c>
     </row>
@@ -10135,7 +10136,7 @@
       <c r="Y112">
         <v>6000</v>
       </c>
-      <c r="Z112">
+      <c r="Z112" s="1">
         <v>45715.425985995367</v>
       </c>
     </row>
@@ -10215,7 +10216,7 @@
       <c r="Y113">
         <v>1800</v>
       </c>
-      <c r="Z113">
+      <c r="Z113" s="1">
         <v>45707.46554355324</v>
       </c>
     </row>
@@ -10295,7 +10296,7 @@
       <c r="Y114">
         <v>2400</v>
       </c>
-      <c r="Z114">
+      <c r="Z114" s="1">
         <v>45707.382853587966</v>
       </c>
     </row>
@@ -10375,7 +10376,7 @@
       <c r="Y115">
         <v>1175</v>
       </c>
-      <c r="Z115">
+      <c r="Z115" s="1">
         <v>45707.467136342595</v>
       </c>
     </row>
@@ -10455,7 +10456,7 @@
       <c r="Y116">
         <v>3200</v>
       </c>
-      <c r="Z116">
+      <c r="Z116" s="1">
         <v>45709.502550960649</v>
       </c>
     </row>
@@ -10535,7 +10536,7 @@
       <c r="Y117">
         <v>4500</v>
       </c>
-      <c r="Z117">
+      <c r="Z117" s="1">
         <v>45706.597614733793</v>
       </c>
     </row>
@@ -10615,7 +10616,7 @@
       <c r="Y118">
         <v>2500</v>
       </c>
-      <c r="Z118">
+      <c r="Z118" s="1">
         <v>45707.471929976855</v>
       </c>
     </row>
@@ -10695,7 +10696,7 @@
       <c r="Y119">
         <v>1152.81</v>
       </c>
-      <c r="Z119">
+      <c r="Z119" s="1">
         <v>45712.700295405091</v>
       </c>
     </row>
@@ -10775,7 +10776,7 @@
       <c r="Y120">
         <v>2000</v>
       </c>
-      <c r="Z120">
+      <c r="Z120" s="1">
         <v>45709.500071759256</v>
       </c>
     </row>
@@ -10855,7 +10856,7 @@
       <c r="Y121">
         <v>1800</v>
       </c>
-      <c r="Z121">
+      <c r="Z121" s="1">
         <v>45707.375472800923</v>
       </c>
     </row>
@@ -10935,7 +10936,7 @@
       <c r="Y122">
         <v>3500</v>
       </c>
-      <c r="Z122">
+      <c r="Z122" s="1">
         <v>45707.379096724537</v>
       </c>
     </row>
@@ -11015,7 +11016,7 @@
       <c r="Y123">
         <v>3800</v>
       </c>
-      <c r="Z123">
+      <c r="Z123" s="1">
         <v>45708.430624537039</v>
       </c>
     </row>
@@ -11095,7 +11096,7 @@
       <c r="Y124">
         <v>3500</v>
       </c>
-      <c r="Z124">
+      <c r="Z124" s="1">
         <v>45712.707418981481</v>
       </c>
     </row>
@@ -11175,7 +11176,7 @@
       <c r="Y125">
         <v>3500</v>
       </c>
-      <c r="Z125">
+      <c r="Z125" s="1">
         <v>45712.706201469904</v>
       </c>
     </row>
@@ -11255,7 +11256,7 @@
       <c r="Y126">
         <v>2222.2199999999998</v>
       </c>
-      <c r="Z126">
+      <c r="Z126" s="1">
         <v>45715.535773344905</v>
       </c>
     </row>
@@ -11335,7 +11336,7 @@
       <c r="Y127">
         <v>1500</v>
       </c>
-      <c r="Z127">
+      <c r="Z127" s="1">
         <v>45712.71153429398</v>
       </c>
     </row>
@@ -11415,7 +11416,7 @@
       <c r="Y128">
         <v>2450</v>
       </c>
-      <c r="Z128">
+      <c r="Z128" s="1">
         <v>45709.608564201386</v>
       </c>
     </row>
@@ -11495,7 +11496,7 @@
       <c r="Y129">
         <v>1500</v>
       </c>
-      <c r="Z129">
+      <c r="Z129" s="1">
         <v>45709.605947534721</v>
       </c>
     </row>
@@ -11575,7 +11576,7 @@
       <c r="Y130">
         <v>2800</v>
       </c>
-      <c r="Z130">
+      <c r="Z130" s="1">
         <v>45708.427169016206</v>
       </c>
     </row>
@@ -11655,7 +11656,7 @@
       <c r="Y131">
         <v>1560</v>
       </c>
-      <c r="Z131">
+      <c r="Z131" s="1">
         <v>45709.612314004633</v>
       </c>
     </row>
@@ -11735,7 +11736,7 @@
       <c r="Y132">
         <v>1200</v>
       </c>
-      <c r="Z132">
+      <c r="Z132" s="1">
         <v>45715.429412349535</v>
       </c>
     </row>
@@ -11815,7 +11816,7 @@
       <c r="Y133">
         <v>1350</v>
       </c>
-      <c r="Z133">
+      <c r="Z133" s="1">
         <v>45715.42851597222</v>
       </c>
     </row>
@@ -11895,7 +11896,7 @@
       <c r="Y134">
         <v>3000</v>
       </c>
-      <c r="Z134">
+      <c r="Z134" s="1">
         <v>45719.536064201391</v>
       </c>
     </row>
@@ -11975,7 +11976,7 @@
       <c r="Y135">
         <v>5000</v>
       </c>
-      <c r="Z135">
+      <c r="Z135" s="1">
         <v>45716.398728009262</v>
       </c>
     </row>
@@ -12055,7 +12056,7 @@
       <c r="Y136">
         <v>122264.72</v>
       </c>
-      <c r="Z136">
+      <c r="Z136" s="1">
         <v>45716.697349849535</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrego la columna nombre_ff
</commit_message>
<xml_diff>
--- a/data/ep_mes_2025.xlsx
+++ b/data/ep_mes_2025.xlsx
@@ -8,24 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6. Código\seguimiento_presupuestal_unsch_streamlit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911742ED-A3BB-4DD9-8DA6-2A7A778B2913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583AE361-3725-4866-BD8A-21C7D7F5393C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="279">
   <si>
     <t>ano_eje</t>
   </si>
@@ -847,6 +857,21 @@
   </si>
   <si>
     <t>2.3. 2  4. 2  1</t>
+  </si>
+  <si>
+    <t>NOMBRE_FF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09: RECURSOS DIRECTAMENTE RECAUDADOS                                                                                                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </t>
+  </si>
+  <si>
+    <t>18: CANON Y SOBRECANON, REGALIAS, RENTA DE ADUANAS Y PARTICIPACIONES</t>
+  </si>
+  <si>
+    <t>nombre_ff</t>
   </si>
 </sst>
 </file>
@@ -882,9 +907,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1165,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z136"/>
+  <dimension ref="A1:AA136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,11 +1202,14 @@
     <col min="8" max="8" width="29.140625" customWidth="1"/>
     <col min="10" max="10" width="19.85546875" customWidth="1"/>
     <col min="11" max="11" width="15.28515625" customWidth="1"/>
-    <col min="22" max="22" width="14" customWidth="1"/>
-    <col min="26" max="26" width="19" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" customWidth="1"/>
+    <col min="21" max="21" width="16.28515625" customWidth="1"/>
+    <col min="22" max="22" width="23.7109375" customWidth="1"/>
+    <col min="23" max="23" width="14" customWidth="1"/>
+    <col min="27" max="27" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1245,22 +1274,25 @@
         <v>21</v>
       </c>
       <c r="V1" t="s">
+        <v>278</v>
+      </c>
+      <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1324,23 +1356,27 @@
       <c r="U2" t="s">
         <v>34</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" t="str">
+        <f>VLOOKUP(U2,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W2" t="s">
         <v>35</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>24</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>36</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>6603.52</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="AA2" s="1">
         <v>45677.679732025463</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1404,23 +1440,27 @@
       <c r="U3" t="s">
         <v>34</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" s="2" t="str">
+        <f>VLOOKUP(U3,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W3" t="s">
         <v>35</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>24</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>36</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>-1343.89</v>
       </c>
-      <c r="Z3" s="1">
+      <c r="AA3" s="1">
         <v>45677.679732025463</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1484,23 +1524,27 @@
       <c r="U4" t="s">
         <v>34</v>
       </c>
-      <c r="V4" t="s">
+      <c r="V4" s="2" t="str">
+        <f>VLOOKUP(U4,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W4" t="s">
         <v>40</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>21</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>36</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>320</v>
       </c>
-      <c r="Z4" s="1">
+      <c r="AA4" s="1">
         <v>45680.692369212964</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1564,23 +1608,27 @@
       <c r="U5" t="s">
         <v>34</v>
       </c>
-      <c r="V5" t="s">
+      <c r="V5" s="2" t="str">
+        <f>VLOOKUP(U5,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W5" t="s">
         <v>40</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>23</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>36</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>224</v>
       </c>
-      <c r="Z5" s="1">
+      <c r="AA5" s="1">
         <v>45688.687467557873</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1644,23 +1692,27 @@
       <c r="U6" t="s">
         <v>34</v>
       </c>
-      <c r="V6" t="s">
+      <c r="V6" s="2" t="str">
+        <f>VLOOKUP(U6,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W6" t="s">
         <v>40</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>23</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>36</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>-4</v>
       </c>
-      <c r="Z6" s="1">
+      <c r="AA6" s="1">
         <v>45688.687467557873</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1724,23 +1776,27 @@
       <c r="U7" t="s">
         <v>34</v>
       </c>
-      <c r="V7" t="s">
+      <c r="V7" s="2" t="str">
+        <f>VLOOKUP(U7,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W7" t="s">
         <v>40</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>22</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>36</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>320</v>
       </c>
-      <c r="Z7" s="1">
+      <c r="AA7" s="1">
         <v>45681.638071909721</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1804,23 +1860,27 @@
       <c r="U8" t="s">
         <v>34</v>
       </c>
-      <c r="V8" t="s">
+      <c r="V8" s="2" t="str">
+        <f>VLOOKUP(U8,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W8" t="s">
         <v>40</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>31</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>36</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>320</v>
       </c>
-      <c r="Z8" s="1">
+      <c r="AA8" s="1">
         <v>45681.638227083335</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1884,23 +1944,27 @@
       <c r="U9" t="s">
         <v>34</v>
       </c>
-      <c r="V9" t="s">
+      <c r="V9" s="2" t="str">
+        <f>VLOOKUP(U9,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W9" t="s">
         <v>40</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>31</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>36</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>-39</v>
       </c>
-      <c r="Z9" s="1">
+      <c r="AA9" s="1">
         <v>45681.638227083335</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1964,23 +2028,27 @@
       <c r="U10" t="s">
         <v>34</v>
       </c>
-      <c r="V10" t="s">
+      <c r="V10" s="2" t="str">
+        <f>VLOOKUP(U10,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W10" t="s">
         <v>40</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>31</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Y10" t="s">
         <v>36</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <v>224</v>
       </c>
-      <c r="Z10" s="1">
+      <c r="AA10" s="1">
         <v>45688.687400381947</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2044,23 +2112,27 @@
       <c r="U11" t="s">
         <v>34</v>
       </c>
-      <c r="V11" t="s">
+      <c r="V11" s="2" t="str">
+        <f>VLOOKUP(U11,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W11" t="s">
         <v>40</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>9</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>53</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>320</v>
       </c>
-      <c r="Z11" s="1">
+      <c r="AA11" s="1">
         <v>45681.638293171294</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2124,23 +2196,27 @@
       <c r="U12" t="s">
         <v>34</v>
       </c>
-      <c r="V12" t="s">
+      <c r="V12" s="2" t="str">
+        <f>VLOOKUP(U12,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W12" t="s">
         <v>40</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>9</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
         <v>53</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <v>-29</v>
       </c>
-      <c r="Z12" s="1">
+      <c r="AA12" s="1">
         <v>45681.638293171294</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2204,23 +2280,27 @@
       <c r="U13" t="s">
         <v>34</v>
       </c>
-      <c r="V13" t="s">
+      <c r="V13" s="2" t="str">
+        <f>VLOOKUP(U13,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W13" t="s">
         <v>40</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>9</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Y13" t="s">
         <v>53</v>
       </c>
-      <c r="Y13">
+      <c r="Z13">
         <v>224</v>
       </c>
-      <c r="Z13" s="1">
+      <c r="AA13" s="1">
         <v>45688.661467789352</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -2284,23 +2364,27 @@
       <c r="U14" t="s">
         <v>34</v>
       </c>
-      <c r="V14" t="s">
+      <c r="V14" s="2" t="str">
+        <f>VLOOKUP(U14,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W14" t="s">
         <v>57</v>
       </c>
-      <c r="W14">
-        <v>34</v>
-      </c>
-      <c r="X14" t="s">
+      <c r="X14">
+        <v>34</v>
+      </c>
+      <c r="Y14" t="s">
         <v>36</v>
       </c>
-      <c r="Y14">
+      <c r="Z14">
         <v>200</v>
       </c>
-      <c r="Z14" s="1">
+      <c r="AA14" s="1">
         <v>45698.605144363428</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2364,23 +2448,27 @@
       <c r="U15" t="s">
         <v>34</v>
       </c>
-      <c r="V15" t="s">
+      <c r="V15" s="2" t="str">
+        <f>VLOOKUP(U15,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W15" t="s">
         <v>40</v>
       </c>
-      <c r="W15">
-        <v>34</v>
-      </c>
-      <c r="X15" t="s">
+      <c r="X15">
+        <v>34</v>
+      </c>
+      <c r="Y15" t="s">
         <v>36</v>
       </c>
-      <c r="Y15">
+      <c r="Z15">
         <v>640</v>
       </c>
-      <c r="Z15" s="1">
+      <c r="AA15" s="1">
         <v>45698.605144363428</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2444,23 +2532,27 @@
       <c r="U16" t="s">
         <v>34</v>
       </c>
-      <c r="V16" t="s">
+      <c r="V16" s="2" t="str">
+        <f>VLOOKUP(U16,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W16" t="s">
         <v>40</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>24</v>
       </c>
-      <c r="X16" t="s">
+      <c r="Y16" t="s">
         <v>36</v>
       </c>
-      <c r="Y16">
+      <c r="Z16">
         <v>380</v>
       </c>
-      <c r="Z16" s="1">
+      <c r="AA16" s="1">
         <v>45700.41507318287</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -2524,23 +2616,27 @@
       <c r="U17" t="s">
         <v>34</v>
       </c>
-      <c r="V17" t="s">
+      <c r="V17" s="2" t="str">
+        <f>VLOOKUP(U17,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W17" t="s">
         <v>57</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <v>7</v>
       </c>
-      <c r="X17" t="s">
+      <c r="Y17" t="s">
         <v>53</v>
       </c>
-      <c r="Y17">
+      <c r="Z17">
         <v>200</v>
       </c>
-      <c r="Z17" s="1">
+      <c r="AA17" s="1">
         <v>45700.477851886571</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -2604,23 +2700,27 @@
       <c r="U18" t="s">
         <v>34</v>
       </c>
-      <c r="V18" t="s">
+      <c r="V18" s="2" t="str">
+        <f>VLOOKUP(U18,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W18" t="s">
         <v>40</v>
       </c>
-      <c r="W18">
+      <c r="X18">
         <v>7</v>
       </c>
-      <c r="X18" t="s">
+      <c r="Y18" t="s">
         <v>53</v>
       </c>
-      <c r="Y18">
+      <c r="Z18">
         <v>320</v>
       </c>
-      <c r="Z18" s="1">
+      <c r="AA18" s="1">
         <v>45700.477851886571</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2684,23 +2784,27 @@
       <c r="U19" t="s">
         <v>34</v>
       </c>
-      <c r="V19" t="s">
+      <c r="V19" s="2" t="str">
+        <f>VLOOKUP(U19,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W19" t="s">
         <v>57</v>
       </c>
-      <c r="W19">
+      <c r="X19">
         <v>10</v>
       </c>
-      <c r="X19" t="s">
+      <c r="Y19" t="s">
         <v>64</v>
       </c>
-      <c r="Y19">
+      <c r="Z19">
         <v>200</v>
       </c>
-      <c r="Z19" s="1">
+      <c r="AA19" s="1">
         <v>45715.366732488423</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -2764,23 +2868,27 @@
       <c r="U20" t="s">
         <v>34</v>
       </c>
-      <c r="V20" t="s">
+      <c r="V20" s="2" t="str">
+        <f>VLOOKUP(U20,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W20" t="s">
         <v>40</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>10</v>
       </c>
-      <c r="X20" t="s">
+      <c r="Y20" t="s">
         <v>64</v>
       </c>
-      <c r="Y20">
+      <c r="Z20">
         <v>280</v>
       </c>
-      <c r="Z20" s="1">
+      <c r="AA20" s="1">
         <v>45715.366732488423</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -2844,23 +2952,27 @@
       <c r="U21" t="s">
         <v>68</v>
       </c>
-      <c r="V21" t="s">
+      <c r="V21" s="2" t="str">
+        <f>VLOOKUP(U21,Hoja2!A$1:B$4,2,0)</f>
+        <v>18: CANON Y SOBRECANON, REGALIAS, RENTA DE ADUANAS Y PARTICIPACIONES</v>
+      </c>
+      <c r="W21" t="s">
         <v>40</v>
       </c>
-      <c r="W21">
+      <c r="X21">
         <v>49</v>
       </c>
-      <c r="X21" t="s">
+      <c r="Y21" t="s">
         <v>36</v>
       </c>
-      <c r="Y21">
+      <c r="Z21">
         <v>200</v>
       </c>
-      <c r="Z21" s="1">
+      <c r="AA21" s="1">
         <v>45702.463211840281</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -2924,23 +3036,27 @@
       <c r="U22" t="s">
         <v>68</v>
       </c>
-      <c r="V22" t="s">
+      <c r="V22" s="2" t="str">
+        <f>VLOOKUP(U22,Hoja2!A$1:B$4,2,0)</f>
+        <v>18: CANON Y SOBRECANON, REGALIAS, RENTA DE ADUANAS Y PARTICIPACIONES</v>
+      </c>
+      <c r="W22" t="s">
         <v>40</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>49</v>
       </c>
-      <c r="X22" t="s">
+      <c r="Y22" t="s">
         <v>36</v>
       </c>
-      <c r="Y22">
+      <c r="Z22">
         <v>200</v>
       </c>
-      <c r="Z22" s="1">
+      <c r="AA22" s="1">
         <v>45702.463400613429</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -3004,23 +3120,27 @@
       <c r="U23" t="s">
         <v>68</v>
       </c>
-      <c r="V23" t="s">
+      <c r="V23" s="2" t="str">
+        <f>VLOOKUP(U23,Hoja2!A$1:B$4,2,0)</f>
+        <v>18: CANON Y SOBRECANON, REGALIAS, RENTA DE ADUANAS Y PARTICIPACIONES</v>
+      </c>
+      <c r="W23" t="s">
         <v>35</v>
       </c>
-      <c r="W23">
+      <c r="X23">
         <v>49</v>
       </c>
-      <c r="X23" t="s">
+      <c r="Y23" t="s">
         <v>36</v>
       </c>
-      <c r="Y23">
+      <c r="Z23">
         <v>12000</v>
       </c>
-      <c r="Z23" s="1">
+      <c r="AA23" s="1">
         <v>45702.463463194443</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -3084,23 +3204,27 @@
       <c r="U24" t="s">
         <v>34</v>
       </c>
-      <c r="V24" t="s">
+      <c r="V24" s="2" t="str">
+        <f>VLOOKUP(U24,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W24" t="s">
         <v>40</v>
       </c>
-      <c r="W24">
+      <c r="X24">
         <v>24</v>
       </c>
-      <c r="X24" t="s">
+      <c r="Y24" t="s">
         <v>36</v>
       </c>
-      <c r="Y24">
+      <c r="Z24">
         <v>380</v>
       </c>
-      <c r="Z24" s="1">
+      <c r="AA24" s="1">
         <v>45707.61117916667</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -3164,23 +3288,27 @@
       <c r="U25" t="s">
         <v>34</v>
       </c>
-      <c r="V25" t="s">
+      <c r="V25" s="2" t="str">
+        <f>VLOOKUP(U25,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W25" t="s">
         <v>40</v>
       </c>
-      <c r="W25">
+      <c r="X25">
         <v>25</v>
       </c>
-      <c r="X25" t="s">
+      <c r="Y25" t="s">
         <v>36</v>
       </c>
-      <c r="Y25">
+      <c r="Z25">
         <v>640</v>
       </c>
-      <c r="Z25" s="1">
+      <c r="AA25" s="1">
         <v>45707.656110914351</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -3244,23 +3372,27 @@
       <c r="U26" t="s">
         <v>34</v>
       </c>
-      <c r="V26" t="s">
+      <c r="V26" s="2" t="str">
+        <f>VLOOKUP(U26,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W26" t="s">
         <v>57</v>
       </c>
-      <c r="W26">
+      <c r="X26">
         <v>10</v>
       </c>
-      <c r="X26" t="s">
+      <c r="Y26" t="s">
         <v>64</v>
       </c>
-      <c r="Y26">
+      <c r="Z26">
         <v>250</v>
       </c>
-      <c r="Z26" s="1">
+      <c r="AA26" s="1">
         <v>45715.365797569444</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -3324,23 +3456,27 @@
       <c r="U27" t="s">
         <v>34</v>
       </c>
-      <c r="V27" t="s">
+      <c r="V27" s="2" t="str">
+        <f>VLOOKUP(U27,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W27" t="s">
         <v>40</v>
       </c>
-      <c r="W27">
+      <c r="X27">
         <v>10</v>
       </c>
-      <c r="X27" t="s">
+      <c r="Y27" t="s">
         <v>64</v>
       </c>
-      <c r="Y27">
+      <c r="Z27">
         <v>320</v>
       </c>
-      <c r="Z27" s="1">
+      <c r="AA27" s="1">
         <v>45715.365797569444</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -3404,23 +3540,27 @@
       <c r="U28" t="s">
         <v>34</v>
       </c>
-      <c r="V28" t="s">
+      <c r="V28" s="2" t="str">
+        <f>VLOOKUP(U28,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W28" t="s">
         <v>57</v>
       </c>
-      <c r="W28">
+      <c r="X28">
         <v>10</v>
       </c>
-      <c r="X28" t="s">
+      <c r="Y28" t="s">
         <v>64</v>
       </c>
-      <c r="Y28">
+      <c r="Z28">
         <v>250</v>
       </c>
-      <c r="Z28" s="1">
+      <c r="AA28" s="1">
         <v>45715.366664236113</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -3484,23 +3624,27 @@
       <c r="U29" t="s">
         <v>34</v>
       </c>
-      <c r="V29" t="s">
+      <c r="V29" s="2" t="str">
+        <f>VLOOKUP(U29,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W29" t="s">
         <v>40</v>
       </c>
-      <c r="W29">
+      <c r="X29">
         <v>10</v>
       </c>
-      <c r="X29" t="s">
+      <c r="Y29" t="s">
         <v>64</v>
       </c>
-      <c r="Y29">
+      <c r="Z29">
         <v>280</v>
       </c>
-      <c r="Z29" s="1">
+      <c r="AA29" s="1">
         <v>45715.366664236113</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -3564,23 +3708,27 @@
       <c r="U30" t="s">
         <v>34</v>
       </c>
-      <c r="V30" t="s">
+      <c r="V30" s="2" t="str">
+        <f>VLOOKUP(U30,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W30" t="s">
         <v>79</v>
       </c>
-      <c r="W30">
+      <c r="X30">
         <v>10</v>
       </c>
-      <c r="X30" t="s">
+      <c r="Y30" t="s">
         <v>64</v>
       </c>
-      <c r="Y30">
+      <c r="Z30">
         <v>35000</v>
       </c>
-      <c r="Z30" s="1">
+      <c r="AA30" s="1">
         <v>45687.748541666668</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -3644,23 +3792,27 @@
       <c r="U31" t="s">
         <v>34</v>
       </c>
-      <c r="V31" t="s">
+      <c r="V31" s="2" t="str">
+        <f>VLOOKUP(U31,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W31" t="s">
         <v>83</v>
       </c>
-      <c r="W31">
+      <c r="X31">
         <v>31</v>
       </c>
-      <c r="X31" t="s">
+      <c r="Y31" t="s">
         <v>36</v>
       </c>
-      <c r="Y31">
+      <c r="Z31">
         <v>83477.2</v>
       </c>
-      <c r="Z31" s="1">
+      <c r="AA31" s="1">
         <v>45692.523941203704</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -3724,23 +3876,27 @@
       <c r="U32" t="s">
         <v>34</v>
       </c>
-      <c r="V32" t="s">
+      <c r="V32" s="2" t="str">
+        <f>VLOOKUP(U32,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W32" t="s">
         <v>86</v>
       </c>
-      <c r="W32">
+      <c r="X32">
         <v>31</v>
       </c>
-      <c r="X32" t="s">
+      <c r="Y32" t="s">
         <v>36</v>
       </c>
-      <c r="Y32">
+      <c r="Z32">
         <v>58787.4</v>
       </c>
-      <c r="Z32" s="1">
+      <c r="AA32" s="1">
         <v>45686.51876230324</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -3804,23 +3960,27 @@
       <c r="U33" t="s">
         <v>34</v>
       </c>
-      <c r="V33" t="s">
+      <c r="V33" s="2" t="str">
+        <f>VLOOKUP(U33,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W33" t="s">
         <v>86</v>
       </c>
-      <c r="W33">
+      <c r="X33">
         <v>31</v>
       </c>
-      <c r="X33" t="s">
+      <c r="Y33" t="s">
         <v>36</v>
       </c>
-      <c r="Y33">
+      <c r="Z33">
         <v>79898.7</v>
       </c>
-      <c r="Z33" s="1">
+      <c r="AA33" s="1">
         <v>45706.496361724538</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -3884,23 +4044,27 @@
       <c r="U34" t="s">
         <v>34</v>
       </c>
-      <c r="V34" t="s">
+      <c r="V34" s="2" t="str">
+        <f>VLOOKUP(U34,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W34" t="s">
         <v>89</v>
       </c>
-      <c r="W34">
+      <c r="X34">
         <v>31</v>
       </c>
-      <c r="X34" t="s">
+      <c r="Y34" t="s">
         <v>36</v>
       </c>
-      <c r="Y34">
+      <c r="Z34">
         <v>1158.17</v>
       </c>
-      <c r="Z34" s="1">
+      <c r="AA34" s="1">
         <v>45688.513609062502</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -3964,23 +4128,27 @@
       <c r="U35" t="s">
         <v>34</v>
       </c>
-      <c r="V35" t="s">
+      <c r="V35" s="2" t="str">
+        <f>VLOOKUP(U35,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W35" t="s">
         <v>89</v>
       </c>
-      <c r="W35">
+      <c r="X35">
         <v>31</v>
       </c>
-      <c r="X35" t="s">
+      <c r="Y35" t="s">
         <v>36</v>
       </c>
-      <c r="Y35">
+      <c r="Z35">
         <v>2144.77</v>
       </c>
-      <c r="Z35" s="1">
+      <c r="AA35" s="1">
         <v>45688.513609062502</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -4044,23 +4212,27 @@
       <c r="U36" t="s">
         <v>34</v>
       </c>
-      <c r="V36" t="s">
+      <c r="V36" s="2" t="str">
+        <f>VLOOKUP(U36,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W36" t="s">
         <v>89</v>
       </c>
-      <c r="W36">
+      <c r="X36">
         <v>31</v>
       </c>
-      <c r="X36" t="s">
+      <c r="Y36" t="s">
         <v>36</v>
       </c>
-      <c r="Y36">
+      <c r="Z36">
         <v>1045.57</v>
       </c>
-      <c r="Z36" s="1">
+      <c r="AA36" s="1">
         <v>45688.513609062502</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -4124,23 +4296,27 @@
       <c r="U37" t="s">
         <v>34</v>
       </c>
-      <c r="V37" t="s">
+      <c r="V37" s="2" t="str">
+        <f>VLOOKUP(U37,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W37" t="s">
         <v>92</v>
       </c>
-      <c r="W37">
+      <c r="X37">
         <v>31</v>
       </c>
-      <c r="X37" t="s">
+      <c r="Y37" t="s">
         <v>36</v>
       </c>
-      <c r="Y37">
+      <c r="Z37">
         <v>2000</v>
       </c>
-      <c r="Z37" s="1">
+      <c r="AA37" s="1">
         <v>45701.461469560185</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -4204,23 +4380,27 @@
       <c r="U38" t="s">
         <v>34</v>
       </c>
-      <c r="V38" t="s">
+      <c r="V38" s="2" t="str">
+        <f>VLOOKUP(U38,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W38" t="s">
         <v>92</v>
       </c>
-      <c r="W38">
+      <c r="X38">
         <v>31</v>
       </c>
-      <c r="X38" t="s">
+      <c r="Y38" t="s">
         <v>36</v>
       </c>
-      <c r="Y38">
+      <c r="Z38">
         <v>2500</v>
       </c>
-      <c r="Z38" s="1">
+      <c r="AA38" s="1">
         <v>45701.457183645834</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -4284,23 +4464,27 @@
       <c r="U39" t="s">
         <v>34</v>
       </c>
-      <c r="V39" t="s">
+      <c r="V39" s="2" t="str">
+        <f>VLOOKUP(U39,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W39" t="s">
         <v>92</v>
       </c>
-      <c r="W39">
+      <c r="X39">
         <v>9</v>
       </c>
-      <c r="X39" t="s">
+      <c r="Y39" t="s">
         <v>53</v>
       </c>
-      <c r="Y39">
+      <c r="Z39">
         <v>2000</v>
       </c>
-      <c r="Z39" s="1">
+      <c r="AA39" s="1">
         <v>45701.628672222221</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -4364,23 +4548,27 @@
       <c r="U40" t="s">
         <v>34</v>
       </c>
-      <c r="V40" t="s">
+      <c r="V40" s="2" t="str">
+        <f>VLOOKUP(U40,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W40" t="s">
         <v>92</v>
       </c>
-      <c r="W40">
+      <c r="X40">
         <v>9</v>
       </c>
-      <c r="X40" t="s">
+      <c r="Y40" t="s">
         <v>53</v>
       </c>
-      <c r="Y40">
+      <c r="Z40">
         <v>3500</v>
       </c>
-      <c r="Z40" s="1">
+      <c r="AA40" s="1">
         <v>45701.645267476852</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -4444,23 +4632,27 @@
       <c r="U41" t="s">
         <v>34</v>
       </c>
-      <c r="V41" t="s">
+      <c r="V41" s="2" t="str">
+        <f>VLOOKUP(U41,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W41" t="s">
         <v>103</v>
       </c>
-      <c r="W41">
+      <c r="X41">
         <v>10</v>
       </c>
-      <c r="X41" t="s">
+      <c r="Y41" t="s">
         <v>64</v>
       </c>
-      <c r="Y41">
+      <c r="Z41">
         <v>1800</v>
       </c>
-      <c r="Z41" s="1">
+      <c r="AA41" s="1">
         <v>45707.371597604164</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -4524,23 +4716,27 @@
       <c r="U42" t="s">
         <v>34</v>
       </c>
-      <c r="V42" t="s">
+      <c r="V42" s="2" t="str">
+        <f>VLOOKUP(U42,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W42" t="s">
         <v>92</v>
       </c>
-      <c r="W42">
+      <c r="X42">
         <v>31</v>
       </c>
-      <c r="X42" t="s">
+      <c r="Y42" t="s">
         <v>36</v>
       </c>
-      <c r="Y42">
+      <c r="Z42">
         <v>2500</v>
       </c>
-      <c r="Z42" s="1">
+      <c r="AA42" s="1">
         <v>45701.469520833336</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -4604,23 +4800,27 @@
       <c r="U43" t="s">
         <v>34</v>
       </c>
-      <c r="V43" t="s">
+      <c r="V43" s="2" t="str">
+        <f>VLOOKUP(U43,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W43" t="s">
         <v>92</v>
       </c>
-      <c r="W43">
+      <c r="X43">
         <v>9</v>
       </c>
-      <c r="X43" t="s">
+      <c r="Y43" t="s">
         <v>53</v>
       </c>
-      <c r="Y43">
+      <c r="Z43">
         <v>6000</v>
       </c>
-      <c r="Z43" s="1">
+      <c r="AA43" s="1">
         <v>45701.640783414354</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>26</v>
       </c>
@@ -4684,23 +4884,27 @@
       <c r="U44" t="s">
         <v>34</v>
       </c>
-      <c r="V44" t="s">
+      <c r="V44" s="2" t="str">
+        <f>VLOOKUP(U44,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W44" t="s">
         <v>92</v>
       </c>
-      <c r="W44">
+      <c r="X44">
         <v>9</v>
       </c>
-      <c r="X44" t="s">
+      <c r="Y44" t="s">
         <v>53</v>
       </c>
-      <c r="Y44">
+      <c r="Z44">
         <v>6000</v>
       </c>
-      <c r="Z44" s="1">
+      <c r="AA44" s="1">
         <v>45701.634319097226</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -4764,23 +4968,27 @@
       <c r="U45" t="s">
         <v>34</v>
       </c>
-      <c r="V45" t="s">
+      <c r="V45" s="2" t="str">
+        <f>VLOOKUP(U45,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W45" t="s">
         <v>92</v>
       </c>
-      <c r="W45">
+      <c r="X45">
         <v>9</v>
       </c>
-      <c r="X45" t="s">
+      <c r="Y45" t="s">
         <v>53</v>
       </c>
-      <c r="Y45">
+      <c r="Z45">
         <v>6000</v>
       </c>
-      <c r="Z45" s="1">
+      <c r="AA45" s="1">
         <v>45702.527147488428</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -4844,23 +5052,27 @@
       <c r="U46" t="s">
         <v>34</v>
       </c>
-      <c r="V46" t="s">
+      <c r="V46" s="2" t="str">
+        <f>VLOOKUP(U46,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W46" t="s">
         <v>92</v>
       </c>
-      <c r="W46">
+      <c r="X46">
         <v>9</v>
       </c>
-      <c r="X46" t="s">
+      <c r="Y46" t="s">
         <v>53</v>
       </c>
-      <c r="Y46">
+      <c r="Z46">
         <v>6000</v>
       </c>
-      <c r="Z46" s="1">
+      <c r="AA46" s="1">
         <v>45702.525631053242</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -4924,23 +5136,27 @@
       <c r="U47" t="s">
         <v>34</v>
       </c>
-      <c r="V47" t="s">
+      <c r="V47" s="2" t="str">
+        <f>VLOOKUP(U47,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W47" t="s">
         <v>92</v>
       </c>
-      <c r="W47">
+      <c r="X47">
         <v>9</v>
       </c>
-      <c r="X47" t="s">
+      <c r="Y47" t="s">
         <v>53</v>
       </c>
-      <c r="Y47">
+      <c r="Z47">
         <v>2500</v>
       </c>
-      <c r="Z47" s="1">
+      <c r="AA47" s="1">
         <v>45701.631847106481</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -5004,23 +5220,27 @@
       <c r="U48" t="s">
         <v>34</v>
       </c>
-      <c r="V48" t="s">
+      <c r="V48" s="2" t="str">
+        <f>VLOOKUP(U48,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W48" t="s">
         <v>92</v>
       </c>
-      <c r="W48">
+      <c r="X48">
         <v>33</v>
       </c>
-      <c r="X48" t="s">
+      <c r="Y48" t="s">
         <v>36</v>
       </c>
-      <c r="Y48">
+      <c r="Z48">
         <v>2400</v>
       </c>
-      <c r="Z48" s="1">
+      <c r="AA48" s="1">
         <v>45699.588922835646</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>26</v>
       </c>
@@ -5084,23 +5304,27 @@
       <c r="U49" t="s">
         <v>34</v>
       </c>
-      <c r="V49" t="s">
+      <c r="V49" s="2" t="str">
+        <f>VLOOKUP(U49,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W49" t="s">
         <v>92</v>
       </c>
-      <c r="W49">
+      <c r="X49">
         <v>33</v>
       </c>
-      <c r="X49" t="s">
+      <c r="Y49" t="s">
         <v>36</v>
       </c>
-      <c r="Y49">
+      <c r="Z49">
         <v>2500</v>
       </c>
-      <c r="Z49" s="1">
+      <c r="AA49" s="1">
         <v>45699.693505439813</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -5164,23 +5388,27 @@
       <c r="U50" t="s">
         <v>34</v>
       </c>
-      <c r="V50" t="s">
+      <c r="V50" s="2" t="str">
+        <f>VLOOKUP(U50,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W50" t="s">
         <v>92</v>
       </c>
-      <c r="W50">
+      <c r="X50">
         <v>33</v>
       </c>
-      <c r="X50" t="s">
+      <c r="Y50" t="s">
         <v>36</v>
       </c>
-      <c r="Y50">
+      <c r="Z50">
         <v>2500</v>
       </c>
-      <c r="Z50" s="1">
+      <c r="AA50" s="1">
         <v>45699.692172650466</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>26</v>
       </c>
@@ -5244,23 +5472,27 @@
       <c r="U51" t="s">
         <v>34</v>
       </c>
-      <c r="V51" t="s">
+      <c r="V51" s="2" t="str">
+        <f>VLOOKUP(U51,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W51" t="s">
         <v>92</v>
       </c>
-      <c r="W51">
+      <c r="X51">
         <v>33</v>
       </c>
-      <c r="X51" t="s">
+      <c r="Y51" t="s">
         <v>36</v>
       </c>
-      <c r="Y51">
+      <c r="Z51">
         <v>2200</v>
       </c>
-      <c r="Z51" s="1">
+      <c r="AA51" s="1">
         <v>45699.690588576392</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>26</v>
       </c>
@@ -5324,23 +5556,27 @@
       <c r="U52" t="s">
         <v>34</v>
       </c>
-      <c r="V52" t="s">
+      <c r="V52" s="2" t="str">
+        <f>VLOOKUP(U52,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W52" t="s">
         <v>92</v>
       </c>
-      <c r="W52">
+      <c r="X52">
         <v>9</v>
       </c>
-      <c r="X52" t="s">
+      <c r="Y52" t="s">
         <v>53</v>
       </c>
-      <c r="Y52">
+      <c r="Z52">
         <v>4500</v>
       </c>
-      <c r="Z52" s="1">
+      <c r="AA52" s="1">
         <v>45701.637598877314</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -5404,23 +5640,27 @@
       <c r="U53" t="s">
         <v>34</v>
       </c>
-      <c r="V53" t="s">
+      <c r="V53" s="2" t="str">
+        <f>VLOOKUP(U53,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W53" t="s">
         <v>92</v>
       </c>
-      <c r="W53">
+      <c r="X53">
         <v>33</v>
       </c>
-      <c r="X53" t="s">
+      <c r="Y53" t="s">
         <v>36</v>
       </c>
-      <c r="Y53">
+      <c r="Z53">
         <v>2500</v>
       </c>
-      <c r="Z53" s="1">
+      <c r="AA53" s="1">
         <v>45699.696334143518</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -5484,23 +5724,27 @@
       <c r="U54" t="s">
         <v>34</v>
       </c>
-      <c r="V54" t="s">
+      <c r="V54" s="2" t="str">
+        <f>VLOOKUP(U54,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W54" t="s">
         <v>127</v>
       </c>
-      <c r="W54">
+      <c r="X54">
         <v>10</v>
       </c>
-      <c r="X54" t="s">
+      <c r="Y54" t="s">
         <v>64</v>
       </c>
-      <c r="Y54">
+      <c r="Z54">
         <v>1250</v>
       </c>
-      <c r="Z54" s="1">
+      <c r="AA54" s="1">
         <v>45707.63599490741</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>26</v>
       </c>
@@ -5564,23 +5808,27 @@
       <c r="U55" t="s">
         <v>34</v>
       </c>
-      <c r="V55" t="s">
+      <c r="V55" s="2" t="str">
+        <f>VLOOKUP(U55,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W55" t="s">
         <v>103</v>
       </c>
-      <c r="W55">
+      <c r="X55">
         <v>23</v>
       </c>
-      <c r="X55" t="s">
+      <c r="Y55" t="s">
         <v>36</v>
       </c>
-      <c r="Y55">
+      <c r="Z55">
         <v>2200</v>
       </c>
-      <c r="Z55" s="1">
+      <c r="AA55" s="1">
         <v>45699.540004513889</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -5644,23 +5892,27 @@
       <c r="U56" t="s">
         <v>34</v>
       </c>
-      <c r="V56" t="s">
+      <c r="V56" s="2" t="str">
+        <f>VLOOKUP(U56,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W56" t="s">
         <v>92</v>
       </c>
-      <c r="W56">
+      <c r="X56">
         <v>24</v>
       </c>
-      <c r="X56" t="s">
+      <c r="Y56" t="s">
         <v>36</v>
       </c>
-      <c r="Y56">
+      <c r="Z56">
         <v>2000</v>
       </c>
-      <c r="Z56" s="1">
+      <c r="AA56" s="1">
         <v>45712.713480208331</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>26</v>
       </c>
@@ -5724,23 +5976,27 @@
       <c r="U57" t="s">
         <v>34</v>
       </c>
-      <c r="V57" t="s">
+      <c r="V57" s="2" t="str">
+        <f>VLOOKUP(U57,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W57" t="s">
         <v>92</v>
       </c>
-      <c r="W57">
-        <v>26</v>
-      </c>
-      <c r="X57" t="s">
+      <c r="X57">
+        <v>26</v>
+      </c>
+      <c r="Y57" t="s">
         <v>36</v>
       </c>
-      <c r="Y57">
+      <c r="Z57">
         <v>2500</v>
       </c>
-      <c r="Z57" s="1">
+      <c r="AA57" s="1">
         <v>45712.709774456016</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>26</v>
       </c>
@@ -5804,23 +6060,27 @@
       <c r="U58" t="s">
         <v>34</v>
       </c>
-      <c r="V58" t="s">
+      <c r="V58" s="2" t="str">
+        <f>VLOOKUP(U58,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W58" t="s">
         <v>92</v>
       </c>
-      <c r="W58">
-        <v>26</v>
-      </c>
-      <c r="X58" t="s">
+      <c r="X58">
+        <v>26</v>
+      </c>
+      <c r="Y58" t="s">
         <v>36</v>
       </c>
-      <c r="Y58">
+      <c r="Z58">
         <v>1500</v>
       </c>
-      <c r="Z58" s="1">
+      <c r="AA58" s="1">
         <v>45715.433138854169</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>26</v>
       </c>
@@ -5884,23 +6144,27 @@
       <c r="U59" t="s">
         <v>34</v>
       </c>
-      <c r="V59" t="s">
+      <c r="V59" s="2" t="str">
+        <f>VLOOKUP(U59,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W59" t="s">
         <v>92</v>
       </c>
-      <c r="W59">
-        <v>26</v>
-      </c>
-      <c r="X59" t="s">
+      <c r="X59">
+        <v>26</v>
+      </c>
+      <c r="Y59" t="s">
         <v>36</v>
       </c>
-      <c r="Y59">
+      <c r="Z59">
         <v>2000</v>
       </c>
-      <c r="Z59" s="1">
+      <c r="AA59" s="1">
         <v>45716.696389895835</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>26</v>
       </c>
@@ -5964,23 +6228,27 @@
       <c r="U60" t="s">
         <v>34</v>
       </c>
-      <c r="V60" t="s">
+      <c r="V60" s="2" t="str">
+        <f>VLOOKUP(U60,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W60" t="s">
         <v>92</v>
       </c>
-      <c r="W60">
+      <c r="X60">
         <v>33</v>
       </c>
-      <c r="X60" t="s">
+      <c r="Y60" t="s">
         <v>36</v>
       </c>
-      <c r="Y60">
+      <c r="Z60">
         <v>2800</v>
       </c>
-      <c r="Z60" s="1">
+      <c r="AA60" s="1">
         <v>45708.642616898149</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -6044,23 +6312,27 @@
       <c r="U61" t="s">
         <v>34</v>
       </c>
-      <c r="V61" t="s">
+      <c r="V61" s="2" t="str">
+        <f>VLOOKUP(U61,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W61" t="s">
         <v>92</v>
       </c>
-      <c r="W61">
+      <c r="X61">
         <v>33</v>
       </c>
-      <c r="X61" t="s">
+      <c r="Y61" t="s">
         <v>36</v>
       </c>
-      <c r="Y61">
+      <c r="Z61">
         <v>2500</v>
       </c>
-      <c r="Z61" s="1">
+      <c r="AA61" s="1">
         <v>45708.63907607639</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>26</v>
       </c>
@@ -6124,23 +6396,27 @@
       <c r="U62" t="s">
         <v>34</v>
       </c>
-      <c r="V62" t="s">
+      <c r="V62" s="2" t="str">
+        <f>VLOOKUP(U62,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W62" t="s">
         <v>149</v>
       </c>
-      <c r="W62">
+      <c r="X62">
         <v>24</v>
       </c>
-      <c r="X62" t="s">
+      <c r="Y62" t="s">
         <v>36</v>
       </c>
-      <c r="Y62">
+      <c r="Z62">
         <v>500</v>
       </c>
-      <c r="Z62" s="1">
+      <c r="AA62" s="1">
         <v>45712.708242210647</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>26</v>
       </c>
@@ -6204,23 +6480,27 @@
       <c r="U63" t="s">
         <v>34</v>
       </c>
-      <c r="V63" t="s">
+      <c r="V63" s="2" t="str">
+        <f>VLOOKUP(U63,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W63" t="s">
         <v>153</v>
       </c>
-      <c r="W63">
+      <c r="X63">
         <v>64</v>
       </c>
-      <c r="X63" t="s">
+      <c r="Y63" t="s">
         <v>154</v>
       </c>
-      <c r="Y63">
+      <c r="Z63">
         <v>400</v>
       </c>
-      <c r="Z63" s="1">
+      <c r="AA63" s="1">
         <v>45716.695539618057</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -6284,23 +6564,27 @@
       <c r="U64" t="s">
         <v>34</v>
       </c>
-      <c r="V64" t="s">
+      <c r="V64" s="2" t="str">
+        <f>VLOOKUP(U64,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W64" t="s">
         <v>103</v>
       </c>
-      <c r="W64">
+      <c r="X64">
         <v>58</v>
       </c>
-      <c r="X64" t="s">
+      <c r="Y64" t="s">
         <v>36</v>
       </c>
-      <c r="Y64">
+      <c r="Z64">
         <v>2000</v>
       </c>
-      <c r="Z64" s="1">
+      <c r="AA64" s="1">
         <v>45700.662263541664</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>26</v>
       </c>
@@ -6364,23 +6648,27 @@
       <c r="U65" t="s">
         <v>34</v>
       </c>
-      <c r="V65" t="s">
+      <c r="V65" s="2" t="str">
+        <f>VLOOKUP(U65,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W65" t="s">
         <v>103</v>
       </c>
-      <c r="W65">
+      <c r="X65">
         <v>58</v>
       </c>
-      <c r="X65" t="s">
+      <c r="Y65" t="s">
         <v>36</v>
       </c>
-      <c r="Y65">
+      <c r="Z65">
         <v>2000</v>
       </c>
-      <c r="Z65" s="1">
+      <c r="AA65" s="1">
         <v>45700.662263541664</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>26</v>
       </c>
@@ -6444,23 +6732,27 @@
       <c r="U66" t="s">
         <v>34</v>
       </c>
-      <c r="V66" t="s">
+      <c r="V66" s="2" t="str">
+        <f>VLOOKUP(U66,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W66" t="s">
         <v>103</v>
       </c>
-      <c r="W66">
+      <c r="X66">
         <v>58</v>
       </c>
-      <c r="X66" t="s">
+      <c r="Y66" t="s">
         <v>36</v>
       </c>
-      <c r="Y66">
+      <c r="Z66">
         <v>2000</v>
       </c>
-      <c r="Z66" s="1">
+      <c r="AA66" s="1">
         <v>45700.663486226855</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -6524,23 +6816,27 @@
       <c r="U67" t="s">
         <v>34</v>
       </c>
-      <c r="V67" t="s">
+      <c r="V67" s="2" t="str">
+        <f>VLOOKUP(U67,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W67" t="s">
         <v>103</v>
       </c>
-      <c r="W67">
+      <c r="X67">
         <v>58</v>
       </c>
-      <c r="X67" t="s">
+      <c r="Y67" t="s">
         <v>36</v>
       </c>
-      <c r="Y67">
+      <c r="Z67">
         <v>2000</v>
       </c>
-      <c r="Z67" s="1">
+      <c r="AA67" s="1">
         <v>45700.663486226855</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>26</v>
       </c>
@@ -6604,23 +6900,27 @@
       <c r="U68" t="s">
         <v>34</v>
       </c>
-      <c r="V68" t="s">
+      <c r="V68" s="2" t="str">
+        <f>VLOOKUP(U68,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W68" t="s">
         <v>103</v>
       </c>
-      <c r="W68">
+      <c r="X68">
         <v>58</v>
       </c>
-      <c r="X68" t="s">
+      <c r="Y68" t="s">
         <v>36</v>
       </c>
-      <c r="Y68">
+      <c r="Z68">
         <v>2000</v>
       </c>
-      <c r="Z68" s="1">
+      <c r="AA68" s="1">
         <v>45700.661114201386</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>26</v>
       </c>
@@ -6684,23 +6984,27 @@
       <c r="U69" t="s">
         <v>34</v>
       </c>
-      <c r="V69" t="s">
+      <c r="V69" s="2" t="str">
+        <f>VLOOKUP(U69,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W69" t="s">
         <v>103</v>
       </c>
-      <c r="W69">
+      <c r="X69">
         <v>58</v>
       </c>
-      <c r="X69" t="s">
+      <c r="Y69" t="s">
         <v>36</v>
       </c>
-      <c r="Y69">
+      <c r="Z69">
         <v>2000</v>
       </c>
-      <c r="Z69" s="1">
+      <c r="AA69" s="1">
         <v>45700.661114201386</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>26</v>
       </c>
@@ -6764,23 +7068,27 @@
       <c r="U70" t="s">
         <v>34</v>
       </c>
-      <c r="V70" t="s">
+      <c r="V70" s="2" t="str">
+        <f>VLOOKUP(U70,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W70" t="s">
         <v>103</v>
       </c>
-      <c r="W70">
+      <c r="X70">
         <v>58</v>
       </c>
-      <c r="X70" t="s">
+      <c r="Y70" t="s">
         <v>36</v>
       </c>
-      <c r="Y70">
+      <c r="Z70">
         <v>2000</v>
       </c>
-      <c r="Z70" s="1">
+      <c r="AA70" s="1">
         <v>45700.652947372684</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>26</v>
       </c>
@@ -6844,23 +7152,27 @@
       <c r="U71" t="s">
         <v>34</v>
       </c>
-      <c r="V71" t="s">
+      <c r="V71" s="2" t="str">
+        <f>VLOOKUP(U71,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W71" t="s">
         <v>103</v>
       </c>
-      <c r="W71">
+      <c r="X71">
         <v>58</v>
       </c>
-      <c r="X71" t="s">
+      <c r="Y71" t="s">
         <v>36</v>
       </c>
-      <c r="Y71">
+      <c r="Z71">
         <v>2000</v>
       </c>
-      <c r="Z71" s="1">
+      <c r="AA71" s="1">
         <v>45700.652947372684</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>26</v>
       </c>
@@ -6924,23 +7236,27 @@
       <c r="U72" t="s">
         <v>34</v>
       </c>
-      <c r="V72" t="s">
+      <c r="V72" s="2" t="str">
+        <f>VLOOKUP(U72,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W72" t="s">
         <v>103</v>
       </c>
-      <c r="W72">
+      <c r="X72">
         <v>58</v>
       </c>
-      <c r="X72" t="s">
+      <c r="Y72" t="s">
         <v>36</v>
       </c>
-      <c r="Y72">
+      <c r="Z72">
         <v>2000</v>
       </c>
-      <c r="Z72" s="1">
+      <c r="AA72" s="1">
         <v>45700.654281944444</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>26</v>
       </c>
@@ -7004,23 +7320,27 @@
       <c r="U73" t="s">
         <v>34</v>
       </c>
-      <c r="V73" t="s">
+      <c r="V73" s="2" t="str">
+        <f>VLOOKUP(U73,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W73" t="s">
         <v>103</v>
       </c>
-      <c r="W73">
+      <c r="X73">
         <v>58</v>
       </c>
-      <c r="X73" t="s">
+      <c r="Y73" t="s">
         <v>36</v>
       </c>
-      <c r="Y73">
+      <c r="Z73">
         <v>2000</v>
       </c>
-      <c r="Z73" s="1">
+      <c r="AA73" s="1">
         <v>45700.654281944444</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>26</v>
       </c>
@@ -7084,23 +7404,27 @@
       <c r="U74" t="s">
         <v>34</v>
       </c>
-      <c r="V74" t="s">
+      <c r="V74" s="2" t="str">
+        <f>VLOOKUP(U74,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W74" t="s">
         <v>103</v>
       </c>
-      <c r="W74">
+      <c r="X74">
         <v>58</v>
       </c>
-      <c r="X74" t="s">
+      <c r="Y74" t="s">
         <v>36</v>
       </c>
-      <c r="Y74">
+      <c r="Z74">
         <v>2000</v>
       </c>
-      <c r="Z74" s="1">
+      <c r="AA74" s="1">
         <v>45702.509515891201</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -7164,23 +7488,27 @@
       <c r="U75" t="s">
         <v>34</v>
       </c>
-      <c r="V75" t="s">
+      <c r="V75" s="2" t="str">
+        <f>VLOOKUP(U75,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W75" t="s">
         <v>103</v>
       </c>
-      <c r="W75">
+      <c r="X75">
         <v>58</v>
       </c>
-      <c r="X75" t="s">
+      <c r="Y75" t="s">
         <v>36</v>
       </c>
-      <c r="Y75">
+      <c r="Z75">
         <v>2000</v>
       </c>
-      <c r="Z75" s="1">
+      <c r="AA75" s="1">
         <v>45702.509515891201</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>26</v>
       </c>
@@ -7244,23 +7572,27 @@
       <c r="U76" t="s">
         <v>34</v>
       </c>
-      <c r="V76" t="s">
+      <c r="V76" s="2" t="str">
+        <f>VLOOKUP(U76,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W76" t="s">
         <v>103</v>
       </c>
-      <c r="W76">
+      <c r="X76">
         <v>58</v>
       </c>
-      <c r="X76" t="s">
+      <c r="Y76" t="s">
         <v>36</v>
       </c>
-      <c r="Y76">
+      <c r="Z76">
         <v>2000</v>
       </c>
-      <c r="Z76" s="1">
+      <c r="AA76" s="1">
         <v>45700.659497835652</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>26</v>
       </c>
@@ -7324,23 +7656,27 @@
       <c r="U77" t="s">
         <v>34</v>
       </c>
-      <c r="V77" t="s">
+      <c r="V77" s="2" t="str">
+        <f>VLOOKUP(U77,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W77" t="s">
         <v>103</v>
       </c>
-      <c r="W77">
+      <c r="X77">
         <v>58</v>
       </c>
-      <c r="X77" t="s">
+      <c r="Y77" t="s">
         <v>36</v>
       </c>
-      <c r="Y77">
+      <c r="Z77">
         <v>2000</v>
       </c>
-      <c r="Z77" s="1">
+      <c r="AA77" s="1">
         <v>45700.659497835652</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>26</v>
       </c>
@@ -7404,23 +7740,27 @@
       <c r="U78" t="s">
         <v>34</v>
       </c>
-      <c r="V78" t="s">
+      <c r="V78" s="2" t="str">
+        <f>VLOOKUP(U78,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W78" t="s">
         <v>103</v>
       </c>
-      <c r="W78">
+      <c r="X78">
         <v>58</v>
       </c>
-      <c r="X78" t="s">
+      <c r="Y78" t="s">
         <v>36</v>
       </c>
-      <c r="Y78">
+      <c r="Z78">
         <v>2000</v>
       </c>
-      <c r="Z78" s="1">
+      <c r="AA78" s="1">
         <v>45700.651365474536</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>26</v>
       </c>
@@ -7484,23 +7824,27 @@
       <c r="U79" t="s">
         <v>34</v>
       </c>
-      <c r="V79" t="s">
+      <c r="V79" s="2" t="str">
+        <f>VLOOKUP(U79,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W79" t="s">
         <v>103</v>
       </c>
-      <c r="W79">
+      <c r="X79">
         <v>58</v>
       </c>
-      <c r="X79" t="s">
+      <c r="Y79" t="s">
         <v>36</v>
       </c>
-      <c r="Y79">
+      <c r="Z79">
         <v>2000</v>
       </c>
-      <c r="Z79" s="1">
+      <c r="AA79" s="1">
         <v>45700.651365474536</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>26</v>
       </c>
@@ -7564,23 +7908,27 @@
       <c r="U80" t="s">
         <v>34</v>
       </c>
-      <c r="V80" t="s">
+      <c r="V80" s="2" t="str">
+        <f>VLOOKUP(U80,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W80" t="s">
         <v>103</v>
       </c>
-      <c r="W80">
+      <c r="X80">
         <v>58</v>
       </c>
-      <c r="X80" t="s">
+      <c r="Y80" t="s">
         <v>36</v>
       </c>
-      <c r="Y80">
+      <c r="Z80">
         <v>2000</v>
       </c>
-      <c r="Z80" s="1">
+      <c r="AA80" s="1">
         <v>45702.520452280092</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>26</v>
       </c>
@@ -7644,23 +7992,27 @@
       <c r="U81" t="s">
         <v>34</v>
       </c>
-      <c r="V81" t="s">
+      <c r="V81" s="2" t="str">
+        <f>VLOOKUP(U81,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W81" t="s">
         <v>103</v>
       </c>
-      <c r="W81">
+      <c r="X81">
         <v>58</v>
       </c>
-      <c r="X81" t="s">
+      <c r="Y81" t="s">
         <v>36</v>
       </c>
-      <c r="Y81">
+      <c r="Z81">
         <v>2000</v>
       </c>
-      <c r="Z81" s="1">
+      <c r="AA81" s="1">
         <v>45702.520452280092</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>26</v>
       </c>
@@ -7724,23 +8076,27 @@
       <c r="U82" t="s">
         <v>34</v>
       </c>
-      <c r="V82" t="s">
+      <c r="V82" s="2" t="str">
+        <f>VLOOKUP(U82,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W82" t="s">
         <v>103</v>
       </c>
-      <c r="W82">
+      <c r="X82">
         <v>58</v>
       </c>
-      <c r="X82" t="s">
+      <c r="Y82" t="s">
         <v>36</v>
       </c>
-      <c r="Y82">
+      <c r="Z82">
         <v>2000</v>
       </c>
-      <c r="Z82" s="1">
+      <c r="AA82" s="1">
         <v>45700.658020451388</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>26</v>
       </c>
@@ -7804,23 +8160,27 @@
       <c r="U83" t="s">
         <v>34</v>
       </c>
-      <c r="V83" t="s">
+      <c r="V83" s="2" t="str">
+        <f>VLOOKUP(U83,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W83" t="s">
         <v>103</v>
       </c>
-      <c r="W83">
+      <c r="X83">
         <v>58</v>
       </c>
-      <c r="X83" t="s">
+      <c r="Y83" t="s">
         <v>36</v>
       </c>
-      <c r="Y83">
+      <c r="Z83">
         <v>2000</v>
       </c>
-      <c r="Z83" s="1">
+      <c r="AA83" s="1">
         <v>45700.658020451388</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>26</v>
       </c>
@@ -7884,23 +8244,27 @@
       <c r="U84" t="s">
         <v>34</v>
       </c>
-      <c r="V84" t="s">
+      <c r="V84" s="2" t="str">
+        <f>VLOOKUP(U84,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W84" t="s">
         <v>92</v>
       </c>
-      <c r="W84">
+      <c r="X84">
         <v>33</v>
       </c>
-      <c r="X84" t="s">
+      <c r="Y84" t="s">
         <v>36</v>
       </c>
-      <c r="Y84">
+      <c r="Z84">
         <v>2500</v>
       </c>
-      <c r="Z84" s="1">
+      <c r="AA84" s="1">
         <v>45699.695142824072</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>26</v>
       </c>
@@ -7964,23 +8328,27 @@
       <c r="U85" t="s">
         <v>34</v>
       </c>
-      <c r="V85" t="s">
+      <c r="V85" s="2" t="str">
+        <f>VLOOKUP(U85,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W85" t="s">
         <v>103</v>
       </c>
-      <c r="W85">
+      <c r="X85">
         <v>58</v>
       </c>
-      <c r="X85" t="s">
+      <c r="Y85" t="s">
         <v>36</v>
       </c>
-      <c r="Y85">
+      <c r="Z85">
         <v>2000</v>
       </c>
-      <c r="Z85" s="1">
+      <c r="AA85" s="1">
         <v>45700.655673067129</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>26</v>
       </c>
@@ -8044,23 +8412,27 @@
       <c r="U86" t="s">
         <v>34</v>
       </c>
-      <c r="V86" t="s">
+      <c r="V86" s="2" t="str">
+        <f>VLOOKUP(U86,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W86" t="s">
         <v>103</v>
       </c>
-      <c r="W86">
+      <c r="X86">
         <v>58</v>
       </c>
-      <c r="X86" t="s">
+      <c r="Y86" t="s">
         <v>36</v>
       </c>
-      <c r="Y86">
+      <c r="Z86">
         <v>2000</v>
       </c>
-      <c r="Z86" s="1">
+      <c r="AA86" s="1">
         <v>45700.655673067129</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>26</v>
       </c>
@@ -8124,23 +8496,27 @@
       <c r="U87" t="s">
         <v>34</v>
       </c>
-      <c r="V87" t="s">
+      <c r="V87" s="2" t="str">
+        <f>VLOOKUP(U87,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W87" t="s">
         <v>153</v>
       </c>
-      <c r="W87">
+      <c r="X87">
         <v>64</v>
       </c>
-      <c r="X87" t="s">
+      <c r="Y87" t="s">
         <v>154</v>
       </c>
-      <c r="Y87">
+      <c r="Z87">
         <v>533.33000000000004</v>
       </c>
-      <c r="Z87" s="1">
+      <c r="AA87" s="1">
         <v>45715.621550729164</v>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>26</v>
       </c>
@@ -8204,23 +8580,27 @@
       <c r="U88" t="s">
         <v>34</v>
       </c>
-      <c r="V88" t="s">
+      <c r="V88" s="2" t="str">
+        <f>VLOOKUP(U88,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W88" t="s">
         <v>92</v>
       </c>
-      <c r="W88">
+      <c r="X88">
         <v>60</v>
       </c>
-      <c r="X88" t="s">
+      <c r="Y88" t="s">
         <v>36</v>
       </c>
-      <c r="Y88">
+      <c r="Z88">
         <v>2500</v>
       </c>
-      <c r="Z88" s="1">
+      <c r="AA88" s="1">
         <v>45712.705184687497</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>26</v>
       </c>
@@ -8284,23 +8664,27 @@
       <c r="U89" t="s">
         <v>34</v>
       </c>
-      <c r="V89" t="s">
+      <c r="V89" s="2" t="str">
+        <f>VLOOKUP(U89,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W89" t="s">
         <v>92</v>
       </c>
-      <c r="W89">
+      <c r="X89">
         <v>65</v>
       </c>
-      <c r="X89" t="s">
+      <c r="Y89" t="s">
         <v>53</v>
       </c>
-      <c r="Y89">
+      <c r="Z89">
         <v>2200</v>
       </c>
-      <c r="Z89" s="1">
+      <c r="AA89" s="1">
         <v>45712.710528275464</v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>26</v>
       </c>
@@ -8364,23 +8748,27 @@
       <c r="U90" t="s">
         <v>34</v>
       </c>
-      <c r="V90" t="s">
+      <c r="V90" s="2" t="str">
+        <f>VLOOKUP(U90,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W90" t="s">
         <v>92</v>
       </c>
-      <c r="W90">
+      <c r="X90">
         <v>65</v>
       </c>
-      <c r="X90" t="s">
+      <c r="Y90" t="s">
         <v>53</v>
       </c>
-      <c r="Y90">
+      <c r="Z90">
         <v>2800</v>
       </c>
-      <c r="Z90" s="1">
+      <c r="AA90" s="1">
         <v>45712.715031793981</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>26</v>
       </c>
@@ -8444,23 +8832,27 @@
       <c r="U91" t="s">
         <v>34</v>
       </c>
-      <c r="V91" t="s">
+      <c r="V91" s="2" t="str">
+        <f>VLOOKUP(U91,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W91" t="s">
         <v>149</v>
       </c>
-      <c r="W91">
+      <c r="X91">
         <v>58</v>
       </c>
-      <c r="X91" t="s">
+      <c r="Y91" t="s">
         <v>36</v>
       </c>
-      <c r="Y91">
+      <c r="Z91">
         <v>1496</v>
       </c>
-      <c r="Z91" s="1">
+      <c r="AA91" s="1">
         <v>45715.423745601853</v>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>26</v>
       </c>
@@ -8524,23 +8916,27 @@
       <c r="U92" t="s">
         <v>34</v>
       </c>
-      <c r="V92" t="s">
+      <c r="V92" s="2" t="str">
+        <f>VLOOKUP(U92,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W92" t="s">
         <v>179</v>
       </c>
-      <c r="W92">
+      <c r="X92">
         <v>24</v>
       </c>
-      <c r="X92" t="s">
+      <c r="Y92" t="s">
         <v>36</v>
       </c>
-      <c r="Y92">
+      <c r="Z92">
         <v>7464.6</v>
       </c>
-      <c r="Z92" s="1">
+      <c r="AA92" s="1">
         <v>45692.523941203704</v>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>26</v>
       </c>
@@ -8604,23 +9000,27 @@
       <c r="U93" t="s">
         <v>34</v>
       </c>
-      <c r="V93" t="s">
+      <c r="V93" s="2" t="str">
+        <f>VLOOKUP(U93,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W93" t="s">
         <v>92</v>
       </c>
-      <c r="W93">
-        <v>32</v>
-      </c>
-      <c r="X93" t="s">
+      <c r="X93">
+        <v>32</v>
+      </c>
+      <c r="Y93" t="s">
         <v>36</v>
       </c>
-      <c r="Y93">
+      <c r="Z93">
         <v>2000</v>
       </c>
-      <c r="Z93" s="1">
+      <c r="AA93" s="1">
         <v>45706.432341238426</v>
       </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>26</v>
       </c>
@@ -8684,23 +9084,27 @@
       <c r="U94" t="s">
         <v>34</v>
       </c>
-      <c r="V94" t="s">
+      <c r="V94" s="2" t="str">
+        <f>VLOOKUP(U94,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W94" t="s">
         <v>149</v>
       </c>
-      <c r="W94">
+      <c r="X94">
         <v>24</v>
       </c>
-      <c r="X94" t="s">
+      <c r="Y94" t="s">
         <v>36</v>
       </c>
-      <c r="Y94">
+      <c r="Z94">
         <v>150</v>
       </c>
-      <c r="Z94" s="1">
+      <c r="AA94" s="1">
         <v>45712.714414930553</v>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>26</v>
       </c>
@@ -8764,23 +9168,27 @@
       <c r="U95" t="s">
         <v>190</v>
       </c>
-      <c r="V95" t="s">
+      <c r="V95" s="2" t="str">
+        <f>VLOOKUP(U95,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">09: RECURSOS DIRECTAMENTE RECAUDADOS                                                                                                                      </v>
+      </c>
+      <c r="W95" t="s">
         <v>103</v>
       </c>
-      <c r="W95">
+      <c r="X95">
         <v>45</v>
       </c>
-      <c r="X95" t="s">
+      <c r="Y95" t="s">
         <v>36</v>
       </c>
-      <c r="Y95">
+      <c r="Z95">
         <v>1700</v>
       </c>
-      <c r="Z95" s="1">
+      <c r="AA95" s="1">
         <v>45715.431714895836</v>
       </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>26</v>
       </c>
@@ -8844,23 +9252,27 @@
       <c r="U96" t="s">
         <v>34</v>
       </c>
-      <c r="V96" t="s">
+      <c r="V96" s="2" t="str">
+        <f>VLOOKUP(U96,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W96" t="s">
         <v>103</v>
       </c>
-      <c r="W96">
+      <c r="X96">
         <v>58</v>
       </c>
-      <c r="X96" t="s">
+      <c r="Y96" t="s">
         <v>36</v>
       </c>
-      <c r="Y96">
+      <c r="Z96">
         <v>2000</v>
       </c>
-      <c r="Z96" s="1">
+      <c r="AA96" s="1">
         <v>45699.697784062497</v>
       </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>26</v>
       </c>
@@ -8924,23 +9336,27 @@
       <c r="U97" t="s">
         <v>34</v>
       </c>
-      <c r="V97" t="s">
+      <c r="V97" s="2" t="str">
+        <f>VLOOKUP(U97,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W97" t="s">
         <v>103</v>
       </c>
-      <c r="W97">
+      <c r="X97">
         <v>58</v>
       </c>
-      <c r="X97" t="s">
+      <c r="Y97" t="s">
         <v>36</v>
       </c>
-      <c r="Y97">
+      <c r="Z97">
         <v>2000</v>
       </c>
-      <c r="Z97" s="1">
+      <c r="AA97" s="1">
         <v>45699.697784062497</v>
       </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>26</v>
       </c>
@@ -9004,23 +9420,27 @@
       <c r="U98" t="s">
         <v>34</v>
       </c>
-      <c r="V98" t="s">
+      <c r="V98" s="2" t="str">
+        <f>VLOOKUP(U98,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W98" t="s">
         <v>92</v>
       </c>
-      <c r="W98">
+      <c r="X98">
         <v>67</v>
       </c>
-      <c r="X98" t="s">
+      <c r="Y98" t="s">
         <v>197</v>
       </c>
-      <c r="Y98">
+      <c r="Z98">
         <v>2800</v>
       </c>
-      <c r="Z98" s="1">
+      <c r="AA98" s="1">
         <v>45715.627838229164</v>
       </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>26</v>
       </c>
@@ -9084,23 +9504,27 @@
       <c r="U99" t="s">
         <v>34</v>
       </c>
-      <c r="V99" t="s">
+      <c r="V99" s="2" t="str">
+        <f>VLOOKUP(U99,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W99" t="s">
         <v>92</v>
       </c>
-      <c r="W99">
+      <c r="X99">
         <v>67</v>
       </c>
-      <c r="X99" t="s">
+      <c r="Y99" t="s">
         <v>197</v>
       </c>
-      <c r="Y99">
+      <c r="Z99">
         <v>2800</v>
       </c>
-      <c r="Z99" s="1">
+      <c r="AA99" s="1">
         <v>45715.634292673611</v>
       </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>26</v>
       </c>
@@ -9164,23 +9588,27 @@
       <c r="U100" t="s">
         <v>34</v>
       </c>
-      <c r="V100" t="s">
+      <c r="V100" s="2" t="str">
+        <f>VLOOKUP(U100,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W100" t="s">
         <v>92</v>
       </c>
-      <c r="W100">
+      <c r="X100">
         <v>67</v>
       </c>
-      <c r="X100" t="s">
+      <c r="Y100" t="s">
         <v>197</v>
       </c>
-      <c r="Y100">
+      <c r="Z100">
         <v>2800</v>
       </c>
-      <c r="Z100" s="1">
+      <c r="AA100" s="1">
         <v>45715.619089155094</v>
       </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>26</v>
       </c>
@@ -9244,23 +9672,27 @@
       <c r="U101" t="s">
         <v>34</v>
       </c>
-      <c r="V101" t="s">
+      <c r="V101" s="2" t="str">
+        <f>VLOOKUP(U101,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W101" t="s">
         <v>92</v>
       </c>
-      <c r="W101">
+      <c r="X101">
         <v>67</v>
       </c>
-      <c r="X101" t="s">
+      <c r="Y101" t="s">
         <v>197</v>
       </c>
-      <c r="Y101">
+      <c r="Z101">
         <v>2800</v>
       </c>
-      <c r="Z101" s="1">
+      <c r="AA101" s="1">
         <v>45715.620652199075</v>
       </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>26</v>
       </c>
@@ -9324,23 +9756,27 @@
       <c r="U102" t="s">
         <v>34</v>
       </c>
-      <c r="V102" t="s">
+      <c r="V102" s="2" t="str">
+        <f>VLOOKUP(U102,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W102" t="s">
         <v>92</v>
       </c>
-      <c r="W102">
+      <c r="X102">
         <v>67</v>
       </c>
-      <c r="X102" t="s">
+      <c r="Y102" t="s">
         <v>197</v>
       </c>
-      <c r="Y102">
+      <c r="Z102">
         <v>2800</v>
       </c>
-      <c r="Z102" s="1">
+      <c r="AA102" s="1">
         <v>45715.617958136572</v>
       </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>26</v>
       </c>
@@ -9404,23 +9840,27 @@
       <c r="U103" t="s">
         <v>34</v>
       </c>
-      <c r="V103" t="s">
+      <c r="V103" s="2" t="str">
+        <f>VLOOKUP(U103,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W103" t="s">
         <v>92</v>
       </c>
-      <c r="W103">
+      <c r="X103">
         <v>67</v>
       </c>
-      <c r="X103" t="s">
+      <c r="Y103" t="s">
         <v>197</v>
       </c>
-      <c r="Y103">
+      <c r="Z103">
         <v>2800</v>
       </c>
-      <c r="Z103" s="1">
+      <c r="AA103" s="1">
         <v>45715.61500150463</v>
       </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>26</v>
       </c>
@@ -9484,23 +9924,27 @@
       <c r="U104" t="s">
         <v>34</v>
       </c>
-      <c r="V104" t="s">
+      <c r="V104" s="2" t="str">
+        <f>VLOOKUP(U104,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W104" t="s">
         <v>92</v>
       </c>
-      <c r="W104">
+      <c r="X104">
         <v>65</v>
       </c>
-      <c r="X104" t="s">
+      <c r="Y104" t="s">
         <v>53</v>
       </c>
-      <c r="Y104">
+      <c r="Z104">
         <v>2800</v>
       </c>
-      <c r="Z104" s="1">
+      <c r="AA104" s="1">
         <v>45712.703846261575</v>
       </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>26</v>
       </c>
@@ -9564,23 +10008,27 @@
       <c r="U105" t="s">
         <v>34</v>
       </c>
-      <c r="V105" t="s">
+      <c r="V105" s="2" t="str">
+        <f>VLOOKUP(U105,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W105" t="s">
         <v>79</v>
       </c>
-      <c r="W105">
+      <c r="X105">
         <v>29</v>
       </c>
-      <c r="X105" t="s">
+      <c r="Y105" t="s">
         <v>36</v>
       </c>
-      <c r="Y105">
+      <c r="Z105">
         <v>2200</v>
       </c>
-      <c r="Z105" s="1">
+      <c r="AA105" s="1">
         <v>45713.632253668984</v>
       </c>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>26</v>
       </c>
@@ -9644,23 +10092,27 @@
       <c r="U106" t="s">
         <v>34</v>
       </c>
-      <c r="V106" t="s">
+      <c r="V106" s="2" t="str">
+        <f>VLOOKUP(U106,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W106" t="s">
         <v>103</v>
       </c>
-      <c r="W106">
+      <c r="X106">
         <v>22</v>
       </c>
-      <c r="X106" t="s">
+      <c r="Y106" t="s">
         <v>36</v>
       </c>
-      <c r="Y106">
+      <c r="Z106">
         <v>2000</v>
       </c>
-      <c r="Z106" s="1">
+      <c r="AA106" s="1">
         <v>45702.524119178241</v>
       </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>26</v>
       </c>
@@ -9724,23 +10176,27 @@
       <c r="U107" t="s">
         <v>34</v>
       </c>
-      <c r="V107" t="s">
+      <c r="V107" s="2" t="str">
+        <f>VLOOKUP(U107,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W107" t="s">
         <v>92</v>
       </c>
-      <c r="W107">
+      <c r="X107">
         <v>65</v>
       </c>
-      <c r="X107" t="s">
+      <c r="Y107" t="s">
         <v>53</v>
       </c>
-      <c r="Y107">
+      <c r="Z107">
         <v>2500</v>
       </c>
-      <c r="Z107" s="1">
+      <c r="AA107" s="1">
         <v>45707.475378506948</v>
       </c>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>26</v>
       </c>
@@ -9804,23 +10260,27 @@
       <c r="U108" t="s">
         <v>34</v>
       </c>
-      <c r="V108" t="s">
+      <c r="V108" s="2" t="str">
+        <f>VLOOKUP(U108,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W108" t="s">
         <v>218</v>
       </c>
-      <c r="W108">
+      <c r="X108">
         <v>7</v>
       </c>
-      <c r="X108" t="s">
+      <c r="Y108" t="s">
         <v>53</v>
       </c>
-      <c r="Y108">
+      <c r="Z108">
         <v>46457.53</v>
       </c>
-      <c r="Z108" s="1">
+      <c r="AA108" s="1">
         <v>45712.702018206015</v>
       </c>
     </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>26</v>
       </c>
@@ -9884,23 +10344,27 @@
       <c r="U109" t="s">
         <v>34</v>
       </c>
-      <c r="V109" t="s">
+      <c r="V109" s="2" t="str">
+        <f>VLOOKUP(U109,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W109" t="s">
         <v>218</v>
       </c>
-      <c r="W109">
+      <c r="X109">
         <v>7</v>
       </c>
-      <c r="X109" t="s">
+      <c r="Y109" t="s">
         <v>53</v>
       </c>
-      <c r="Y109">
+      <c r="Z109">
         <v>46457.53</v>
       </c>
-      <c r="Z109" s="1">
+      <c r="AA109" s="1">
         <v>45712.703188888889</v>
       </c>
     </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>26</v>
       </c>
@@ -9964,23 +10428,27 @@
       <c r="U110" t="s">
         <v>34</v>
       </c>
-      <c r="V110" t="s">
+      <c r="V110" s="2" t="str">
+        <f>VLOOKUP(U110,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W110" t="s">
         <v>221</v>
       </c>
-      <c r="W110">
+      <c r="X110">
         <v>31</v>
       </c>
-      <c r="X110" t="s">
+      <c r="Y110" t="s">
         <v>36</v>
       </c>
-      <c r="Y110">
+      <c r="Z110">
         <v>312</v>
       </c>
-      <c r="Z110" s="1">
+      <c r="AA110" s="1">
         <v>45707.443961111108</v>
       </c>
     </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>26</v>
       </c>
@@ -10044,23 +10512,27 @@
       <c r="U111" t="s">
         <v>34</v>
       </c>
-      <c r="V111" t="s">
+      <c r="V111" s="2" t="str">
+        <f>VLOOKUP(U111,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W111" t="s">
         <v>92</v>
       </c>
-      <c r="W111">
+      <c r="X111">
         <v>10</v>
       </c>
-      <c r="X111" t="s">
+      <c r="Y111" t="s">
         <v>64</v>
       </c>
-      <c r="Y111">
+      <c r="Z111">
         <v>2200</v>
       </c>
-      <c r="Z111" s="1">
+      <c r="AA111" s="1">
         <v>45716.397964699077</v>
       </c>
     </row>
-    <row r="112" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>26</v>
       </c>
@@ -10124,23 +10596,27 @@
       <c r="U112" t="s">
         <v>34</v>
       </c>
-      <c r="V112" t="s">
+      <c r="V112" s="2" t="str">
+        <f>VLOOKUP(U112,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W112" t="s">
         <v>92</v>
       </c>
-      <c r="W112">
+      <c r="X112">
         <v>65</v>
       </c>
-      <c r="X112" t="s">
+      <c r="Y112" t="s">
         <v>53</v>
       </c>
-      <c r="Y112">
+      <c r="Z112">
         <v>6000</v>
       </c>
-      <c r="Z112" s="1">
+      <c r="AA112" s="1">
         <v>45715.425985995367</v>
       </c>
     </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>26</v>
       </c>
@@ -10204,23 +10680,27 @@
       <c r="U113" t="s">
         <v>34</v>
       </c>
-      <c r="V113" t="s">
+      <c r="V113" s="2" t="str">
+        <f>VLOOKUP(U113,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W113" t="s">
         <v>92</v>
       </c>
-      <c r="W113">
+      <c r="X113">
         <v>7</v>
       </c>
-      <c r="X113" t="s">
+      <c r="Y113" t="s">
         <v>53</v>
       </c>
-      <c r="Y113">
+      <c r="Z113">
         <v>1800</v>
       </c>
-      <c r="Z113" s="1">
+      <c r="AA113" s="1">
         <v>45707.46554355324</v>
       </c>
     </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>26</v>
       </c>
@@ -10284,23 +10764,27 @@
       <c r="U114" t="s">
         <v>34</v>
       </c>
-      <c r="V114" t="s">
+      <c r="V114" s="2" t="str">
+        <f>VLOOKUP(U114,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W114" t="s">
         <v>92</v>
       </c>
-      <c r="W114">
+      <c r="X114">
         <v>65</v>
       </c>
-      <c r="X114" t="s">
+      <c r="Y114" t="s">
         <v>53</v>
       </c>
-      <c r="Y114">
+      <c r="Z114">
         <v>2400</v>
       </c>
-      <c r="Z114" s="1">
+      <c r="AA114" s="1">
         <v>45707.382853587966</v>
       </c>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>26</v>
       </c>
@@ -10364,23 +10848,27 @@
       <c r="U115" t="s">
         <v>34</v>
       </c>
-      <c r="V115" t="s">
+      <c r="V115" s="2" t="str">
+        <f>VLOOKUP(U115,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W115" t="s">
         <v>57</v>
       </c>
-      <c r="W115">
+      <c r="X115">
         <v>24</v>
       </c>
-      <c r="X115" t="s">
+      <c r="Y115" t="s">
         <v>36</v>
       </c>
-      <c r="Y115">
+      <c r="Z115">
         <v>1175</v>
       </c>
-      <c r="Z115" s="1">
+      <c r="AA115" s="1">
         <v>45707.467136342595</v>
       </c>
     </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>26</v>
       </c>
@@ -10444,23 +10932,27 @@
       <c r="U116" t="s">
         <v>34</v>
       </c>
-      <c r="V116" t="s">
+      <c r="V116" s="2" t="str">
+        <f>VLOOKUP(U116,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W116" t="s">
         <v>92</v>
       </c>
-      <c r="W116">
+      <c r="X116">
         <v>9</v>
       </c>
-      <c r="X116" t="s">
+      <c r="Y116" t="s">
         <v>53</v>
       </c>
-      <c r="Y116">
+      <c r="Z116">
         <v>3200</v>
       </c>
-      <c r="Z116" s="1">
+      <c r="AA116" s="1">
         <v>45709.502550960649</v>
       </c>
     </row>
-    <row r="117" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>26</v>
       </c>
@@ -10524,23 +11016,27 @@
       <c r="U117" t="s">
         <v>34</v>
       </c>
-      <c r="V117" t="s">
+      <c r="V117" s="2" t="str">
+        <f>VLOOKUP(U117,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W117" t="s">
         <v>92</v>
       </c>
-      <c r="W117">
+      <c r="X117">
         <v>9</v>
       </c>
-      <c r="X117" t="s">
+      <c r="Y117" t="s">
         <v>53</v>
       </c>
-      <c r="Y117">
+      <c r="Z117">
         <v>4500</v>
       </c>
-      <c r="Z117" s="1">
+      <c r="AA117" s="1">
         <v>45706.597614733793</v>
       </c>
     </row>
-    <row r="118" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>26</v>
       </c>
@@ -10604,23 +11100,27 @@
       <c r="U118" t="s">
         <v>34</v>
       </c>
-      <c r="V118" t="s">
+      <c r="V118" s="2" t="str">
+        <f>VLOOKUP(U118,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W118" t="s">
         <v>92</v>
       </c>
-      <c r="W118">
+      <c r="X118">
         <v>18</v>
       </c>
-      <c r="X118" t="s">
+      <c r="Y118" t="s">
         <v>238</v>
       </c>
-      <c r="Y118">
+      <c r="Z118">
         <v>2500</v>
       </c>
-      <c r="Z118" s="1">
+      <c r="AA118" s="1">
         <v>45707.471929976855</v>
       </c>
     </row>
-    <row r="119" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>26</v>
       </c>
@@ -10684,23 +11184,27 @@
       <c r="U119" t="s">
         <v>68</v>
       </c>
-      <c r="V119" t="s">
+      <c r="V119" s="2" t="str">
+        <f>VLOOKUP(U119,Hoja2!A$1:B$4,2,0)</f>
+        <v>18: CANON Y SOBRECANON, REGALIAS, RENTA DE ADUANAS Y PARTICIPACIONES</v>
+      </c>
+      <c r="W119" t="s">
         <v>89</v>
       </c>
-      <c r="W119">
+      <c r="X119">
         <v>49</v>
       </c>
-      <c r="X119" t="s">
+      <c r="Y119" t="s">
         <v>36</v>
       </c>
-      <c r="Y119">
+      <c r="Z119">
         <v>1152.81</v>
       </c>
-      <c r="Z119" s="1">
+      <c r="AA119" s="1">
         <v>45712.700295405091</v>
       </c>
     </row>
-    <row r="120" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>26</v>
       </c>
@@ -10764,23 +11268,27 @@
       <c r="U120" t="s">
         <v>34</v>
       </c>
-      <c r="V120" t="s">
+      <c r="V120" s="2" t="str">
+        <f>VLOOKUP(U120,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W120" t="s">
         <v>103</v>
       </c>
-      <c r="W120">
-        <v>32</v>
-      </c>
-      <c r="X120" t="s">
+      <c r="X120">
+        <v>32</v>
+      </c>
+      <c r="Y120" t="s">
         <v>36</v>
       </c>
-      <c r="Y120">
+      <c r="Z120">
         <v>2000</v>
       </c>
-      <c r="Z120" s="1">
+      <c r="AA120" s="1">
         <v>45709.500071759256</v>
       </c>
     </row>
-    <row r="121" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>26</v>
       </c>
@@ -10844,23 +11352,27 @@
       <c r="U121" t="s">
         <v>34</v>
       </c>
-      <c r="V121" t="s">
+      <c r="V121" s="2" t="str">
+        <f>VLOOKUP(U121,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W121" t="s">
         <v>247</v>
       </c>
-      <c r="W121">
+      <c r="X121">
         <v>20</v>
       </c>
-      <c r="X121" t="s">
+      <c r="Y121" t="s">
         <v>36</v>
       </c>
-      <c r="Y121">
+      <c r="Z121">
         <v>1800</v>
       </c>
-      <c r="Z121" s="1">
+      <c r="AA121" s="1">
         <v>45707.375472800923</v>
       </c>
     </row>
-    <row r="122" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>26</v>
       </c>
@@ -10924,23 +11436,27 @@
       <c r="U122" t="s">
         <v>34</v>
       </c>
-      <c r="V122" t="s">
+      <c r="V122" s="2" t="str">
+        <f>VLOOKUP(U122,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W122" t="s">
         <v>92</v>
       </c>
-      <c r="W122">
+      <c r="X122">
         <v>36</v>
       </c>
-      <c r="X122" t="s">
+      <c r="Y122" t="s">
         <v>36</v>
       </c>
-      <c r="Y122">
+      <c r="Z122">
         <v>3500</v>
       </c>
-      <c r="Z122" s="1">
+      <c r="AA122" s="1">
         <v>45707.379096724537</v>
       </c>
     </row>
-    <row r="123" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>26</v>
       </c>
@@ -11004,23 +11520,27 @@
       <c r="U123" t="s">
         <v>34</v>
       </c>
-      <c r="V123" t="s">
+      <c r="V123" s="2" t="str">
+        <f>VLOOKUP(U123,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W123" t="s">
         <v>92</v>
       </c>
-      <c r="W123">
+      <c r="X123">
         <v>9</v>
       </c>
-      <c r="X123" t="s">
+      <c r="Y123" t="s">
         <v>53</v>
       </c>
-      <c r="Y123">
+      <c r="Z123">
         <v>3800</v>
       </c>
-      <c r="Z123" s="1">
+      <c r="AA123" s="1">
         <v>45708.430624537039</v>
       </c>
     </row>
-    <row r="124" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>26</v>
       </c>
@@ -11084,23 +11604,27 @@
       <c r="U124" t="s">
         <v>34</v>
       </c>
-      <c r="V124" t="s">
+      <c r="V124" s="2" t="str">
+        <f>VLOOKUP(U124,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W124" t="s">
         <v>92</v>
       </c>
-      <c r="W124">
+      <c r="X124">
         <v>36</v>
       </c>
-      <c r="X124" t="s">
+      <c r="Y124" t="s">
         <v>36</v>
       </c>
-      <c r="Y124">
+      <c r="Z124">
         <v>3500</v>
       </c>
-      <c r="Z124" s="1">
+      <c r="AA124" s="1">
         <v>45712.707418981481</v>
       </c>
     </row>
-    <row r="125" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>26</v>
       </c>
@@ -11164,23 +11688,27 @@
       <c r="U125" t="s">
         <v>34</v>
       </c>
-      <c r="V125" t="s">
+      <c r="V125" s="2" t="str">
+        <f>VLOOKUP(U125,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W125" t="s">
         <v>92</v>
       </c>
-      <c r="W125">
+      <c r="X125">
         <v>36</v>
       </c>
-      <c r="X125" t="s">
+      <c r="Y125" t="s">
         <v>36</v>
       </c>
-      <c r="Y125">
+      <c r="Z125">
         <v>3500</v>
       </c>
-      <c r="Z125" s="1">
+      <c r="AA125" s="1">
         <v>45712.706201469904</v>
       </c>
     </row>
-    <row r="126" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>26</v>
       </c>
@@ -11244,23 +11772,27 @@
       <c r="U126" t="s">
         <v>34</v>
       </c>
-      <c r="V126" t="s">
+      <c r="V126" s="2" t="str">
+        <f>VLOOKUP(U126,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W126" t="s">
         <v>103</v>
       </c>
-      <c r="W126">
+      <c r="X126">
         <v>56</v>
       </c>
-      <c r="X126" t="s">
+      <c r="Y126" t="s">
         <v>53</v>
       </c>
-      <c r="Y126">
+      <c r="Z126">
         <v>2222.2199999999998</v>
       </c>
-      <c r="Z126" s="1">
+      <c r="AA126" s="1">
         <v>45715.535773344905</v>
       </c>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>26</v>
       </c>
@@ -11324,23 +11856,27 @@
       <c r="U127" t="s">
         <v>34</v>
       </c>
-      <c r="V127" t="s">
+      <c r="V127" s="2" t="str">
+        <f>VLOOKUP(U127,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W127" t="s">
         <v>92</v>
       </c>
-      <c r="W127">
+      <c r="X127">
         <v>7</v>
       </c>
-      <c r="X127" t="s">
+      <c r="Y127" t="s">
         <v>53</v>
       </c>
-      <c r="Y127">
+      <c r="Z127">
         <v>1500</v>
       </c>
-      <c r="Z127" s="1">
+      <c r="AA127" s="1">
         <v>45712.71153429398</v>
       </c>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>26</v>
       </c>
@@ -11404,23 +11940,27 @@
       <c r="U128" t="s">
         <v>34</v>
       </c>
-      <c r="V128" t="s">
+      <c r="V128" s="2" t="str">
+        <f>VLOOKUP(U128,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W128" t="s">
         <v>92</v>
       </c>
-      <c r="W128">
+      <c r="X128">
         <v>21</v>
       </c>
-      <c r="X128" t="s">
+      <c r="Y128" t="s">
         <v>36</v>
       </c>
-      <c r="Y128">
+      <c r="Z128">
         <v>2450</v>
       </c>
-      <c r="Z128" s="1">
+      <c r="AA128" s="1">
         <v>45709.608564201386</v>
       </c>
     </row>
-    <row r="129" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>26</v>
       </c>
@@ -11484,23 +12024,27 @@
       <c r="U129" t="s">
         <v>34</v>
       </c>
-      <c r="V129" t="s">
+      <c r="V129" s="2" t="str">
+        <f>VLOOKUP(U129,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W129" t="s">
         <v>92</v>
       </c>
-      <c r="W129">
+      <c r="X129">
         <v>65</v>
       </c>
-      <c r="X129" t="s">
+      <c r="Y129" t="s">
         <v>53</v>
       </c>
-      <c r="Y129">
+      <c r="Z129">
         <v>1500</v>
       </c>
-      <c r="Z129" s="1">
+      <c r="AA129" s="1">
         <v>45709.605947534721</v>
       </c>
     </row>
-    <row r="130" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>26</v>
       </c>
@@ -11564,23 +12108,27 @@
       <c r="U130" t="s">
         <v>34</v>
       </c>
-      <c r="V130" t="s">
+      <c r="V130" s="2" t="str">
+        <f>VLOOKUP(U130,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W130" t="s">
         <v>103</v>
       </c>
-      <c r="W130">
+      <c r="X130">
         <v>20</v>
       </c>
-      <c r="X130" t="s">
+      <c r="Y130" t="s">
         <v>36</v>
       </c>
-      <c r="Y130">
+      <c r="Z130">
         <v>2800</v>
       </c>
-      <c r="Z130" s="1">
+      <c r="AA130" s="1">
         <v>45708.427169016206</v>
       </c>
     </row>
-    <row r="131" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>26</v>
       </c>
@@ -11644,23 +12192,27 @@
       <c r="U131" t="s">
         <v>68</v>
       </c>
-      <c r="V131" t="s">
+      <c r="V131" s="2" t="str">
+        <f>VLOOKUP(U131,Hoja2!A$1:B$4,2,0)</f>
+        <v>18: CANON Y SOBRECANON, REGALIAS, RENTA DE ADUANAS Y PARTICIPACIONES</v>
+      </c>
+      <c r="W131" t="s">
         <v>57</v>
       </c>
-      <c r="W131">
+      <c r="X131">
         <v>49</v>
       </c>
-      <c r="X131" t="s">
+      <c r="Y131" t="s">
         <v>36</v>
       </c>
-      <c r="Y131">
+      <c r="Z131">
         <v>1560</v>
       </c>
-      <c r="Z131" s="1">
+      <c r="AA131" s="1">
         <v>45709.612314004633</v>
       </c>
     </row>
-    <row r="132" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>26</v>
       </c>
@@ -11724,23 +12276,27 @@
       <c r="U132" t="s">
         <v>34</v>
       </c>
-      <c r="V132" t="s">
+      <c r="V132" s="2" t="str">
+        <f>VLOOKUP(U132,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W132" t="s">
         <v>57</v>
       </c>
-      <c r="W132">
+      <c r="X132">
         <v>24</v>
       </c>
-      <c r="X132" t="s">
+      <c r="Y132" t="s">
         <v>36</v>
       </c>
-      <c r="Y132">
+      <c r="Z132">
         <v>1200</v>
       </c>
-      <c r="Z132" s="1">
+      <c r="AA132" s="1">
         <v>45715.429412349535</v>
       </c>
     </row>
-    <row r="133" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>26</v>
       </c>
@@ -11804,23 +12360,27 @@
       <c r="U133" t="s">
         <v>34</v>
       </c>
-      <c r="V133" t="s">
+      <c r="V133" s="2" t="str">
+        <f>VLOOKUP(U133,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W133" t="s">
         <v>57</v>
       </c>
-      <c r="W133">
+      <c r="X133">
         <v>25</v>
       </c>
-      <c r="X133" t="s">
+      <c r="Y133" t="s">
         <v>36</v>
       </c>
-      <c r="Y133">
+      <c r="Z133">
         <v>1350</v>
       </c>
-      <c r="Z133" s="1">
+      <c r="AA133" s="1">
         <v>45715.42851597222</v>
       </c>
     </row>
-    <row r="134" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>26</v>
       </c>
@@ -11884,23 +12444,27 @@
       <c r="U134" t="s">
         <v>34</v>
       </c>
-      <c r="V134" t="s">
+      <c r="V134" s="2" t="str">
+        <f>VLOOKUP(U134,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W134" t="s">
         <v>103</v>
       </c>
-      <c r="W134">
+      <c r="X134">
         <v>31</v>
       </c>
-      <c r="X134" t="s">
+      <c r="Y134" t="s">
         <v>36</v>
       </c>
-      <c r="Y134">
+      <c r="Z134">
         <v>3000</v>
       </c>
-      <c r="Z134" s="1">
+      <c r="AA134" s="1">
         <v>45719.536064201391</v>
       </c>
     </row>
-    <row r="135" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>26</v>
       </c>
@@ -11964,23 +12528,27 @@
       <c r="U135" t="s">
         <v>34</v>
       </c>
-      <c r="V135" t="s">
+      <c r="V135" s="2" t="str">
+        <f>VLOOKUP(U135,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W135" t="s">
         <v>92</v>
       </c>
-      <c r="W135">
+      <c r="X135">
         <v>9</v>
       </c>
-      <c r="X135" t="s">
+      <c r="Y135" t="s">
         <v>53</v>
       </c>
-      <c r="Y135">
+      <c r="Z135">
         <v>5000</v>
       </c>
-      <c r="Z135" s="1">
+      <c r="AA135" s="1">
         <v>45716.398728009262</v>
       </c>
     </row>
-    <row r="136" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>26</v>
       </c>
@@ -12044,20 +12612,74 @@
       <c r="U136" t="s">
         <v>34</v>
       </c>
-      <c r="V136" t="s">
+      <c r="V136" s="2" t="str">
+        <f>VLOOKUP(U136,Hoja2!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W136" t="s">
         <v>273</v>
       </c>
-      <c r="W136">
+      <c r="X136">
         <v>56</v>
       </c>
-      <c r="X136" t="s">
+      <c r="Y136" t="s">
         <v>53</v>
       </c>
-      <c r="Y136">
+      <c r="Z136">
         <v>122264.72</v>
       </c>
-      <c r="Z136" s="1">
+      <c r="AA136" s="1">
         <v>45716.697349849535</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6221D2DB-799F-4324-BBD2-ADABBC53D541}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="46.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agrego la data de siaf
</commit_message>
<xml_diff>
--- a/data/ep_mes_2025.xlsx
+++ b/data/ep_mes_2025.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6. Código\seguimiento_presupuestal_unsch_streamlit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C9F058-CBC5-4F9E-9AD5-1F3FB44433A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592FABA8-7EAD-472B-B910-5F6413374F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="fuente_financiamiento" sheetId="2" r:id="rId2"/>
-    <sheet name="clasificador" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja2" sheetId="4" r:id="rId2"/>
+    <sheet name="fuente_financiamiento" sheetId="2" r:id="rId3"/>
+    <sheet name="clasificador" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$AB$136</definedName>
@@ -25,12 +26,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4819" uniqueCount="3532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5209" uniqueCount="3567">
   <si>
     <t>ano_eje</t>
   </si>
@@ -10626,13 +10636,118 @@
   </si>
   <si>
     <t>2.8. 3  2. 3 99: OTROS CREDITOS INTERNOS</t>
+  </si>
+  <si>
+    <t>OFICINA DE COOPERACIÓN Y RELACIONES INTERINSTITUCIONALES</t>
+  </si>
+  <si>
+    <t>94.02.18.04</t>
+  </si>
+  <si>
+    <t>ESCUELA PROFESIONAL DE ENFERMERÍA</t>
+  </si>
+  <si>
+    <t>EJECUCION DEL PAGO DE MULTA INTERPUESTA POR LA SUNAFIL</t>
+  </si>
+  <si>
+    <t>SUBVENCION ECONOMICA PARA ESTUDIANTES DEL PROGRAMA DE MOVILIDAD ACADEMICA ESTUDIANTIL</t>
+  </si>
+  <si>
+    <t>REALIZACION DE PRACTICAS PRE PROFESIONALES (EP. ENFERMERIA)</t>
+  </si>
+  <si>
+    <t>MEJORAMIENTO SERVICIO DE FORMACION PROFESIONAL E INVESTIGACION DE LA BIODIVERSIDAD Y EL ECOSISTEMA EN LA FACULTAD DE CIENCIAS BIOLOGICAS DE LA UNSCH</t>
+  </si>
+  <si>
+    <t>ASIGNACIÓN EXTRAORDINARIA POR MOVILIDAD AL PERSONAL ADMINISTRATIVO</t>
+  </si>
+  <si>
+    <t>IMPLEMENTACION Y DESARROLLO DE ACTIVIDADES ADMINISTRATIVAS DE PLANIFICACION</t>
+  </si>
+  <si>
+    <t>REALIZACIÓN DE LA TRANSFERENCIA A LA CONTRALORIA GENERAL DE LA REPÚBLICA PARA ACCIONES DE CONTROL</t>
+  </si>
+  <si>
+    <t>ADEUDO CONTRAIDO POR MULTA IMPUESTA POR LA SUNAFIL, CONFORMEA LO ESTABLECIDO EN LA RESOLUCION DE SUB INTENDENCIA DE SAN CION N° 238-2023-SUNAFIL/IRE CUSCO-SISA, DE FECHA 31 DE MARZO DE 2023, NTD 2475599</t>
+  </si>
+  <si>
+    <t>PLANILLA DE PAGOS N° 001-25/234, CORRESPONDIENTE AL PAGO DE SUBVENCIONES ECONOMICA- PROGRAMA DE MOVILIDAD ESTUDIANTIL ENLA UNIVERSIDAD MICHOACANA DE SAN NICOLAS DE HIDALGO DE MEXI CO, ENERO 2025</t>
+  </si>
+  <si>
+    <t>POR EL PAGO DE LA OBLIGACIÓN DE DECLARACION JURADA ANUAL, IMPUESTO PREDIAL Y ARBITRIOS MUNICIPALES CORRESPONDIENTE AL EJERCICIO 2025</t>
+  </si>
+  <si>
+    <t>HRP NRO 027-028; PAGOS SALARIALES AL COMPONENTE I PISTAS Y VEREDAS DEL PROYECTO: MEJORAMIENTO DEL SERVICIO DE GESTION INTITUCIONAL EN EDUCACION SUPERIOR UNIVERSITARIA EN SERVICIOS BASICOS Y URBANISTICOS DE LA UNSCH. SEGUN MEMO 806 -25-UNSCH-DIGA</t>
+  </si>
+  <si>
+    <t>HRP NRO 064-065; PAGOS SALARIALES AL COMPONENTE I PISTAS Y VEREDAS DEL PROYECTO: MEJORAMIENTO DEL SERVICIO DE GESTION INTITUCIONAL EN EDUCACION SUPERIOR UNIVERSITARIA EN SERVICIOS BASICOS Y URBANISTICOS DE LA UNSCH. SEGUN MEMO 1572 -25-UNSCH-DIGA</t>
+  </si>
+  <si>
+    <t>PLANILLA DE PAGOS N° 002-25/234, A PARTIR DEL 06/01 AL 06/03/2025 EN LA CIUDAD DE LIMA. NTD 254341 CORRESPONDIENTE AL PAGO DE AYUDA ECONOMICA A LOS ALUMNOS MATRICULADOS EN LA ASIGNATURA PP-442 PRACTICAS PRE-PROFESIONALES-I DE LA E.P. DE ENFERMERIA</t>
+  </si>
+  <si>
+    <t>HRP NRO 025-026; PAGOS SALARIALES A OBREROS DE LA OBRA MEJORAMIENTO SERVICIO DE FORMACION PROFESIONAL E INVESTIGACION DELA BIODIVERSIDAD Y EL ECOSISTEMA EN LA FACULTAD DE CIENCIAS BIOLOGICAS DE LA UNSCH AYACUCHO</t>
+  </si>
+  <si>
+    <t>H/R/P 054-055, REINTEGRO DE SALARIOS Y BENEFICIOS LABORALES DEL PERSONAL OBRERO CORRESPONDIENTE AL MES DE SETIEMBRE DEL 2024 DE LA OBRA MEJORAMIENTO SERVICIO DE FORMACION PROFESIONAL E INVESTIGACION DE LA BIODIVERSIDAD Y EL ECOSISTEMA EN LAFACULTAD</t>
+  </si>
+  <si>
+    <t>H/R/P 056-057, REINTEGRO DE SALARIOS Y BENEFICIOS LABORALES DEL PERSONAL OBRERO CORRESPONDIENTE AL MES DE OCTUBRE DEL 2024 DE LA OBRA MEJORAMIENTO SERVICIO DE FORMACION PROFESIONALE INVESTIGACION DE LA BIODIVERSIDAD EN LA FACULTAD DE BIOLO GIA</t>
+  </si>
+  <si>
+    <t>H/R/P 058-059, RECALCULO Y REINTEGRO DE SALARIOS Y BENEFICIOS LABORALES DEL PERSONAL OBRERO CORRESPONDIENTE AL MES DE OCTUBRE DEL 2024 DE LA OBRA MEJORAMIENTO SERVICIO DE FORMACIONPROFESIONAL E INVESTIGACION DE LA BIODIVERSIDAD EN LA FACUL TAD DE BIO</t>
+  </si>
+  <si>
+    <t>H/R/P 060-061, REINTEGRO DE SALARIOS Y BENEFICIOS LABORALES DEL PERSONAL OBRERO CORRESPONDIENTE AL MES DE NOVIEMBRE DEL 2024 DE LA OBRA MEJORAMIENTO SERVICIO DE FORMACION PROFESIONAL E INVESTIGACION DE LA BIODIVERSIDAD EN LA FACULTAD DE BIOLOGIA</t>
+  </si>
+  <si>
+    <t>H/R/P 062-063, REINTEGRO DE SALARIOS Y BENEFICIOS LABORALES DEL PERSONAL OBRERO CORRESPONDIENTE AL MES DE DICIEMBRE DEL 2024 DE LA OBRA MEJORAMIENTO SERVICIO DE FORMACION PROFESIONAL E INVESTIGACION DE LA BIODIVERSIDAD EN LA FACULTAD DE BIOLOGIA</t>
+  </si>
+  <si>
+    <t>HRP NRO 070-071; PAGOS SALARIALES A LA OBRA MEJORAMIENTO SERVICIO DE FORMACION PROFESIONAL E INVESTIGACION DE LA BIODIVERSIDAD Y EL ECOSISTEMA EN LA FACULTAD DE CIENCIAS BIOLOGICASDE LA UNSCH AYACUCHO EN FEBRERO 2025</t>
+  </si>
+  <si>
+    <t>H/R/P 072-073. SALARIOS AL PERSONAL TECNICO ADMINISTRATIVO DE LA OBRA MEJORAMIENTO SERVICIO DE FORMACION PROFESIONAL E INVESTIGACION DE LA BIODIVERSIDAD Y EL ECOSISTEMA EN LA FACULTAD DE CIENCIAS BIOLOGICAS DE LA UNSCH AYACUCHO EN FEBRERO 2025</t>
+  </si>
+  <si>
+    <t>PAGO DE INTERESES Y COSTAS GENERADAS POR ADEUDO CONTRAIDO POR MULTA IMPUESTA POR LA SUNAFIL, CONFORME A LO ESTABLECIDO EN LA RESOLUCION DE SUB INTENDENCIA DE SANCION N° 238-2023-SUNAFIL/IRE CUSCO-SISA, DE FECHA 31 DE MARZO DE 2023, NTD 253159</t>
+  </si>
+  <si>
+    <t>HRP 029-030 : ASIGNACION EXTRAORDINARIA POR MOVILIDAD MAS INCREMENTO EN MARCO DE LA CLAUSULA CUARTA DEL CONVENIO COLECTIVO 2025 - UNSCH. ENERO 2025</t>
+  </si>
+  <si>
+    <t>HRP 052 - 053 : CUMPLIMIENTO DE LA RESOLUCION RECTORAL N° 092-2025-UNSCH-R y la RD. 074-2025-DIGA/UNSCH , ASIGNACION EXTRAORDINARIA POR MOVILIDAD PARA EL PERSONAL DEL DL 276. FEBRERO 2025</t>
+  </si>
+  <si>
+    <t>RECONOCER Y AUTORIZAR EL REEMBOLSO DE GASTOS POR CONCEPTO DEPASAJE A LA CIUDAD DE LIMA A FAVOR DE ENVER BORDA ALVIZURI NTD 2500212 A FIN DE PARTICIPAR EN EL TALLER PARA EL FORTAL ECIMIENTO DE LA GESTION DE LAS UNIVERSIDADES PUBLICAS DESARROLLA</t>
+  </si>
+  <si>
+    <t>POR LA TRANSFERENCIA FINANCIERA A FAVOR DE LA CONTRALORIA GENERAL DE LA REPUBLICA, PARA LA DESIGNACIÓN DE LA SOCIEDAD AUDITORA, AUDITORIA FINANCIERA 2024</t>
+  </si>
+  <si>
+    <t>POR EL PAGO DE LA OBLIGACIÓN POR EL CONCEPTO DE ARBITRIOS MUNICIPALES DEL EJERCICIO 2025, DE LOS INMUEBLES DE LA UNIVERSIDAD NACIONAL DE SAN CRISTOBAL DE HUAMANGA, UBICADOS EN EL DISTRITO DE ANDRES AVELINO CACERES DORREGARAY NTD 2500542</t>
+  </si>
+  <si>
+    <t>PLANILLA DE PAGOS N° 003-25/234, CORRESPONDIENTE AL PAGO DE SUBVENCIONES ECONOMICA- PROGRAMA DE MOVILIDAD ESTUDIANTIL ENLA PONTIFICIA UNIVERSIDAD DE VALPARAISO DE CHILE, FEBRERO 2 025</t>
+  </si>
+  <si>
+    <t>HRP NRO 068-069; PAGOS SALARIALES AL COMPONENTE II ADECUADO TRATAMIENTO DE AREAS VERDES DEL PROYECTO: MEJORAMIENTO DEL SERVICIO DE GESTION INTITUCIONAL EN EDUCACION SUPERIOR UNIVERSITARIA EN SERVICIOS BASICOS Y URBANISTICOS -UNSCH. MEMO 1613-25-DIGA</t>
+  </si>
+  <si>
+    <t>HRP NRO 066-067; PAGOS SALARIALES AL COMPONENTE IV CERCO PERIMETRICO DEL PROYECTO: MEJORAMIENTO DEL SERVICIO DE GESTION INTITUCIONAL EN EDUCACION SUPERIOR UNIVERSITARIA EN SERVICIOS BASICOS Y URBANISTICOS DE LA UNSCH. SEGUN MEMO 1575 -25-UNSCH-DIGA</t>
+  </si>
+  <si>
+    <t>3000785</t>
+  </si>
+  <si>
+    <t>2402381</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10640,13 +10755,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -10661,9 +10788,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10944,23 +11074,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB136"/>
+  <dimension ref="A1:AB175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="G129" sqref="G129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="29.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="58.7109375" customWidth="1"/>
     <col min="10" max="10" width="19.85546875" customWidth="1"/>
     <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="15" max="15" width="43.85546875" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
+    <col min="17" max="17" width="23.7109375" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" customWidth="1"/>
     <col min="20" max="20" width="15.28515625" customWidth="1"/>
     <col min="21" max="21" width="16.28515625" customWidth="1"/>
     <col min="22" max="22" width="23.7109375" customWidth="1"/>
     <col min="23" max="23" width="14" customWidth="1"/>
     <col min="24" max="24" width="19.7109375" customWidth="1"/>
-    <col min="28" max="28" width="19" customWidth="1"/>
+    <col min="28" max="28" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -22929,18 +23065,2865 @@
         <v>45716.697349849535</v>
       </c>
     </row>
+    <row r="137" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B137" s="3">
+        <v>9</v>
+      </c>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E137" s="3"/>
+      <c r="F137" s="3"/>
+      <c r="G137" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H137" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I137" s="3"/>
+      <c r="J137" s="3" t="s">
+        <v>3535</v>
+      </c>
+      <c r="K137" s="3"/>
+      <c r="L137" s="3"/>
+      <c r="M137" s="3"/>
+      <c r="N137" s="3"/>
+      <c r="O137" s="3" t="s">
+        <v>3542</v>
+      </c>
+      <c r="P137" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q137" s="3"/>
+      <c r="R137" s="3"/>
+      <c r="S137" s="3"/>
+      <c r="T137" s="3">
+        <v>0</v>
+      </c>
+      <c r="U137" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V137" s="3" t="str">
+        <f>VLOOKUP(U137,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W137" s="3" t="s">
+        <v>2679</v>
+      </c>
+      <c r="X137" s="3" t="str">
+        <f>VLOOKUP(W137,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.5. 4  1. 3  1: MULTAS</v>
+      </c>
+      <c r="Y137" s="3">
+        <v>31</v>
+      </c>
+      <c r="Z137" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA137" s="3">
+        <v>53479.77</v>
+      </c>
+      <c r="AB137" s="4">
+        <v>45671.69734953704</v>
+      </c>
+    </row>
+    <row r="138" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B138" s="3">
+        <v>83</v>
+      </c>
+      <c r="C138" s="3"/>
+      <c r="D138" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E138" s="3"/>
+      <c r="F138" s="3"/>
+      <c r="G138" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H138" s="3" t="s">
+        <v>3532</v>
+      </c>
+      <c r="I138" s="3"/>
+      <c r="J138" s="3" t="s">
+        <v>3536</v>
+      </c>
+      <c r="K138" s="3"/>
+      <c r="L138" s="3"/>
+      <c r="M138" s="3"/>
+      <c r="N138" s="3"/>
+      <c r="O138" s="3" t="s">
+        <v>3543</v>
+      </c>
+      <c r="P138" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q138" s="3"/>
+      <c r="R138" s="3"/>
+      <c r="S138" s="3"/>
+      <c r="T138" s="3">
+        <v>0</v>
+      </c>
+      <c r="U138" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V138" s="3" t="str">
+        <f>VLOOKUP(U138,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W138" s="3" t="s">
+        <v>2657</v>
+      </c>
+      <c r="X138" s="3" t="str">
+        <f>VLOOKUP(W138,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.5. 3  1. 1  1: A ESTUDIANTES</v>
+      </c>
+      <c r="Y138" s="3">
+        <v>57</v>
+      </c>
+      <c r="Z138" s="3" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA138" s="3">
+        <v>40000</v>
+      </c>
+      <c r="AB138" s="4">
+        <v>45681.69734953704</v>
+      </c>
+    </row>
+    <row r="139" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B139" s="3">
+        <v>119</v>
+      </c>
+      <c r="C139" s="3"/>
+      <c r="D139" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E139" s="3"/>
+      <c r="F139" s="3"/>
+      <c r="G139" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H139" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I139" s="3"/>
+      <c r="J139" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K139" s="3"/>
+      <c r="L139" s="3"/>
+      <c r="M139" s="3"/>
+      <c r="N139" s="3"/>
+      <c r="O139" s="3" t="s">
+        <v>3544</v>
+      </c>
+      <c r="P139" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q139" s="3"/>
+      <c r="R139" s="3"/>
+      <c r="S139" s="3"/>
+      <c r="T139" s="3">
+        <v>0</v>
+      </c>
+      <c r="U139" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V139" s="3" t="str">
+        <f>VLOOKUP(U139,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W139" s="3" t="s">
+        <v>2695</v>
+      </c>
+      <c r="X139" s="3" t="str">
+        <f>VLOOKUP(W139,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.5. 4  3. 1  1: IMPUESTOS</v>
+      </c>
+      <c r="Y139" s="3">
+        <v>31</v>
+      </c>
+      <c r="Z139" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA139" s="3">
+        <v>44.7</v>
+      </c>
+      <c r="AB139" s="4">
+        <v>45687.69734953704</v>
+      </c>
+    </row>
+    <row r="140" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B140" s="3">
+        <v>119</v>
+      </c>
+      <c r="C140" s="3"/>
+      <c r="D140" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E140" s="3"/>
+      <c r="F140" s="3"/>
+      <c r="G140" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H140" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I140" s="3">
+        <v>284</v>
+      </c>
+      <c r="J140" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K140" s="3"/>
+      <c r="L140" s="3"/>
+      <c r="M140" s="3"/>
+      <c r="N140" s="3"/>
+      <c r="O140" s="3" t="s">
+        <v>3544</v>
+      </c>
+      <c r="P140" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q140" s="3"/>
+      <c r="R140" s="3"/>
+      <c r="S140" s="3"/>
+      <c r="T140" s="3">
+        <v>0</v>
+      </c>
+      <c r="U140" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V140" s="3" t="str">
+        <f>VLOOKUP(U140,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W140" s="3" t="s">
+        <v>2699</v>
+      </c>
+      <c r="X140" s="3" t="str">
+        <f>VLOOKUP(W140,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.5. 4  3. 2  1: DERECHOS ADMINISTRATIVOS</v>
+      </c>
+      <c r="Y140" s="3">
+        <v>31</v>
+      </c>
+      <c r="Z140" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA140" s="3">
+        <v>67836.240000000005</v>
+      </c>
+      <c r="AB140" s="4">
+        <v>45687.69734953704</v>
+      </c>
+    </row>
+    <row r="141" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A141" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B141" s="3">
+        <v>246</v>
+      </c>
+      <c r="C141" s="3"/>
+      <c r="D141" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E141" s="3"/>
+      <c r="F141" s="3"/>
+      <c r="G141" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H141" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I141" s="3">
+        <v>368</v>
+      </c>
+      <c r="J141" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K141" s="3"/>
+      <c r="L141" s="3"/>
+      <c r="M141" s="3"/>
+      <c r="N141" s="3"/>
+      <c r="O141" s="3" t="s">
+        <v>3545</v>
+      </c>
+      <c r="P141" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q141" s="3"/>
+      <c r="R141" s="3"/>
+      <c r="S141" s="3"/>
+      <c r="T141" s="3">
+        <v>0</v>
+      </c>
+      <c r="U141" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V141" s="3" t="str">
+        <f>VLOOKUP(U141,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W141" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X141" s="3" t="str">
+        <f>VLOOKUP(W141,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y141" s="3">
+        <v>64</v>
+      </c>
+      <c r="Z141" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA141" s="3">
+        <v>29164.32</v>
+      </c>
+      <c r="AB141" s="4">
+        <v>45694.69734953704</v>
+      </c>
+    </row>
+    <row r="142" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A142" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B142" s="3">
+        <v>246</v>
+      </c>
+      <c r="C142" s="3"/>
+      <c r="D142" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E142" s="3"/>
+      <c r="F142" s="3"/>
+      <c r="G142" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I142" s="3">
+        <v>368</v>
+      </c>
+      <c r="J142" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K142" s="3"/>
+      <c r="L142" s="3"/>
+      <c r="M142" s="3"/>
+      <c r="N142" s="3"/>
+      <c r="O142" s="3" t="s">
+        <v>3545</v>
+      </c>
+      <c r="P142" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q142" s="3"/>
+      <c r="R142" s="3"/>
+      <c r="S142" s="3"/>
+      <c r="T142" s="3">
+        <v>0</v>
+      </c>
+      <c r="U142" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V142" s="3" t="str">
+        <f>VLOOKUP(U142,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W142" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X142" s="3" t="str">
+        <f>VLOOKUP(W142,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y142" s="3">
+        <v>64</v>
+      </c>
+      <c r="Z142" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA142" s="3">
+        <v>7763.28</v>
+      </c>
+      <c r="AB142" s="4">
+        <v>45694.69734953704</v>
+      </c>
+    </row>
+    <row r="143" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B143" s="3">
+        <v>554</v>
+      </c>
+      <c r="C143" s="3"/>
+      <c r="D143" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E143" s="3"/>
+      <c r="F143" s="3"/>
+      <c r="G143" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H143" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I143" s="3">
+        <v>368</v>
+      </c>
+      <c r="J143" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K143" s="3"/>
+      <c r="L143" s="3"/>
+      <c r="M143" s="3"/>
+      <c r="N143" s="3"/>
+      <c r="O143" s="3" t="s">
+        <v>3546</v>
+      </c>
+      <c r="P143" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q143" s="3"/>
+      <c r="R143" s="3"/>
+      <c r="S143" s="3"/>
+      <c r="T143" s="3">
+        <v>0</v>
+      </c>
+      <c r="U143" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V143" s="3" t="str">
+        <f>VLOOKUP(U143,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W143" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X143" s="3" t="str">
+        <f>VLOOKUP(W143,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y143" s="3">
+        <v>64</v>
+      </c>
+      <c r="Z143" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA143" s="3">
+        <v>131434.19</v>
+      </c>
+      <c r="AB143" s="4">
+        <v>45716.697349849535</v>
+      </c>
+    </row>
+    <row r="144" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A144" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B144" s="3">
+        <v>554</v>
+      </c>
+      <c r="C144" s="3"/>
+      <c r="D144" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E144" s="3"/>
+      <c r="F144" s="3"/>
+      <c r="G144" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H144" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I144" s="3">
+        <v>368</v>
+      </c>
+      <c r="J144" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K144" s="3"/>
+      <c r="L144" s="3"/>
+      <c r="M144" s="3"/>
+      <c r="N144" s="3"/>
+      <c r="O144" s="3" t="s">
+        <v>3546</v>
+      </c>
+      <c r="P144" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q144" s="3"/>
+      <c r="R144" s="3"/>
+      <c r="S144" s="3"/>
+      <c r="T144" s="3">
+        <v>0</v>
+      </c>
+      <c r="U144" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V144" s="3" t="str">
+        <f>VLOOKUP(U144,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W144" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X144" s="3" t="str">
+        <f>VLOOKUP(W144,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y144" s="3">
+        <v>64</v>
+      </c>
+      <c r="Z144" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA144" s="3">
+        <v>30652.27</v>
+      </c>
+      <c r="AB144" s="4">
+        <v>45716.697349849535</v>
+      </c>
+    </row>
+    <row r="145" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B145" s="3">
+        <v>210</v>
+      </c>
+      <c r="C145" s="3"/>
+      <c r="D145" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E145" s="3"/>
+      <c r="F145" s="3"/>
+      <c r="G145" s="3" t="s">
+        <v>3533</v>
+      </c>
+      <c r="H145" s="3" t="s">
+        <v>3534</v>
+      </c>
+      <c r="I145" s="3"/>
+      <c r="J145" s="3" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K145" s="3"/>
+      <c r="L145" s="3"/>
+      <c r="M145" s="3"/>
+      <c r="N145" s="3"/>
+      <c r="O145" s="3" t="s">
+        <v>3547</v>
+      </c>
+      <c r="P145" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q145" s="3"/>
+      <c r="R145" s="3"/>
+      <c r="S145" s="3"/>
+      <c r="T145" s="3">
+        <v>9</v>
+      </c>
+      <c r="U145" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="V145" s="3" t="str">
+        <f>VLOOKUP(U145,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">09: RECURSOS DIRECTAMENTE RECAUDADOS                                                                                                                      </v>
+      </c>
+      <c r="W145" s="3" t="s">
+        <v>2657</v>
+      </c>
+      <c r="X145" s="3" t="str">
+        <f>VLOOKUP(W145,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.5. 3  1. 1  1: A ESTUDIANTES</v>
+      </c>
+      <c r="Y145" s="3">
+        <v>67</v>
+      </c>
+      <c r="Z145" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA145" s="3">
+        <v>38940</v>
+      </c>
+      <c r="AB145" s="4">
+        <v>45698.69734953704</v>
+      </c>
+    </row>
+    <row r="146" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B146" s="3">
+        <v>233</v>
+      </c>
+      <c r="C146" s="3"/>
+      <c r="D146" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E146" s="3"/>
+      <c r="F146" s="3"/>
+      <c r="G146" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H146" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I146" s="3">
+        <v>362</v>
+      </c>
+      <c r="J146" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K146" s="3"/>
+      <c r="L146" s="3"/>
+      <c r="M146" s="3"/>
+      <c r="N146" s="3"/>
+      <c r="O146" s="3" t="s">
+        <v>3548</v>
+      </c>
+      <c r="P146" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q146" s="3"/>
+      <c r="R146" s="3"/>
+      <c r="S146" s="3"/>
+      <c r="T146" s="3">
+        <v>0</v>
+      </c>
+      <c r="U146" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V146" s="3" t="str">
+        <f>VLOOKUP(U146,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W146" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X146" s="3" t="str">
+        <f>VLOOKUP(W146,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y146" s="3">
+        <v>63</v>
+      </c>
+      <c r="Z146" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="AA146" s="3">
+        <v>54892.11</v>
+      </c>
+      <c r="AB146" s="4">
+        <v>45699.69734953704</v>
+      </c>
+    </row>
+    <row r="147" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A147" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B147" s="3">
+        <v>233</v>
+      </c>
+      <c r="C147" s="3"/>
+      <c r="D147" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E147" s="3"/>
+      <c r="F147" s="3"/>
+      <c r="G147" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H147" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I147" s="3">
+        <v>362</v>
+      </c>
+      <c r="J147" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K147" s="3"/>
+      <c r="L147" s="3"/>
+      <c r="M147" s="3"/>
+      <c r="N147" s="3"/>
+      <c r="O147" s="3" t="s">
+        <v>3548</v>
+      </c>
+      <c r="P147" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q147" s="3"/>
+      <c r="R147" s="3"/>
+      <c r="S147" s="3"/>
+      <c r="T147" s="3">
+        <v>0</v>
+      </c>
+      <c r="U147" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V147" s="3" t="str">
+        <f>VLOOKUP(U147,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W147" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X147" s="3" t="str">
+        <f>VLOOKUP(W147,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y147" s="3">
+        <v>63</v>
+      </c>
+      <c r="Z147" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="AA147" s="3">
+        <v>12871.08</v>
+      </c>
+      <c r="AB147" s="4">
+        <v>45699.69734953704</v>
+      </c>
+    </row>
+    <row r="148" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A148" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B148" s="3">
+        <v>522</v>
+      </c>
+      <c r="C148" s="3"/>
+      <c r="D148" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E148" s="3"/>
+      <c r="F148" s="3"/>
+      <c r="G148" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H148" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I148" s="3">
+        <v>362</v>
+      </c>
+      <c r="J148" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K148" s="3"/>
+      <c r="L148" s="3"/>
+      <c r="M148" s="3"/>
+      <c r="N148" s="3"/>
+      <c r="O148" s="3" t="s">
+        <v>3549</v>
+      </c>
+      <c r="P148" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q148" s="3"/>
+      <c r="R148" s="3"/>
+      <c r="S148" s="3"/>
+      <c r="T148" s="3">
+        <v>0</v>
+      </c>
+      <c r="U148" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V148" s="3" t="str">
+        <f>VLOOKUP(U148,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W148" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X148" s="3" t="str">
+        <f>VLOOKUP(W148,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y148" s="3">
+        <v>63</v>
+      </c>
+      <c r="Z148" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="AA148" s="3">
+        <v>5201.99</v>
+      </c>
+      <c r="AB148" s="4">
+        <v>45714.69734953704</v>
+      </c>
+    </row>
+    <row r="149" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A149" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B149" s="3">
+        <v>522</v>
+      </c>
+      <c r="C149" s="3"/>
+      <c r="D149" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E149" s="3"/>
+      <c r="F149" s="3"/>
+      <c r="G149" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H149" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I149" s="3">
+        <v>362</v>
+      </c>
+      <c r="J149" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K149" s="3"/>
+      <c r="L149" s="3"/>
+      <c r="M149" s="3"/>
+      <c r="N149" s="3"/>
+      <c r="O149" s="3" t="s">
+        <v>3549</v>
+      </c>
+      <c r="P149" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q149" s="3"/>
+      <c r="R149" s="3"/>
+      <c r="S149" s="3"/>
+      <c r="T149" s="3">
+        <v>0</v>
+      </c>
+      <c r="U149" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V149" s="3" t="str">
+        <f>VLOOKUP(U149,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W149" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X149" s="3" t="str">
+        <f>VLOOKUP(W149,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y149" s="3">
+        <v>63</v>
+      </c>
+      <c r="Z149" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="AA149" s="3">
+        <v>446.69</v>
+      </c>
+      <c r="AB149" s="4">
+        <v>45714.69734953704</v>
+      </c>
+    </row>
+    <row r="150" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B150" s="3">
+        <v>523</v>
+      </c>
+      <c r="C150" s="3"/>
+      <c r="D150" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E150" s="3"/>
+      <c r="F150" s="3"/>
+      <c r="G150" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H150" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I150" s="3">
+        <v>362</v>
+      </c>
+      <c r="J150" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K150" s="3"/>
+      <c r="L150" s="3"/>
+      <c r="M150" s="3"/>
+      <c r="N150" s="3"/>
+      <c r="O150" s="3" t="s">
+        <v>3550</v>
+      </c>
+      <c r="P150" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q150" s="3"/>
+      <c r="R150" s="3"/>
+      <c r="S150" s="3"/>
+      <c r="T150" s="3">
+        <v>0</v>
+      </c>
+      <c r="U150" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V150" s="3" t="str">
+        <f>VLOOKUP(U150,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W150" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X150" s="3" t="str">
+        <f>VLOOKUP(W150,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y150" s="3">
+        <v>63</v>
+      </c>
+      <c r="Z150" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="AA150" s="3">
+        <v>10286.459999999999</v>
+      </c>
+      <c r="AB150" s="4">
+        <v>45714.69734953704</v>
+      </c>
+    </row>
+    <row r="151" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A151" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B151" s="3">
+        <v>523</v>
+      </c>
+      <c r="C151" s="3"/>
+      <c r="D151" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E151" s="3"/>
+      <c r="F151" s="3"/>
+      <c r="G151" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H151" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I151" s="3">
+        <v>362</v>
+      </c>
+      <c r="J151" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K151" s="3"/>
+      <c r="L151" s="3"/>
+      <c r="M151" s="3"/>
+      <c r="N151" s="3"/>
+      <c r="O151" s="3" t="s">
+        <v>3550</v>
+      </c>
+      <c r="P151" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q151" s="3"/>
+      <c r="R151" s="3"/>
+      <c r="S151" s="3"/>
+      <c r="T151" s="3">
+        <v>0</v>
+      </c>
+      <c r="U151" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V151" s="3" t="str">
+        <f>VLOOKUP(U151,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W151" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X151" s="3" t="str">
+        <f>VLOOKUP(W151,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y151" s="3">
+        <v>63</v>
+      </c>
+      <c r="Z151" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="AA151" s="3">
+        <v>312.25</v>
+      </c>
+      <c r="AB151" s="4">
+        <v>45714.69734953704</v>
+      </c>
+    </row>
+    <row r="152" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A152" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B152" s="3">
+        <v>524</v>
+      </c>
+      <c r="C152" s="3"/>
+      <c r="D152" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E152" s="3"/>
+      <c r="F152" s="3"/>
+      <c r="G152" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H152" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I152" s="3">
+        <v>362</v>
+      </c>
+      <c r="J152" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K152" s="3"/>
+      <c r="L152" s="3"/>
+      <c r="M152" s="3"/>
+      <c r="N152" s="3"/>
+      <c r="O152" s="3" t="s">
+        <v>3551</v>
+      </c>
+      <c r="P152" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q152" s="3"/>
+      <c r="R152" s="3"/>
+      <c r="S152" s="3"/>
+      <c r="T152" s="3">
+        <v>0</v>
+      </c>
+      <c r="U152" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V152" s="3" t="str">
+        <f>VLOOKUP(U152,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W152" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X152" s="3" t="str">
+        <f>VLOOKUP(W152,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y152" s="3">
+        <v>63</v>
+      </c>
+      <c r="Z152" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="AA152" s="3">
+        <v>1163.76</v>
+      </c>
+      <c r="AB152" s="4">
+        <v>45714.69734953704</v>
+      </c>
+    </row>
+    <row r="153" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A153" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B153" s="3">
+        <v>524</v>
+      </c>
+      <c r="C153" s="3"/>
+      <c r="D153" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E153" s="3"/>
+      <c r="F153" s="3"/>
+      <c r="G153" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H153" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I153" s="3">
+        <v>362</v>
+      </c>
+      <c r="J153" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K153" s="3"/>
+      <c r="L153" s="3"/>
+      <c r="M153" s="3"/>
+      <c r="N153" s="3"/>
+      <c r="O153" s="3" t="s">
+        <v>3551</v>
+      </c>
+      <c r="P153" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q153" s="3"/>
+      <c r="R153" s="3"/>
+      <c r="S153" s="3"/>
+      <c r="T153" s="3">
+        <v>0</v>
+      </c>
+      <c r="U153" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V153" s="3" t="str">
+        <f>VLOOKUP(U153,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W153" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X153" s="3" t="str">
+        <f>VLOOKUP(W153,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y153" s="3">
+        <v>63</v>
+      </c>
+      <c r="Z153" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="AA153" s="3">
+        <v>112.7</v>
+      </c>
+      <c r="AB153" s="4">
+        <v>45714.69734953704</v>
+      </c>
+    </row>
+    <row r="154" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A154" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B154" s="3">
+        <v>525</v>
+      </c>
+      <c r="C154" s="3"/>
+      <c r="D154" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E154" s="3"/>
+      <c r="F154" s="3"/>
+      <c r="G154" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H154" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I154" s="3">
+        <v>362</v>
+      </c>
+      <c r="J154" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K154" s="3"/>
+      <c r="L154" s="3"/>
+      <c r="M154" s="3"/>
+      <c r="N154" s="3"/>
+      <c r="O154" s="3" t="s">
+        <v>3552</v>
+      </c>
+      <c r="P154" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q154" s="3"/>
+      <c r="R154" s="3"/>
+      <c r="S154" s="3"/>
+      <c r="T154" s="3">
+        <v>0</v>
+      </c>
+      <c r="U154" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V154" s="3" t="str">
+        <f>VLOOKUP(U154,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W154" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X154" s="3" t="str">
+        <f>VLOOKUP(W154,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y154" s="3">
+        <v>63</v>
+      </c>
+      <c r="Z154" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="AA154" s="3">
+        <v>7663.6</v>
+      </c>
+      <c r="AB154" s="4">
+        <v>45714.69734953704</v>
+      </c>
+    </row>
+    <row r="155" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A155" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B155" s="3">
+        <v>525</v>
+      </c>
+      <c r="C155" s="3"/>
+      <c r="D155" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E155" s="3"/>
+      <c r="F155" s="3"/>
+      <c r="G155" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H155" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I155" s="3">
+        <v>362</v>
+      </c>
+      <c r="J155" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K155" s="3"/>
+      <c r="L155" s="3"/>
+      <c r="M155" s="3"/>
+      <c r="N155" s="3"/>
+      <c r="O155" s="3" t="s">
+        <v>3552</v>
+      </c>
+      <c r="P155" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q155" s="3"/>
+      <c r="R155" s="3"/>
+      <c r="S155" s="3"/>
+      <c r="T155" s="3">
+        <v>0</v>
+      </c>
+      <c r="U155" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V155" s="3" t="str">
+        <f>VLOOKUP(U155,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W155" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X155" s="3" t="str">
+        <f>VLOOKUP(W155,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y155" s="3">
+        <v>63</v>
+      </c>
+      <c r="Z155" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="AA155" s="3">
+        <v>1913.38</v>
+      </c>
+      <c r="AB155" s="4">
+        <v>45714.69734953704</v>
+      </c>
+    </row>
+    <row r="156" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A156" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B156" s="3">
+        <v>526</v>
+      </c>
+      <c r="C156" s="3"/>
+      <c r="D156" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E156" s="3"/>
+      <c r="F156" s="3"/>
+      <c r="G156" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H156" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I156" s="3">
+        <v>362</v>
+      </c>
+      <c r="J156" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K156" s="3"/>
+      <c r="L156" s="3"/>
+      <c r="M156" s="3"/>
+      <c r="N156" s="3"/>
+      <c r="O156" s="3" t="s">
+        <v>3553</v>
+      </c>
+      <c r="P156" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q156" s="3"/>
+      <c r="R156" s="3"/>
+      <c r="S156" s="3"/>
+      <c r="T156" s="3">
+        <v>0</v>
+      </c>
+      <c r="U156" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V156" s="3" t="str">
+        <f>VLOOKUP(U156,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W156" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X156" s="3" t="str">
+        <f>VLOOKUP(W156,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y156" s="3">
+        <v>63</v>
+      </c>
+      <c r="Z156" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="AA156" s="3">
+        <v>5266.27</v>
+      </c>
+      <c r="AB156" s="4">
+        <v>45714.69734953704</v>
+      </c>
+    </row>
+    <row r="157" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A157" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B157" s="3">
+        <v>526</v>
+      </c>
+      <c r="C157" s="3"/>
+      <c r="D157" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E157" s="3"/>
+      <c r="F157" s="3"/>
+      <c r="G157" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H157" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I157" s="3">
+        <v>362</v>
+      </c>
+      <c r="J157" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K157" s="3"/>
+      <c r="L157" s="3"/>
+      <c r="M157" s="3"/>
+      <c r="N157" s="3"/>
+      <c r="O157" s="3" t="s">
+        <v>3553</v>
+      </c>
+      <c r="P157" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q157" s="3"/>
+      <c r="R157" s="3"/>
+      <c r="S157" s="3"/>
+      <c r="T157" s="3">
+        <v>0</v>
+      </c>
+      <c r="U157" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V157" s="3" t="str">
+        <f>VLOOKUP(U157,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W157" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X157" s="3" t="str">
+        <f>VLOOKUP(W157,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y157" s="3">
+        <v>63</v>
+      </c>
+      <c r="Z157" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="AA157" s="3">
+        <v>9807.02</v>
+      </c>
+      <c r="AB157" s="4">
+        <v>45714.69734953704</v>
+      </c>
+    </row>
+    <row r="158" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B158" s="3">
+        <v>571</v>
+      </c>
+      <c r="C158" s="3"/>
+      <c r="D158" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E158" s="3"/>
+      <c r="F158" s="3"/>
+      <c r="G158" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H158" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I158" s="3">
+        <v>362</v>
+      </c>
+      <c r="J158" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K158" s="3"/>
+      <c r="L158" s="3"/>
+      <c r="M158" s="3"/>
+      <c r="N158" s="3"/>
+      <c r="O158" s="3" t="s">
+        <v>3554</v>
+      </c>
+      <c r="P158" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q158" s="3"/>
+      <c r="R158" s="3"/>
+      <c r="S158" s="3"/>
+      <c r="T158" s="3">
+        <v>0</v>
+      </c>
+      <c r="U158" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V158" s="3" t="str">
+        <f>VLOOKUP(U158,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W158" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X158" s="3" t="str">
+        <f>VLOOKUP(W158,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y158" s="3">
+        <v>63</v>
+      </c>
+      <c r="Z158" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="AA158" s="3">
+        <v>257917.62</v>
+      </c>
+      <c r="AB158" s="4">
+        <v>45716.697349849535</v>
+      </c>
+    </row>
+    <row r="159" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B159" s="3">
+        <v>571</v>
+      </c>
+      <c r="C159" s="3"/>
+      <c r="D159" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E159" s="3"/>
+      <c r="F159" s="3"/>
+      <c r="G159" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H159" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I159" s="3">
+        <v>362</v>
+      </c>
+      <c r="J159" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K159" s="3"/>
+      <c r="L159" s="3"/>
+      <c r="M159" s="3"/>
+      <c r="N159" s="3"/>
+      <c r="O159" s="3" t="s">
+        <v>3554</v>
+      </c>
+      <c r="P159" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q159" s="3"/>
+      <c r="R159" s="3"/>
+      <c r="S159" s="3"/>
+      <c r="T159" s="3">
+        <v>0</v>
+      </c>
+      <c r="U159" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V159" s="3" t="str">
+        <f>VLOOKUP(U159,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W159" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X159" s="3" t="str">
+        <f>VLOOKUP(W159,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y159" s="3">
+        <v>63</v>
+      </c>
+      <c r="Z159" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="AA159" s="3">
+        <v>55123.31</v>
+      </c>
+      <c r="AB159" s="4">
+        <v>45716.697349849535</v>
+      </c>
+    </row>
+    <row r="160" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B160" s="3">
+        <v>582</v>
+      </c>
+      <c r="C160" s="3"/>
+      <c r="D160" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E160" s="3"/>
+      <c r="F160" s="3"/>
+      <c r="G160" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H160" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I160" s="3">
+        <v>362</v>
+      </c>
+      <c r="J160" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K160" s="3"/>
+      <c r="L160" s="3"/>
+      <c r="M160" s="3"/>
+      <c r="N160" s="3"/>
+      <c r="O160" s="3" t="s">
+        <v>3555</v>
+      </c>
+      <c r="P160" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q160" s="3"/>
+      <c r="R160" s="3"/>
+      <c r="S160" s="3"/>
+      <c r="T160" s="3">
+        <v>0</v>
+      </c>
+      <c r="U160" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V160" s="3" t="str">
+        <f>VLOOKUP(U160,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W160" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X160" s="3" t="str">
+        <f>VLOOKUP(W160,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y160" s="3">
+        <v>63</v>
+      </c>
+      <c r="Z160" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="AA160" s="3">
+        <v>67617.5</v>
+      </c>
+      <c r="AB160" s="4">
+        <v>45716.697349849535</v>
+      </c>
+    </row>
+    <row r="161" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A161" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B161" s="3">
+        <v>582</v>
+      </c>
+      <c r="C161" s="3"/>
+      <c r="D161" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E161" s="3"/>
+      <c r="F161" s="3"/>
+      <c r="G161" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H161" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I161" s="3">
+        <v>362</v>
+      </c>
+      <c r="J161" s="3" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K161" s="3"/>
+      <c r="L161" s="3"/>
+      <c r="M161" s="3"/>
+      <c r="N161" s="3"/>
+      <c r="O161" s="3" t="s">
+        <v>3555</v>
+      </c>
+      <c r="P161" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q161" s="3"/>
+      <c r="R161" s="3"/>
+      <c r="S161" s="3"/>
+      <c r="T161" s="3">
+        <v>0</v>
+      </c>
+      <c r="U161" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V161" s="3" t="str">
+        <f>VLOOKUP(U161,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W161" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X161" s="3" t="str">
+        <f>VLOOKUP(W161,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y161" s="3">
+        <v>63</v>
+      </c>
+      <c r="Z161" s="3" t="s">
+        <v>3566</v>
+      </c>
+      <c r="AA161" s="3">
+        <v>15767.5</v>
+      </c>
+      <c r="AB161" s="4">
+        <v>45716.697349849535</v>
+      </c>
+    </row>
+    <row r="162" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B162" s="3">
+        <v>225</v>
+      </c>
+      <c r="C162" s="3"/>
+      <c r="D162" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E162" s="3"/>
+      <c r="F162" s="3"/>
+      <c r="G162" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H162" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I162" s="3">
+        <v>362</v>
+      </c>
+      <c r="J162" s="3" t="s">
+        <v>3535</v>
+      </c>
+      <c r="K162" s="3"/>
+      <c r="L162" s="3"/>
+      <c r="M162" s="3"/>
+      <c r="N162" s="3"/>
+      <c r="O162" s="3" t="s">
+        <v>3556</v>
+      </c>
+      <c r="P162" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q162" s="3"/>
+      <c r="R162" s="3"/>
+      <c r="S162" s="3"/>
+      <c r="T162" s="3">
+        <v>0</v>
+      </c>
+      <c r="U162" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V162" s="3" t="str">
+        <f>VLOOKUP(U162,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W162" s="3" t="s">
+        <v>2679</v>
+      </c>
+      <c r="X162" s="3" t="str">
+        <f>VLOOKUP(W162,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.5. 4  1. 3  1: MULTAS</v>
+      </c>
+      <c r="Y162" s="3">
+        <v>31</v>
+      </c>
+      <c r="Z162" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA162" s="3">
+        <v>1162.79</v>
+      </c>
+      <c r="AB162" s="4">
+        <v>45693.428518518522</v>
+      </c>
+    </row>
+    <row r="163" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B163" s="3">
+        <v>247</v>
+      </c>
+      <c r="C163" s="3"/>
+      <c r="D163" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E163" s="3"/>
+      <c r="F163" s="3"/>
+      <c r="G163" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H163" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I163" s="3"/>
+      <c r="J163" s="3" t="s">
+        <v>3539</v>
+      </c>
+      <c r="K163" s="3"/>
+      <c r="L163" s="3"/>
+      <c r="M163" s="3"/>
+      <c r="N163" s="3"/>
+      <c r="O163" s="3" t="s">
+        <v>3557</v>
+      </c>
+      <c r="P163" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q163" s="3"/>
+      <c r="R163" s="3"/>
+      <c r="S163" s="3"/>
+      <c r="T163" s="3">
+        <v>9</v>
+      </c>
+      <c r="U163" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="V163" s="3" t="str">
+        <f>VLOOKUP(U163,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">09: RECURSOS DIRECTAMENTE RECAUDADOS                                                                                                                      </v>
+      </c>
+      <c r="W163" s="3" t="s">
+        <v>2135</v>
+      </c>
+      <c r="X163" s="3" t="str">
+        <f>VLOOKUP(W163,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.3. 2  1. 2 99: OTROS GASTOS</v>
+      </c>
+      <c r="Y163" s="3">
+        <v>24</v>
+      </c>
+      <c r="Z163" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA163" s="3">
+        <v>221931.16</v>
+      </c>
+      <c r="AB163" s="4">
+        <v>45695.428518518522</v>
+      </c>
+    </row>
+    <row r="164" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A164" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B164" s="3">
+        <v>247</v>
+      </c>
+      <c r="C164" s="3"/>
+      <c r="D164" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E164" s="3"/>
+      <c r="F164" s="3"/>
+      <c r="G164" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H164" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I164" s="3"/>
+      <c r="J164" s="3" t="s">
+        <v>3539</v>
+      </c>
+      <c r="K164" s="3"/>
+      <c r="L164" s="3"/>
+      <c r="M164" s="3"/>
+      <c r="N164" s="3"/>
+      <c r="O164" s="3" t="s">
+        <v>3557</v>
+      </c>
+      <c r="P164" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q164" s="3"/>
+      <c r="R164" s="3"/>
+      <c r="S164" s="3"/>
+      <c r="T164" s="3">
+        <v>9</v>
+      </c>
+      <c r="U164" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="V164" s="3" t="str">
+        <f>VLOOKUP(U164,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">09: RECURSOS DIRECTAMENTE RECAUDADOS                                                                                                                      </v>
+      </c>
+      <c r="W164" s="3" t="s">
+        <v>2135</v>
+      </c>
+      <c r="X164" s="3" t="str">
+        <f>VLOOKUP(W164,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.3. 2  1. 2 99: OTROS GASTOS</v>
+      </c>
+      <c r="Y164" s="3">
+        <v>24</v>
+      </c>
+      <c r="Z164" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA164" s="3">
+        <v>2161.84</v>
+      </c>
+      <c r="AB164" s="4">
+        <v>45695.428518518522</v>
+      </c>
+    </row>
+    <row r="165" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B165" s="3">
+        <v>507</v>
+      </c>
+      <c r="C165" s="3"/>
+      <c r="D165" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E165" s="3"/>
+      <c r="F165" s="3"/>
+      <c r="G165" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H165" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I165" s="3"/>
+      <c r="J165" s="3" t="s">
+        <v>3539</v>
+      </c>
+      <c r="K165" s="3"/>
+      <c r="L165" s="3"/>
+      <c r="M165" s="3"/>
+      <c r="N165" s="3"/>
+      <c r="O165" s="3" t="s">
+        <v>3558</v>
+      </c>
+      <c r="P165" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q165" s="3"/>
+      <c r="R165" s="3"/>
+      <c r="S165" s="3"/>
+      <c r="T165" s="3">
+        <v>9</v>
+      </c>
+      <c r="U165" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="V165" s="3" t="str">
+        <f>VLOOKUP(U165,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">09: RECURSOS DIRECTAMENTE RECAUDADOS                                                                                                                      </v>
+      </c>
+      <c r="W165" s="3" t="s">
+        <v>2135</v>
+      </c>
+      <c r="X165" s="3" t="str">
+        <f>VLOOKUP(W165,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.3. 2  1. 2 99: OTROS GASTOS</v>
+      </c>
+      <c r="Y165" s="3">
+        <v>24</v>
+      </c>
+      <c r="Z165" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA165" s="3">
+        <v>221743.31</v>
+      </c>
+      <c r="AB165" s="4">
+        <v>45715.42851597222</v>
+      </c>
+    </row>
+    <row r="166" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A166" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B166" s="3">
+        <v>507</v>
+      </c>
+      <c r="C166" s="3"/>
+      <c r="D166" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E166" s="3"/>
+      <c r="F166" s="3"/>
+      <c r="G166" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H166" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I166" s="3"/>
+      <c r="J166" s="3" t="s">
+        <v>3539</v>
+      </c>
+      <c r="K166" s="3"/>
+      <c r="L166" s="3"/>
+      <c r="M166" s="3"/>
+      <c r="N166" s="3"/>
+      <c r="O166" s="3" t="s">
+        <v>3558</v>
+      </c>
+      <c r="P166" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q166" s="3"/>
+      <c r="R166" s="3"/>
+      <c r="S166" s="3"/>
+      <c r="T166" s="3">
+        <v>9</v>
+      </c>
+      <c r="U166" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="V166" s="3" t="str">
+        <f>VLOOKUP(U166,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">09: RECURSOS DIRECTAMENTE RECAUDADOS                                                                                                                      </v>
+      </c>
+      <c r="W166" s="3" t="s">
+        <v>2135</v>
+      </c>
+      <c r="X166" s="3" t="str">
+        <f>VLOOKUP(W166,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.3. 2  1. 2 99: OTROS GASTOS</v>
+      </c>
+      <c r="Y166" s="3">
+        <v>24</v>
+      </c>
+      <c r="Z166" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA166" s="3">
+        <v>2419.69</v>
+      </c>
+      <c r="AB166" s="4">
+        <v>45715.42851597222</v>
+      </c>
+    </row>
+    <row r="167" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A167" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B167" s="3">
+        <v>327</v>
+      </c>
+      <c r="C167" s="3"/>
+      <c r="D167" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E167" s="3"/>
+      <c r="F167" s="3"/>
+      <c r="G167" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H167" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I167" s="3">
+        <v>196</v>
+      </c>
+      <c r="J167" s="3" t="s">
+        <v>3540</v>
+      </c>
+      <c r="K167" s="3"/>
+      <c r="L167" s="3"/>
+      <c r="M167" s="3"/>
+      <c r="N167" s="3"/>
+      <c r="O167" s="3" t="s">
+        <v>3559</v>
+      </c>
+      <c r="P167" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q167" s="3"/>
+      <c r="R167" s="3"/>
+      <c r="S167" s="3"/>
+      <c r="T167" s="3">
+        <v>0</v>
+      </c>
+      <c r="U167" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V167" s="3" t="str">
+        <f>VLOOKUP(U167,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W167" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="X167" s="3" t="str">
+        <f>VLOOKUP(W167,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.3. 2  1. 2  1: PASAJES Y GASTOS DE TRANSPORTE</v>
+      </c>
+      <c r="Y167" s="3">
+        <v>22</v>
+      </c>
+      <c r="Z167" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA167" s="3">
+        <v>90</v>
+      </c>
+      <c r="AB167" s="4">
+        <v>45702.520452280092</v>
+      </c>
+    </row>
+    <row r="168" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A168" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B168" s="3">
+        <v>346</v>
+      </c>
+      <c r="C168" s="3"/>
+      <c r="D168" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E168" s="3"/>
+      <c r="F168" s="3"/>
+      <c r="G168" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H168" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I168" s="3"/>
+      <c r="J168" s="3" t="s">
+        <v>3541</v>
+      </c>
+      <c r="K168" s="3"/>
+      <c r="L168" s="3"/>
+      <c r="M168" s="3"/>
+      <c r="N168" s="3"/>
+      <c r="O168" s="3" t="s">
+        <v>3560</v>
+      </c>
+      <c r="P168" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q168" s="3"/>
+      <c r="R168" s="3"/>
+      <c r="S168" s="3"/>
+      <c r="T168" s="3">
+        <v>0</v>
+      </c>
+      <c r="U168" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V168" s="3" t="str">
+        <f>VLOOKUP(U168,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W168" s="3" t="s">
+        <v>2517</v>
+      </c>
+      <c r="X168" s="3" t="str">
+        <f>VLOOKUP(W168,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.4. 1  3. 1  1: A OTRAS UNIDADES DEL GOBIERNO NACIONAL</v>
+      </c>
+      <c r="Y168" s="3">
+        <v>39</v>
+      </c>
+      <c r="Z168" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA168" s="3">
+        <v>68270</v>
+      </c>
+      <c r="AB168" s="4">
+        <v>45702.520452280092</v>
+      </c>
+    </row>
+    <row r="169" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A169" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B169" s="3">
+        <v>347</v>
+      </c>
+      <c r="C169" s="3"/>
+      <c r="D169" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E169" s="3"/>
+      <c r="F169" s="3"/>
+      <c r="G169" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H169" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I169" s="3">
+        <v>284</v>
+      </c>
+      <c r="J169" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K169" s="3"/>
+      <c r="L169" s="3"/>
+      <c r="M169" s="3"/>
+      <c r="N169" s="3"/>
+      <c r="O169" s="3" t="s">
+        <v>3561</v>
+      </c>
+      <c r="P169" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q169" s="3"/>
+      <c r="R169" s="3"/>
+      <c r="S169" s="3"/>
+      <c r="T169" s="3">
+        <v>0</v>
+      </c>
+      <c r="U169" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V169" s="3" t="str">
+        <f>VLOOKUP(U169,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W169" s="3" t="s">
+        <v>2695</v>
+      </c>
+      <c r="X169" s="3" t="str">
+        <f>VLOOKUP(W169,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.5. 4  3. 1  1: IMPUESTOS</v>
+      </c>
+      <c r="Y169" s="3">
+        <v>31</v>
+      </c>
+      <c r="Z169" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA169" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="AB169" s="4">
+        <v>45702.520452280092</v>
+      </c>
+    </row>
+    <row r="170" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A170" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B170" s="3">
+        <v>347</v>
+      </c>
+      <c r="C170" s="3"/>
+      <c r="D170" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E170" s="3"/>
+      <c r="F170" s="3"/>
+      <c r="G170" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H170" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I170" s="3">
+        <v>284</v>
+      </c>
+      <c r="J170" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K170" s="3"/>
+      <c r="L170" s="3"/>
+      <c r="M170" s="3"/>
+      <c r="N170" s="3"/>
+      <c r="O170" s="3" t="s">
+        <v>3561</v>
+      </c>
+      <c r="P170" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q170" s="3"/>
+      <c r="R170" s="3"/>
+      <c r="S170" s="3"/>
+      <c r="T170" s="3">
+        <v>0</v>
+      </c>
+      <c r="U170" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V170" s="3" t="str">
+        <f>VLOOKUP(U170,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W170" s="3" t="s">
+        <v>2699</v>
+      </c>
+      <c r="X170" s="3" t="str">
+        <f>VLOOKUP(W170,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.5. 4  3. 2  1: DERECHOS ADMINISTRATIVOS</v>
+      </c>
+      <c r="Y170" s="3">
+        <v>31</v>
+      </c>
+      <c r="Z170" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA170" s="3">
+        <v>716.4</v>
+      </c>
+      <c r="AB170" s="4">
+        <v>45702.520452280092</v>
+      </c>
+    </row>
+    <row r="171" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A171" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B171" s="3">
+        <v>431</v>
+      </c>
+      <c r="C171" s="3"/>
+      <c r="D171" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E171" s="3"/>
+      <c r="F171" s="3"/>
+      <c r="G171" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H171" s="3" t="s">
+        <v>3532</v>
+      </c>
+      <c r="I171" s="3"/>
+      <c r="J171" s="3" t="s">
+        <v>3536</v>
+      </c>
+      <c r="K171" s="3"/>
+      <c r="L171" s="3"/>
+      <c r="M171" s="3"/>
+      <c r="N171" s="3"/>
+      <c r="O171" s="3" t="s">
+        <v>3562</v>
+      </c>
+      <c r="P171" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q171" s="3"/>
+      <c r="R171" s="3"/>
+      <c r="S171" s="3"/>
+      <c r="T171" s="3">
+        <v>0</v>
+      </c>
+      <c r="U171" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V171" s="3" t="str">
+        <f>VLOOKUP(U171,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
+      </c>
+      <c r="W171" s="3" t="s">
+        <v>2657</v>
+      </c>
+      <c r="X171" s="3" t="str">
+        <f>VLOOKUP(W171,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.5. 3  1. 1  1: A ESTUDIANTES</v>
+      </c>
+      <c r="Y171" s="3">
+        <v>57</v>
+      </c>
+      <c r="Z171" s="3" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA171" s="3">
+        <v>50000</v>
+      </c>
+      <c r="AB171" s="4">
+        <v>45706.597614733793</v>
+      </c>
+    </row>
+    <row r="172" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A172" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B172" s="3">
+        <v>570</v>
+      </c>
+      <c r="C172" s="3"/>
+      <c r="D172" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E172" s="3"/>
+      <c r="F172" s="3"/>
+      <c r="G172" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H172" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I172" s="3">
+        <v>368</v>
+      </c>
+      <c r="J172" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K172" s="3"/>
+      <c r="L172" s="3"/>
+      <c r="M172" s="3"/>
+      <c r="N172" s="3"/>
+      <c r="O172" s="3" t="s">
+        <v>3563</v>
+      </c>
+      <c r="P172" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q172" s="3"/>
+      <c r="R172" s="3"/>
+      <c r="S172" s="3"/>
+      <c r="T172" s="3">
+        <v>18</v>
+      </c>
+      <c r="U172" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V172" s="3" t="str">
+        <f>VLOOKUP(U172,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v>18: CANON Y SOBRECANON, REGALIAS, RENTA DE ADUANAS Y PARTICIPACIONES</v>
+      </c>
+      <c r="W172" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X172" s="3" t="str">
+        <f>VLOOKUP(W172,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y172" s="3">
+        <v>64</v>
+      </c>
+      <c r="Z172" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA172" s="3">
+        <v>28595.64</v>
+      </c>
+      <c r="AB172" s="4">
+        <v>45716.697349849535</v>
+      </c>
+    </row>
+    <row r="173" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A173" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B173" s="3">
+        <v>570</v>
+      </c>
+      <c r="C173" s="3"/>
+      <c r="D173" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E173" s="3"/>
+      <c r="F173" s="3"/>
+      <c r="G173" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H173" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I173" s="3">
+        <v>368</v>
+      </c>
+      <c r="J173" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K173" s="3"/>
+      <c r="L173" s="3"/>
+      <c r="M173" s="3"/>
+      <c r="N173" s="3"/>
+      <c r="O173" s="3" t="s">
+        <v>3563</v>
+      </c>
+      <c r="P173" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q173" s="3"/>
+      <c r="R173" s="3"/>
+      <c r="S173" s="3"/>
+      <c r="T173" s="3">
+        <v>18</v>
+      </c>
+      <c r="U173" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V173" s="3" t="str">
+        <f>VLOOKUP(U173,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v>18: CANON Y SOBRECANON, REGALIAS, RENTA DE ADUANAS Y PARTICIPACIONES</v>
+      </c>
+      <c r="W173" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X173" s="3" t="str">
+        <f>VLOOKUP(W173,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y173" s="3">
+        <v>64</v>
+      </c>
+      <c r="Z173" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA173" s="3">
+        <v>6766.9</v>
+      </c>
+      <c r="AB173" s="4">
+        <v>45716.697349849535</v>
+      </c>
+    </row>
+    <row r="174" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B174" s="3">
+        <v>569</v>
+      </c>
+      <c r="C174" s="3"/>
+      <c r="D174" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E174" s="3"/>
+      <c r="F174" s="3"/>
+      <c r="G174" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H174" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I174" s="3">
+        <v>368</v>
+      </c>
+      <c r="J174" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K174" s="3"/>
+      <c r="L174" s="3"/>
+      <c r="M174" s="3"/>
+      <c r="N174" s="3"/>
+      <c r="O174" s="3" t="s">
+        <v>3564</v>
+      </c>
+      <c r="P174" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q174" s="3"/>
+      <c r="R174" s="3"/>
+      <c r="S174" s="3"/>
+      <c r="T174" s="3">
+        <v>18</v>
+      </c>
+      <c r="U174" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V174" s="3" t="str">
+        <f>VLOOKUP(U174,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v>18: CANON Y SOBRECANON, REGALIAS, RENTA DE ADUANAS Y PARTICIPACIONES</v>
+      </c>
+      <c r="W174" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X174" s="3" t="str">
+        <f>VLOOKUP(W174,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y174" s="3">
+        <v>69</v>
+      </c>
+      <c r="Z174" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA174" s="3">
+        <v>19012.62</v>
+      </c>
+      <c r="AB174" s="4">
+        <v>45716.697349849535</v>
+      </c>
+    </row>
+    <row r="175" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A175" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B175" s="3">
+        <v>569</v>
+      </c>
+      <c r="C175" s="3"/>
+      <c r="D175" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E175" s="3"/>
+      <c r="F175" s="3"/>
+      <c r="G175" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H175" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I175" s="3">
+        <v>368</v>
+      </c>
+      <c r="J175" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="K175" s="3"/>
+      <c r="L175" s="3"/>
+      <c r="M175" s="3"/>
+      <c r="N175" s="3"/>
+      <c r="O175" s="3" t="s">
+        <v>3564</v>
+      </c>
+      <c r="P175" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q175" s="3"/>
+      <c r="R175" s="3"/>
+      <c r="S175" s="3"/>
+      <c r="T175" s="3">
+        <v>18</v>
+      </c>
+      <c r="U175" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="V175" s="3" t="str">
+        <f>VLOOKUP(U175,fuente_financiamiento!A$1:B$4,2,0)</f>
+        <v>18: CANON Y SOBRECANON, REGALIAS, RENTA DE ADUANAS Y PARTICIPACIONES</v>
+      </c>
+      <c r="W175" s="3" t="s">
+        <v>2817</v>
+      </c>
+      <c r="X175" s="3" t="str">
+        <f>VLOOKUP(W175,clasificador!A$1:B$1635,2,0)</f>
+        <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
+      </c>
+      <c r="Y175" s="3">
+        <v>69</v>
+      </c>
+      <c r="Z175" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA175" s="3">
+        <v>4537.21</v>
+      </c>
+      <c r="AB175" s="4">
+        <v>45716.697349849535</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AB136" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FF48C4-0B42-4380-95AC-0257E17CBFC1}">
+  <dimension ref="A1:A39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <v>45671</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>45681</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>45687</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>45687</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>45694</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>45694</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>45716</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>45716</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>45698</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>45699</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>45699</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>45714</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>45714</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>45714</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>45714</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>45714</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>45714</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>45714</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>45714</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>45714</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>45714</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>45716</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>45716</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>45716</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>45716</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>45693</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>45695</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>45695</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>45715</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>45715</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>45702</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>45702</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>45702</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>45702</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>45706</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>45716</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>45716</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>45716</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>45716</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6221D2DB-799F-4324-BBD2-ADABBC53D541}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22985,16 +25968,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5195F7-D3C3-4C49-8E44-49F942F20CCF}">
   <dimension ref="A1:B1635"/>
   <sheetViews>
-    <sheetView topLeftCell="A1598" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A1200" workbookViewId="0">
+      <selection activeCell="A1209" sqref="A1209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
actualizacion de la data del siaf
</commit_message>
<xml_diff>
--- a/data/ep_mes_2025.xlsx
+++ b/data/ep_mes_2025.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6. Código\seguimiento_presupuestal_unsch_streamlit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592FABA8-7EAD-472B-B910-5F6413374F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D373BD79-3B53-4936-8211-F6E8E915143A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="4" r:id="rId2"/>
-    <sheet name="fuente_financiamiento" sheetId="2" r:id="rId3"/>
-    <sheet name="clasificador" sheetId="3" r:id="rId4"/>
+    <sheet name="fuente_financiamiento" sheetId="2" r:id="rId2"/>
+    <sheet name="clasificador" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$AB$136</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$AB$175</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5209" uniqueCount="3567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5209" uniqueCount="3566">
   <si>
     <t>ano_eje</t>
   </si>
@@ -10636,9 +10635,6 @@
   </si>
   <si>
     <t>2.8. 3  2. 3 99: OTROS CREDITOS INTERNOS</t>
-  </si>
-  <si>
-    <t>OFICINA DE COOPERACIÓN Y RELACIONES INTERINSTITUCIONALES</t>
   </si>
   <si>
     <t>94.02.18.04</t>
@@ -10788,10 +10784,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -11076,14 +11071,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="G129" sqref="G129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="22.42578125" customWidth="1"/>
-    <col min="8" max="8" width="58.7109375" customWidth="1"/>
+    <col min="8" max="8" width="78.42578125" customWidth="1"/>
     <col min="10" max="10" width="19.85546875" customWidth="1"/>
     <col min="11" max="11" width="15.28515625" customWidth="1"/>
     <col min="15" max="15" width="43.85546875" customWidth="1"/>
@@ -23066,2639 +23061,2638 @@
       </c>
     </row>
     <row r="137" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A137" s="3" t="s">
+      <c r="A137" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B137" s="3">
+      <c r="B137" s="2">
         <v>9</v>
       </c>
-      <c r="C137" s="3"/>
-      <c r="D137" s="3" t="s">
+      <c r="C137" s="2"/>
+      <c r="D137" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E137" s="3"/>
-      <c r="F137" s="3"/>
-      <c r="G137" s="3" t="s">
+      <c r="E137" s="2"/>
+      <c r="F137" s="2"/>
+      <c r="G137" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H137" s="3" t="s">
+      <c r="H137" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I137" s="3"/>
-      <c r="J137" s="3" t="s">
-        <v>3535</v>
-      </c>
-      <c r="K137" s="3"/>
-      <c r="L137" s="3"/>
-      <c r="M137" s="3"/>
-      <c r="N137" s="3"/>
-      <c r="O137" s="3" t="s">
-        <v>3542</v>
-      </c>
-      <c r="P137" s="3" t="s">
+      <c r="I137" s="2"/>
+      <c r="J137" s="2" t="s">
+        <v>3534</v>
+      </c>
+      <c r="K137" s="2"/>
+      <c r="L137" s="2"/>
+      <c r="M137" s="2"/>
+      <c r="N137" s="2"/>
+      <c r="O137" s="2" t="s">
+        <v>3541</v>
+      </c>
+      <c r="P137" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q137" s="3"/>
-      <c r="R137" s="3"/>
-      <c r="S137" s="3"/>
-      <c r="T137" s="3">
+      <c r="Q137" s="2"/>
+      <c r="R137" s="2"/>
+      <c r="S137" s="2"/>
+      <c r="T137" s="2">
         <v>0</v>
       </c>
-      <c r="U137" s="3" t="s">
+      <c r="U137" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V137" s="3" t="str">
+      <c r="V137" s="2" t="str">
         <f>VLOOKUP(U137,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W137" s="3" t="s">
+      <c r="W137" s="2" t="s">
         <v>2679</v>
       </c>
-      <c r="X137" s="3" t="str">
+      <c r="X137" s="2" t="str">
         <f>VLOOKUP(W137,clasificador!A$1:B$1635,2,0)</f>
         <v>2.5. 4  1. 3  1: MULTAS</v>
       </c>
-      <c r="Y137" s="3">
+      <c r="Y137" s="2">
         <v>31</v>
       </c>
-      <c r="Z137" s="3" t="s">
+      <c r="Z137" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AA137" s="3">
+      <c r="AA137" s="2">
         <v>53479.77</v>
       </c>
-      <c r="AB137" s="4">
+      <c r="AB137" s="3">
         <v>45671.69734953704</v>
       </c>
     </row>
     <row r="138" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A138" s="3" t="s">
+      <c r="A138" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B138" s="3">
+      <c r="B138" s="2">
         <v>83</v>
       </c>
-      <c r="C138" s="3"/>
-      <c r="D138" s="3" t="s">
+      <c r="C138" s="2"/>
+      <c r="D138" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E138" s="3"/>
-      <c r="F138" s="3"/>
-      <c r="G138" s="3" t="s">
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
+      <c r="G138" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H138" s="3" t="s">
-        <v>3532</v>
-      </c>
-      <c r="I138" s="3"/>
-      <c r="J138" s="3" t="s">
-        <v>3536</v>
-      </c>
-      <c r="K138" s="3"/>
-      <c r="L138" s="3"/>
-      <c r="M138" s="3"/>
-      <c r="N138" s="3"/>
-      <c r="O138" s="3" t="s">
-        <v>3543</v>
-      </c>
-      <c r="P138" s="3" t="s">
+      <c r="H138" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I138" s="2"/>
+      <c r="J138" s="2" t="s">
+        <v>3535</v>
+      </c>
+      <c r="K138" s="2"/>
+      <c r="L138" s="2"/>
+      <c r="M138" s="2"/>
+      <c r="N138" s="2"/>
+      <c r="O138" s="2" t="s">
+        <v>3542</v>
+      </c>
+      <c r="P138" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q138" s="3"/>
-      <c r="R138" s="3"/>
-      <c r="S138" s="3"/>
-      <c r="T138" s="3">
+      <c r="Q138" s="2"/>
+      <c r="R138" s="2"/>
+      <c r="S138" s="2"/>
+      <c r="T138" s="2">
         <v>0</v>
       </c>
-      <c r="U138" s="3" t="s">
+      <c r="U138" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V138" s="3" t="str">
+      <c r="V138" s="2" t="str">
         <f>VLOOKUP(U138,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W138" s="3" t="s">
+      <c r="W138" s="2" t="s">
         <v>2657</v>
       </c>
-      <c r="X138" s="3" t="str">
+      <c r="X138" s="2" t="str">
         <f>VLOOKUP(W138,clasificador!A$1:B$1635,2,0)</f>
         <v>2.5. 3  1. 1  1: A ESTUDIANTES</v>
       </c>
-      <c r="Y138" s="3">
+      <c r="Y138" s="2">
         <v>57</v>
       </c>
-      <c r="Z138" s="3" t="s">
-        <v>3565</v>
-      </c>
-      <c r="AA138" s="3">
+      <c r="Z138" s="2" t="s">
+        <v>3564</v>
+      </c>
+      <c r="AA138" s="2">
         <v>40000</v>
       </c>
-      <c r="AB138" s="4">
+      <c r="AB138" s="3">
         <v>45681.69734953704</v>
       </c>
     </row>
     <row r="139" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A139" s="3" t="s">
+      <c r="A139" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B139" s="3">
+      <c r="B139" s="2">
         <v>119</v>
       </c>
-      <c r="C139" s="3"/>
-      <c r="D139" s="3" t="s">
+      <c r="C139" s="2"/>
+      <c r="D139" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E139" s="3"/>
-      <c r="F139" s="3"/>
-      <c r="G139" s="3" t="s">
+      <c r="E139" s="2"/>
+      <c r="F139" s="2"/>
+      <c r="G139" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H139" s="3" t="s">
+      <c r="H139" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I139" s="3"/>
-      <c r="J139" s="3" t="s">
+      <c r="I139" s="2"/>
+      <c r="J139" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K139" s="3"/>
-      <c r="L139" s="3"/>
-      <c r="M139" s="3"/>
-      <c r="N139" s="3"/>
-      <c r="O139" s="3" t="s">
-        <v>3544</v>
-      </c>
-      <c r="P139" s="3" t="s">
+      <c r="K139" s="2"/>
+      <c r="L139" s="2"/>
+      <c r="M139" s="2"/>
+      <c r="N139" s="2"/>
+      <c r="O139" s="2" t="s">
+        <v>3543</v>
+      </c>
+      <c r="P139" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q139" s="3"/>
-      <c r="R139" s="3"/>
-      <c r="S139" s="3"/>
-      <c r="T139" s="3">
+      <c r="Q139" s="2"/>
+      <c r="R139" s="2"/>
+      <c r="S139" s="2"/>
+      <c r="T139" s="2">
         <v>0</v>
       </c>
-      <c r="U139" s="3" t="s">
+      <c r="U139" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V139" s="3" t="str">
+      <c r="V139" s="2" t="str">
         <f>VLOOKUP(U139,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W139" s="3" t="s">
+      <c r="W139" s="2" t="s">
         <v>2695</v>
       </c>
-      <c r="X139" s="3" t="str">
+      <c r="X139" s="2" t="str">
         <f>VLOOKUP(W139,clasificador!A$1:B$1635,2,0)</f>
         <v>2.5. 4  3. 1  1: IMPUESTOS</v>
       </c>
-      <c r="Y139" s="3">
+      <c r="Y139" s="2">
         <v>31</v>
       </c>
-      <c r="Z139" s="3" t="s">
+      <c r="Z139" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AA139" s="3">
+      <c r="AA139" s="2">
         <v>44.7</v>
       </c>
-      <c r="AB139" s="4">
+      <c r="AB139" s="3">
         <v>45687.69734953704</v>
       </c>
     </row>
     <row r="140" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A140" s="3" t="s">
+      <c r="A140" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B140" s="3">
+      <c r="B140" s="2">
         <v>119</v>
       </c>
-      <c r="C140" s="3"/>
-      <c r="D140" s="3" t="s">
+      <c r="C140" s="2"/>
+      <c r="D140" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E140" s="3"/>
-      <c r="F140" s="3"/>
-      <c r="G140" s="3" t="s">
+      <c r="E140" s="2"/>
+      <c r="F140" s="2"/>
+      <c r="G140" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H140" s="3" t="s">
+      <c r="H140" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I140" s="3">
+      <c r="I140" s="2">
         <v>284</v>
       </c>
-      <c r="J140" s="3" t="s">
+      <c r="J140" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K140" s="3"/>
-      <c r="L140" s="3"/>
-      <c r="M140" s="3"/>
-      <c r="N140" s="3"/>
-      <c r="O140" s="3" t="s">
-        <v>3544</v>
-      </c>
-      <c r="P140" s="3" t="s">
+      <c r="K140" s="2"/>
+      <c r="L140" s="2"/>
+      <c r="M140" s="2"/>
+      <c r="N140" s="2"/>
+      <c r="O140" s="2" t="s">
+        <v>3543</v>
+      </c>
+      <c r="P140" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q140" s="3"/>
-      <c r="R140" s="3"/>
-      <c r="S140" s="3"/>
-      <c r="T140" s="3">
+      <c r="Q140" s="2"/>
+      <c r="R140" s="2"/>
+      <c r="S140" s="2"/>
+      <c r="T140" s="2">
         <v>0</v>
       </c>
-      <c r="U140" s="3" t="s">
+      <c r="U140" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V140" s="3" t="str">
+      <c r="V140" s="2" t="str">
         <f>VLOOKUP(U140,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W140" s="3" t="s">
+      <c r="W140" s="2" t="s">
         <v>2699</v>
       </c>
-      <c r="X140" s="3" t="str">
+      <c r="X140" s="2" t="str">
         <f>VLOOKUP(W140,clasificador!A$1:B$1635,2,0)</f>
         <v>2.5. 4  3. 2  1: DERECHOS ADMINISTRATIVOS</v>
       </c>
-      <c r="Y140" s="3">
+      <c r="Y140" s="2">
         <v>31</v>
       </c>
-      <c r="Z140" s="3" t="s">
+      <c r="Z140" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AA140" s="3">
+      <c r="AA140" s="2">
         <v>67836.240000000005</v>
       </c>
-      <c r="AB140" s="4">
+      <c r="AB140" s="3">
         <v>45687.69734953704</v>
       </c>
     </row>
     <row r="141" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A141" s="3" t="s">
+      <c r="A141" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B141" s="3">
+      <c r="B141" s="2">
         <v>246</v>
       </c>
-      <c r="C141" s="3"/>
-      <c r="D141" s="3" t="s">
+      <c r="C141" s="2"/>
+      <c r="D141" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E141" s="3"/>
-      <c r="F141" s="3"/>
-      <c r="G141" s="3" t="s">
+      <c r="E141" s="2"/>
+      <c r="F141" s="2"/>
+      <c r="G141" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H141" s="3" t="s">
+      <c r="H141" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I141" s="3">
+      <c r="I141" s="2">
         <v>368</v>
       </c>
-      <c r="J141" s="3" t="s">
+      <c r="J141" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="K141" s="3"/>
-      <c r="L141" s="3"/>
-      <c r="M141" s="3"/>
-      <c r="N141" s="3"/>
-      <c r="O141" s="3" t="s">
-        <v>3545</v>
-      </c>
-      <c r="P141" s="3" t="s">
+      <c r="K141" s="2"/>
+      <c r="L141" s="2"/>
+      <c r="M141" s="2"/>
+      <c r="N141" s="2"/>
+      <c r="O141" s="2" t="s">
+        <v>3544</v>
+      </c>
+      <c r="P141" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q141" s="3"/>
-      <c r="R141" s="3"/>
-      <c r="S141" s="3"/>
-      <c r="T141" s="3">
+      <c r="Q141" s="2"/>
+      <c r="R141" s="2"/>
+      <c r="S141" s="2"/>
+      <c r="T141" s="2">
         <v>0</v>
       </c>
-      <c r="U141" s="3" t="s">
+      <c r="U141" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V141" s="3" t="str">
+      <c r="V141" s="2" t="str">
         <f>VLOOKUP(U141,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W141" s="3" t="s">
+      <c r="W141" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X141" s="3" t="str">
+      <c r="X141" s="2" t="str">
         <f>VLOOKUP(W141,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y141" s="3">
+      <c r="Y141" s="2">
         <v>64</v>
       </c>
-      <c r="Z141" s="3" t="s">
+      <c r="Z141" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="AA141" s="3">
+      <c r="AA141" s="2">
         <v>29164.32</v>
       </c>
-      <c r="AB141" s="4">
+      <c r="AB141" s="3">
         <v>45694.69734953704</v>
       </c>
     </row>
     <row r="142" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A142" s="3" t="s">
+      <c r="A142" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B142" s="3">
+      <c r="B142" s="2">
         <v>246</v>
       </c>
-      <c r="C142" s="3"/>
-      <c r="D142" s="3" t="s">
+      <c r="C142" s="2"/>
+      <c r="D142" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E142" s="3"/>
-      <c r="F142" s="3"/>
-      <c r="G142" s="3" t="s">
+      <c r="E142" s="2"/>
+      <c r="F142" s="2"/>
+      <c r="G142" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H142" s="3" t="s">
+      <c r="H142" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I142" s="3">
+      <c r="I142" s="2">
         <v>368</v>
       </c>
-      <c r="J142" s="3" t="s">
+      <c r="J142" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="K142" s="3"/>
-      <c r="L142" s="3"/>
-      <c r="M142" s="3"/>
-      <c r="N142" s="3"/>
-      <c r="O142" s="3" t="s">
-        <v>3545</v>
-      </c>
-      <c r="P142" s="3" t="s">
+      <c r="K142" s="2"/>
+      <c r="L142" s="2"/>
+      <c r="M142" s="2"/>
+      <c r="N142" s="2"/>
+      <c r="O142" s="2" t="s">
+        <v>3544</v>
+      </c>
+      <c r="P142" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q142" s="3"/>
-      <c r="R142" s="3"/>
-      <c r="S142" s="3"/>
-      <c r="T142" s="3">
+      <c r="Q142" s="2"/>
+      <c r="R142" s="2"/>
+      <c r="S142" s="2"/>
+      <c r="T142" s="2">
         <v>0</v>
       </c>
-      <c r="U142" s="3" t="s">
+      <c r="U142" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V142" s="3" t="str">
+      <c r="V142" s="2" t="str">
         <f>VLOOKUP(U142,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W142" s="3" t="s">
+      <c r="W142" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X142" s="3" t="str">
+      <c r="X142" s="2" t="str">
         <f>VLOOKUP(W142,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y142" s="3">
+      <c r="Y142" s="2">
         <v>64</v>
       </c>
-      <c r="Z142" s="3" t="s">
+      <c r="Z142" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="AA142" s="3">
+      <c r="AA142" s="2">
         <v>7763.28</v>
       </c>
-      <c r="AB142" s="4">
+      <c r="AB142" s="3">
         <v>45694.69734953704</v>
       </c>
     </row>
     <row r="143" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A143" s="3" t="s">
+      <c r="A143" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B143" s="3">
+      <c r="B143" s="2">
         <v>554</v>
       </c>
-      <c r="C143" s="3"/>
-      <c r="D143" s="3" t="s">
+      <c r="C143" s="2"/>
+      <c r="D143" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E143" s="3"/>
-      <c r="F143" s="3"/>
-      <c r="G143" s="3" t="s">
+      <c r="E143" s="2"/>
+      <c r="F143" s="2"/>
+      <c r="G143" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H143" s="3" t="s">
+      <c r="H143" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I143" s="3">
+      <c r="I143" s="2">
         <v>368</v>
       </c>
-      <c r="J143" s="3" t="s">
+      <c r="J143" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="K143" s="3"/>
-      <c r="L143" s="3"/>
-      <c r="M143" s="3"/>
-      <c r="N143" s="3"/>
-      <c r="O143" s="3" t="s">
-        <v>3546</v>
-      </c>
-      <c r="P143" s="3" t="s">
+      <c r="K143" s="2"/>
+      <c r="L143" s="2"/>
+      <c r="M143" s="2"/>
+      <c r="N143" s="2"/>
+      <c r="O143" s="2" t="s">
+        <v>3545</v>
+      </c>
+      <c r="P143" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q143" s="3"/>
-      <c r="R143" s="3"/>
-      <c r="S143" s="3"/>
-      <c r="T143" s="3">
+      <c r="Q143" s="2"/>
+      <c r="R143" s="2"/>
+      <c r="S143" s="2"/>
+      <c r="T143" s="2">
         <v>0</v>
       </c>
-      <c r="U143" s="3" t="s">
+      <c r="U143" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V143" s="3" t="str">
+      <c r="V143" s="2" t="str">
         <f>VLOOKUP(U143,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W143" s="3" t="s">
+      <c r="W143" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X143" s="3" t="str">
+      <c r="X143" s="2" t="str">
         <f>VLOOKUP(W143,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y143" s="3">
+      <c r="Y143" s="2">
         <v>64</v>
       </c>
-      <c r="Z143" s="3" t="s">
+      <c r="Z143" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="AA143" s="3">
+      <c r="AA143" s="2">
         <v>131434.19</v>
       </c>
-      <c r="AB143" s="4">
+      <c r="AB143" s="3">
         <v>45716.697349849535</v>
       </c>
     </row>
     <row r="144" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A144" s="3" t="s">
+      <c r="A144" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B144" s="3">
+      <c r="B144" s="2">
         <v>554</v>
       </c>
-      <c r="C144" s="3"/>
-      <c r="D144" s="3" t="s">
+      <c r="C144" s="2"/>
+      <c r="D144" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E144" s="3"/>
-      <c r="F144" s="3"/>
-      <c r="G144" s="3" t="s">
+      <c r="E144" s="2"/>
+      <c r="F144" s="2"/>
+      <c r="G144" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H144" s="3" t="s">
+      <c r="H144" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I144" s="3">
+      <c r="I144" s="2">
         <v>368</v>
       </c>
-      <c r="J144" s="3" t="s">
+      <c r="J144" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="K144" s="3"/>
-      <c r="L144" s="3"/>
-      <c r="M144" s="3"/>
-      <c r="N144" s="3"/>
-      <c r="O144" s="3" t="s">
-        <v>3546</v>
-      </c>
-      <c r="P144" s="3" t="s">
+      <c r="K144" s="2"/>
+      <c r="L144" s="2"/>
+      <c r="M144" s="2"/>
+      <c r="N144" s="2"/>
+      <c r="O144" s="2" t="s">
+        <v>3545</v>
+      </c>
+      <c r="P144" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q144" s="3"/>
-      <c r="R144" s="3"/>
-      <c r="S144" s="3"/>
-      <c r="T144" s="3">
+      <c r="Q144" s="2"/>
+      <c r="R144" s="2"/>
+      <c r="S144" s="2"/>
+      <c r="T144" s="2">
         <v>0</v>
       </c>
-      <c r="U144" s="3" t="s">
+      <c r="U144" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V144" s="3" t="str">
+      <c r="V144" s="2" t="str">
         <f>VLOOKUP(U144,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W144" s="3" t="s">
+      <c r="W144" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X144" s="3" t="str">
+      <c r="X144" s="2" t="str">
         <f>VLOOKUP(W144,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y144" s="3">
+      <c r="Y144" s="2">
         <v>64</v>
       </c>
-      <c r="Z144" s="3" t="s">
+      <c r="Z144" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="AA144" s="3">
+      <c r="AA144" s="2">
         <v>30652.27</v>
       </c>
-      <c r="AB144" s="4">
+      <c r="AB144" s="3">
         <v>45716.697349849535</v>
       </c>
     </row>
     <row r="145" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A145" s="3" t="s">
+      <c r="A145" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B145" s="3">
+      <c r="B145" s="2">
         <v>210</v>
       </c>
-      <c r="C145" s="3"/>
-      <c r="D145" s="3" t="s">
+      <c r="C145" s="2"/>
+      <c r="D145" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E145" s="3"/>
-      <c r="F145" s="3"/>
-      <c r="G145" s="3" t="s">
+      <c r="E145" s="2"/>
+      <c r="F145" s="2"/>
+      <c r="G145" s="2" t="s">
+        <v>3532</v>
+      </c>
+      <c r="H145" s="2" t="s">
         <v>3533</v>
       </c>
-      <c r="H145" s="3" t="s">
-        <v>3534</v>
-      </c>
-      <c r="I145" s="3"/>
-      <c r="J145" s="3" t="s">
-        <v>3537</v>
-      </c>
-      <c r="K145" s="3"/>
-      <c r="L145" s="3"/>
-      <c r="M145" s="3"/>
-      <c r="N145" s="3"/>
-      <c r="O145" s="3" t="s">
-        <v>3547</v>
-      </c>
-      <c r="P145" s="3" t="s">
+      <c r="I145" s="2"/>
+      <c r="J145" s="2" t="s">
+        <v>3536</v>
+      </c>
+      <c r="K145" s="2"/>
+      <c r="L145" s="2"/>
+      <c r="M145" s="2"/>
+      <c r="N145" s="2"/>
+      <c r="O145" s="2" t="s">
+        <v>3546</v>
+      </c>
+      <c r="P145" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q145" s="3"/>
-      <c r="R145" s="3"/>
-      <c r="S145" s="3"/>
-      <c r="T145" s="3">
+      <c r="Q145" s="2"/>
+      <c r="R145" s="2"/>
+      <c r="S145" s="2"/>
+      <c r="T145" s="2">
         <v>9</v>
       </c>
-      <c r="U145" s="3" t="s">
+      <c r="U145" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="V145" s="3" t="str">
+      <c r="V145" s="2" t="str">
         <f>VLOOKUP(U145,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">09: RECURSOS DIRECTAMENTE RECAUDADOS                                                                                                                      </v>
       </c>
-      <c r="W145" s="3" t="s">
+      <c r="W145" s="2" t="s">
         <v>2657</v>
       </c>
-      <c r="X145" s="3" t="str">
+      <c r="X145" s="2" t="str">
         <f>VLOOKUP(W145,clasificador!A$1:B$1635,2,0)</f>
         <v>2.5. 3  1. 1  1: A ESTUDIANTES</v>
       </c>
-      <c r="Y145" s="3">
+      <c r="Y145" s="2">
         <v>67</v>
       </c>
-      <c r="Z145" s="3" t="s">
+      <c r="Z145" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="AA145" s="3">
+      <c r="AA145" s="2">
         <v>38940</v>
       </c>
-      <c r="AB145" s="4">
+      <c r="AB145" s="3">
         <v>45698.69734953704</v>
       </c>
     </row>
     <row r="146" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A146" s="3" t="s">
+      <c r="A146" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B146" s="3">
+      <c r="B146" s="2">
         <v>233</v>
       </c>
-      <c r="C146" s="3"/>
-      <c r="D146" s="3" t="s">
+      <c r="C146" s="2"/>
+      <c r="D146" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E146" s="3"/>
-      <c r="F146" s="3"/>
-      <c r="G146" s="3" t="s">
+      <c r="E146" s="2"/>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H146" s="3" t="s">
+      <c r="H146" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I146" s="3">
+      <c r="I146" s="2">
         <v>362</v>
       </c>
-      <c r="J146" s="3" t="s">
-        <v>3538</v>
-      </c>
-      <c r="K146" s="3"/>
-      <c r="L146" s="3"/>
-      <c r="M146" s="3"/>
-      <c r="N146" s="3"/>
-      <c r="O146" s="3" t="s">
-        <v>3548</v>
-      </c>
-      <c r="P146" s="3" t="s">
+      <c r="J146" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K146" s="2"/>
+      <c r="L146" s="2"/>
+      <c r="M146" s="2"/>
+      <c r="N146" s="2"/>
+      <c r="O146" s="2" t="s">
+        <v>3547</v>
+      </c>
+      <c r="P146" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q146" s="3"/>
-      <c r="R146" s="3"/>
-      <c r="S146" s="3"/>
-      <c r="T146" s="3">
+      <c r="Q146" s="2"/>
+      <c r="R146" s="2"/>
+      <c r="S146" s="2"/>
+      <c r="T146" s="2">
         <v>0</v>
       </c>
-      <c r="U146" s="3" t="s">
+      <c r="U146" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V146" s="3" t="str">
+      <c r="V146" s="2" t="str">
         <f>VLOOKUP(U146,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W146" s="3" t="s">
+      <c r="W146" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X146" s="3" t="str">
+      <c r="X146" s="2" t="str">
         <f>VLOOKUP(W146,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y146" s="3">
+      <c r="Y146" s="2">
         <v>63</v>
       </c>
-      <c r="Z146" s="3" t="s">
-        <v>3566</v>
-      </c>
-      <c r="AA146" s="3">
+      <c r="Z146" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA146" s="2">
         <v>54892.11</v>
       </c>
-      <c r="AB146" s="4">
+      <c r="AB146" s="3">
         <v>45699.69734953704</v>
       </c>
     </row>
     <row r="147" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A147" s="3" t="s">
+      <c r="A147" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B147" s="3">
+      <c r="B147" s="2">
         <v>233</v>
       </c>
-      <c r="C147" s="3"/>
-      <c r="D147" s="3" t="s">
+      <c r="C147" s="2"/>
+      <c r="D147" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E147" s="3"/>
-      <c r="F147" s="3"/>
-      <c r="G147" s="3" t="s">
+      <c r="E147" s="2"/>
+      <c r="F147" s="2"/>
+      <c r="G147" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H147" s="3" t="s">
+      <c r="H147" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I147" s="3">
+      <c r="I147" s="2">
         <v>362</v>
       </c>
-      <c r="J147" s="3" t="s">
-        <v>3538</v>
-      </c>
-      <c r="K147" s="3"/>
-      <c r="L147" s="3"/>
-      <c r="M147" s="3"/>
-      <c r="N147" s="3"/>
-      <c r="O147" s="3" t="s">
-        <v>3548</v>
-      </c>
-      <c r="P147" s="3" t="s">
+      <c r="J147" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K147" s="2"/>
+      <c r="L147" s="2"/>
+      <c r="M147" s="2"/>
+      <c r="N147" s="2"/>
+      <c r="O147" s="2" t="s">
+        <v>3547</v>
+      </c>
+      <c r="P147" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q147" s="3"/>
-      <c r="R147" s="3"/>
-      <c r="S147" s="3"/>
-      <c r="T147" s="3">
+      <c r="Q147" s="2"/>
+      <c r="R147" s="2"/>
+      <c r="S147" s="2"/>
+      <c r="T147" s="2">
         <v>0</v>
       </c>
-      <c r="U147" s="3" t="s">
+      <c r="U147" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V147" s="3" t="str">
+      <c r="V147" s="2" t="str">
         <f>VLOOKUP(U147,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W147" s="3" t="s">
+      <c r="W147" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X147" s="3" t="str">
+      <c r="X147" s="2" t="str">
         <f>VLOOKUP(W147,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y147" s="3">
+      <c r="Y147" s="2">
         <v>63</v>
       </c>
-      <c r="Z147" s="3" t="s">
-        <v>3566</v>
-      </c>
-      <c r="AA147" s="3">
+      <c r="Z147" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA147" s="2">
         <v>12871.08</v>
       </c>
-      <c r="AB147" s="4">
+      <c r="AB147" s="3">
         <v>45699.69734953704</v>
       </c>
     </row>
     <row r="148" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A148" s="3" t="s">
+      <c r="A148" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B148" s="3">
+      <c r="B148" s="2">
         <v>522</v>
       </c>
-      <c r="C148" s="3"/>
-      <c r="D148" s="3" t="s">
+      <c r="C148" s="2"/>
+      <c r="D148" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E148" s="3"/>
-      <c r="F148" s="3"/>
-      <c r="G148" s="3" t="s">
+      <c r="E148" s="2"/>
+      <c r="F148" s="2"/>
+      <c r="G148" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H148" s="3" t="s">
+      <c r="H148" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I148" s="3">
+      <c r="I148" s="2">
         <v>362</v>
       </c>
-      <c r="J148" s="3" t="s">
-        <v>3538</v>
-      </c>
-      <c r="K148" s="3"/>
-      <c r="L148" s="3"/>
-      <c r="M148" s="3"/>
-      <c r="N148" s="3"/>
-      <c r="O148" s="3" t="s">
-        <v>3549</v>
-      </c>
-      <c r="P148" s="3" t="s">
+      <c r="J148" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K148" s="2"/>
+      <c r="L148" s="2"/>
+      <c r="M148" s="2"/>
+      <c r="N148" s="2"/>
+      <c r="O148" s="2" t="s">
+        <v>3548</v>
+      </c>
+      <c r="P148" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q148" s="3"/>
-      <c r="R148" s="3"/>
-      <c r="S148" s="3"/>
-      <c r="T148" s="3">
+      <c r="Q148" s="2"/>
+      <c r="R148" s="2"/>
+      <c r="S148" s="2"/>
+      <c r="T148" s="2">
         <v>0</v>
       </c>
-      <c r="U148" s="3" t="s">
+      <c r="U148" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V148" s="3" t="str">
+      <c r="V148" s="2" t="str">
         <f>VLOOKUP(U148,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W148" s="3" t="s">
+      <c r="W148" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X148" s="3" t="str">
+      <c r="X148" s="2" t="str">
         <f>VLOOKUP(W148,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y148" s="3">
+      <c r="Y148" s="2">
         <v>63</v>
       </c>
-      <c r="Z148" s="3" t="s">
-        <v>3566</v>
-      </c>
-      <c r="AA148" s="3">
+      <c r="Z148" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA148" s="2">
         <v>5201.99</v>
       </c>
-      <c r="AB148" s="4">
+      <c r="AB148" s="3">
         <v>45714.69734953704</v>
       </c>
     </row>
     <row r="149" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A149" s="3" t="s">
+      <c r="A149" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B149" s="3">
+      <c r="B149" s="2">
         <v>522</v>
       </c>
-      <c r="C149" s="3"/>
-      <c r="D149" s="3" t="s">
+      <c r="C149" s="2"/>
+      <c r="D149" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E149" s="3"/>
-      <c r="F149" s="3"/>
-      <c r="G149" s="3" t="s">
+      <c r="E149" s="2"/>
+      <c r="F149" s="2"/>
+      <c r="G149" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H149" s="3" t="s">
+      <c r="H149" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I149" s="3">
+      <c r="I149" s="2">
         <v>362</v>
       </c>
-      <c r="J149" s="3" t="s">
-        <v>3538</v>
-      </c>
-      <c r="K149" s="3"/>
-      <c r="L149" s="3"/>
-      <c r="M149" s="3"/>
-      <c r="N149" s="3"/>
-      <c r="O149" s="3" t="s">
-        <v>3549</v>
-      </c>
-      <c r="P149" s="3" t="s">
+      <c r="J149" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K149" s="2"/>
+      <c r="L149" s="2"/>
+      <c r="M149" s="2"/>
+      <c r="N149" s="2"/>
+      <c r="O149" s="2" t="s">
+        <v>3548</v>
+      </c>
+      <c r="P149" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q149" s="3"/>
-      <c r="R149" s="3"/>
-      <c r="S149" s="3"/>
-      <c r="T149" s="3">
+      <c r="Q149" s="2"/>
+      <c r="R149" s="2"/>
+      <c r="S149" s="2"/>
+      <c r="T149" s="2">
         <v>0</v>
       </c>
-      <c r="U149" s="3" t="s">
+      <c r="U149" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V149" s="3" t="str">
+      <c r="V149" s="2" t="str">
         <f>VLOOKUP(U149,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W149" s="3" t="s">
+      <c r="W149" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X149" s="3" t="str">
+      <c r="X149" s="2" t="str">
         <f>VLOOKUP(W149,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y149" s="3">
+      <c r="Y149" s="2">
         <v>63</v>
       </c>
-      <c r="Z149" s="3" t="s">
-        <v>3566</v>
-      </c>
-      <c r="AA149" s="3">
+      <c r="Z149" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA149" s="2">
         <v>446.69</v>
       </c>
-      <c r="AB149" s="4">
+      <c r="AB149" s="3">
         <v>45714.69734953704</v>
       </c>
     </row>
     <row r="150" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A150" s="3" t="s">
+      <c r="A150" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B150" s="3">
+      <c r="B150" s="2">
         <v>523</v>
       </c>
-      <c r="C150" s="3"/>
-      <c r="D150" s="3" t="s">
+      <c r="C150" s="2"/>
+      <c r="D150" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E150" s="3"/>
-      <c r="F150" s="3"/>
-      <c r="G150" s="3" t="s">
+      <c r="E150" s="2"/>
+      <c r="F150" s="2"/>
+      <c r="G150" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H150" s="3" t="s">
+      <c r="H150" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I150" s="3">
+      <c r="I150" s="2">
         <v>362</v>
       </c>
-      <c r="J150" s="3" t="s">
-        <v>3538</v>
-      </c>
-      <c r="K150" s="3"/>
-      <c r="L150" s="3"/>
-      <c r="M150" s="3"/>
-      <c r="N150" s="3"/>
-      <c r="O150" s="3" t="s">
-        <v>3550</v>
-      </c>
-      <c r="P150" s="3" t="s">
+      <c r="J150" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K150" s="2"/>
+      <c r="L150" s="2"/>
+      <c r="M150" s="2"/>
+      <c r="N150" s="2"/>
+      <c r="O150" s="2" t="s">
+        <v>3549</v>
+      </c>
+      <c r="P150" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q150" s="3"/>
-      <c r="R150" s="3"/>
-      <c r="S150" s="3"/>
-      <c r="T150" s="3">
+      <c r="Q150" s="2"/>
+      <c r="R150" s="2"/>
+      <c r="S150" s="2"/>
+      <c r="T150" s="2">
         <v>0</v>
       </c>
-      <c r="U150" s="3" t="s">
+      <c r="U150" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V150" s="3" t="str">
+      <c r="V150" s="2" t="str">
         <f>VLOOKUP(U150,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W150" s="3" t="s">
+      <c r="W150" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X150" s="3" t="str">
+      <c r="X150" s="2" t="str">
         <f>VLOOKUP(W150,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y150" s="3">
+      <c r="Y150" s="2">
         <v>63</v>
       </c>
-      <c r="Z150" s="3" t="s">
-        <v>3566</v>
-      </c>
-      <c r="AA150" s="3">
+      <c r="Z150" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA150" s="2">
         <v>10286.459999999999</v>
       </c>
-      <c r="AB150" s="4">
+      <c r="AB150" s="3">
         <v>45714.69734953704</v>
       </c>
     </row>
     <row r="151" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A151" s="3" t="s">
+      <c r="A151" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B151" s="3">
+      <c r="B151" s="2">
         <v>523</v>
       </c>
-      <c r="C151" s="3"/>
-      <c r="D151" s="3" t="s">
+      <c r="C151" s="2"/>
+      <c r="D151" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E151" s="3"/>
-      <c r="F151" s="3"/>
-      <c r="G151" s="3" t="s">
+      <c r="E151" s="2"/>
+      <c r="F151" s="2"/>
+      <c r="G151" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H151" s="3" t="s">
+      <c r="H151" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I151" s="3">
+      <c r="I151" s="2">
         <v>362</v>
       </c>
-      <c r="J151" s="3" t="s">
-        <v>3538</v>
-      </c>
-      <c r="K151" s="3"/>
-      <c r="L151" s="3"/>
-      <c r="M151" s="3"/>
-      <c r="N151" s="3"/>
-      <c r="O151" s="3" t="s">
-        <v>3550</v>
-      </c>
-      <c r="P151" s="3" t="s">
+      <c r="J151" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K151" s="2"/>
+      <c r="L151" s="2"/>
+      <c r="M151" s="2"/>
+      <c r="N151" s="2"/>
+      <c r="O151" s="2" t="s">
+        <v>3549</v>
+      </c>
+      <c r="P151" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q151" s="3"/>
-      <c r="R151" s="3"/>
-      <c r="S151" s="3"/>
-      <c r="T151" s="3">
+      <c r="Q151" s="2"/>
+      <c r="R151" s="2"/>
+      <c r="S151" s="2"/>
+      <c r="T151" s="2">
         <v>0</v>
       </c>
-      <c r="U151" s="3" t="s">
+      <c r="U151" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V151" s="3" t="str">
+      <c r="V151" s="2" t="str">
         <f>VLOOKUP(U151,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W151" s="3" t="s">
+      <c r="W151" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X151" s="3" t="str">
+      <c r="X151" s="2" t="str">
         <f>VLOOKUP(W151,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y151" s="3">
+      <c r="Y151" s="2">
         <v>63</v>
       </c>
-      <c r="Z151" s="3" t="s">
-        <v>3566</v>
-      </c>
-      <c r="AA151" s="3">
+      <c r="Z151" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA151" s="2">
         <v>312.25</v>
       </c>
-      <c r="AB151" s="4">
+      <c r="AB151" s="3">
         <v>45714.69734953704</v>
       </c>
     </row>
     <row r="152" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A152" s="3" t="s">
+      <c r="A152" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B152" s="3">
+      <c r="B152" s="2">
         <v>524</v>
       </c>
-      <c r="C152" s="3"/>
-      <c r="D152" s="3" t="s">
+      <c r="C152" s="2"/>
+      <c r="D152" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E152" s="3"/>
-      <c r="F152" s="3"/>
-      <c r="G152" s="3" t="s">
+      <c r="E152" s="2"/>
+      <c r="F152" s="2"/>
+      <c r="G152" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H152" s="3" t="s">
+      <c r="H152" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I152" s="3">
+      <c r="I152" s="2">
         <v>362</v>
       </c>
-      <c r="J152" s="3" t="s">
-        <v>3538</v>
-      </c>
-      <c r="K152" s="3"/>
-      <c r="L152" s="3"/>
-      <c r="M152" s="3"/>
-      <c r="N152" s="3"/>
-      <c r="O152" s="3" t="s">
-        <v>3551</v>
-      </c>
-      <c r="P152" s="3" t="s">
+      <c r="J152" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K152" s="2"/>
+      <c r="L152" s="2"/>
+      <c r="M152" s="2"/>
+      <c r="N152" s="2"/>
+      <c r="O152" s="2" t="s">
+        <v>3550</v>
+      </c>
+      <c r="P152" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q152" s="3"/>
-      <c r="R152" s="3"/>
-      <c r="S152" s="3"/>
-      <c r="T152" s="3">
+      <c r="Q152" s="2"/>
+      <c r="R152" s="2"/>
+      <c r="S152" s="2"/>
+      <c r="T152" s="2">
         <v>0</v>
       </c>
-      <c r="U152" s="3" t="s">
+      <c r="U152" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V152" s="3" t="str">
+      <c r="V152" s="2" t="str">
         <f>VLOOKUP(U152,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W152" s="3" t="s">
+      <c r="W152" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X152" s="3" t="str">
+      <c r="X152" s="2" t="str">
         <f>VLOOKUP(W152,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y152" s="3">
+      <c r="Y152" s="2">
         <v>63</v>
       </c>
-      <c r="Z152" s="3" t="s">
-        <v>3566</v>
-      </c>
-      <c r="AA152" s="3">
+      <c r="Z152" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA152" s="2">
         <v>1163.76</v>
       </c>
-      <c r="AB152" s="4">
+      <c r="AB152" s="3">
         <v>45714.69734953704</v>
       </c>
     </row>
     <row r="153" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A153" s="3" t="s">
+      <c r="A153" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B153" s="3">
+      <c r="B153" s="2">
         <v>524</v>
       </c>
-      <c r="C153" s="3"/>
-      <c r="D153" s="3" t="s">
+      <c r="C153" s="2"/>
+      <c r="D153" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E153" s="3"/>
-      <c r="F153" s="3"/>
-      <c r="G153" s="3" t="s">
+      <c r="E153" s="2"/>
+      <c r="F153" s="2"/>
+      <c r="G153" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H153" s="3" t="s">
+      <c r="H153" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I153" s="3">
+      <c r="I153" s="2">
         <v>362</v>
       </c>
-      <c r="J153" s="3" t="s">
-        <v>3538</v>
-      </c>
-      <c r="K153" s="3"/>
-      <c r="L153" s="3"/>
-      <c r="M153" s="3"/>
-      <c r="N153" s="3"/>
-      <c r="O153" s="3" t="s">
-        <v>3551</v>
-      </c>
-      <c r="P153" s="3" t="s">
+      <c r="J153" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K153" s="2"/>
+      <c r="L153" s="2"/>
+      <c r="M153" s="2"/>
+      <c r="N153" s="2"/>
+      <c r="O153" s="2" t="s">
+        <v>3550</v>
+      </c>
+      <c r="P153" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q153" s="3"/>
-      <c r="R153" s="3"/>
-      <c r="S153" s="3"/>
-      <c r="T153" s="3">
+      <c r="Q153" s="2"/>
+      <c r="R153" s="2"/>
+      <c r="S153" s="2"/>
+      <c r="T153" s="2">
         <v>0</v>
       </c>
-      <c r="U153" s="3" t="s">
+      <c r="U153" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V153" s="3" t="str">
+      <c r="V153" s="2" t="str">
         <f>VLOOKUP(U153,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W153" s="3" t="s">
+      <c r="W153" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X153" s="3" t="str">
+      <c r="X153" s="2" t="str">
         <f>VLOOKUP(W153,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y153" s="3">
+      <c r="Y153" s="2">
         <v>63</v>
       </c>
-      <c r="Z153" s="3" t="s">
-        <v>3566</v>
-      </c>
-      <c r="AA153" s="3">
+      <c r="Z153" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA153" s="2">
         <v>112.7</v>
       </c>
-      <c r="AB153" s="4">
+      <c r="AB153" s="3">
         <v>45714.69734953704</v>
       </c>
     </row>
     <row r="154" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A154" s="3" t="s">
+      <c r="A154" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B154" s="3">
+      <c r="B154" s="2">
         <v>525</v>
       </c>
-      <c r="C154" s="3"/>
-      <c r="D154" s="3" t="s">
+      <c r="C154" s="2"/>
+      <c r="D154" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E154" s="3"/>
-      <c r="F154" s="3"/>
-      <c r="G154" s="3" t="s">
+      <c r="E154" s="2"/>
+      <c r="F154" s="2"/>
+      <c r="G154" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H154" s="3" t="s">
+      <c r="H154" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I154" s="3">
+      <c r="I154" s="2">
         <v>362</v>
       </c>
-      <c r="J154" s="3" t="s">
-        <v>3538</v>
-      </c>
-      <c r="K154" s="3"/>
-      <c r="L154" s="3"/>
-      <c r="M154" s="3"/>
-      <c r="N154" s="3"/>
-      <c r="O154" s="3" t="s">
-        <v>3552</v>
-      </c>
-      <c r="P154" s="3" t="s">
+      <c r="J154" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K154" s="2"/>
+      <c r="L154" s="2"/>
+      <c r="M154" s="2"/>
+      <c r="N154" s="2"/>
+      <c r="O154" s="2" t="s">
+        <v>3551</v>
+      </c>
+      <c r="P154" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q154" s="3"/>
-      <c r="R154" s="3"/>
-      <c r="S154" s="3"/>
-      <c r="T154" s="3">
+      <c r="Q154" s="2"/>
+      <c r="R154" s="2"/>
+      <c r="S154" s="2"/>
+      <c r="T154" s="2">
         <v>0</v>
       </c>
-      <c r="U154" s="3" t="s">
+      <c r="U154" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V154" s="3" t="str">
+      <c r="V154" s="2" t="str">
         <f>VLOOKUP(U154,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W154" s="3" t="s">
+      <c r="W154" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X154" s="3" t="str">
+      <c r="X154" s="2" t="str">
         <f>VLOOKUP(W154,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y154" s="3">
+      <c r="Y154" s="2">
         <v>63</v>
       </c>
-      <c r="Z154" s="3" t="s">
-        <v>3566</v>
-      </c>
-      <c r="AA154" s="3">
+      <c r="Z154" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA154" s="2">
         <v>7663.6</v>
       </c>
-      <c r="AB154" s="4">
+      <c r="AB154" s="3">
         <v>45714.69734953704</v>
       </c>
     </row>
     <row r="155" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A155" s="3" t="s">
+      <c r="A155" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B155" s="3">
+      <c r="B155" s="2">
         <v>525</v>
       </c>
-      <c r="C155" s="3"/>
-      <c r="D155" s="3" t="s">
+      <c r="C155" s="2"/>
+      <c r="D155" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E155" s="3"/>
-      <c r="F155" s="3"/>
-      <c r="G155" s="3" t="s">
+      <c r="E155" s="2"/>
+      <c r="F155" s="2"/>
+      <c r="G155" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H155" s="3" t="s">
+      <c r="H155" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I155" s="3">
+      <c r="I155" s="2">
         <v>362</v>
       </c>
-      <c r="J155" s="3" t="s">
-        <v>3538</v>
-      </c>
-      <c r="K155" s="3"/>
-      <c r="L155" s="3"/>
-      <c r="M155" s="3"/>
-      <c r="N155" s="3"/>
-      <c r="O155" s="3" t="s">
-        <v>3552</v>
-      </c>
-      <c r="P155" s="3" t="s">
+      <c r="J155" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K155" s="2"/>
+      <c r="L155" s="2"/>
+      <c r="M155" s="2"/>
+      <c r="N155" s="2"/>
+      <c r="O155" s="2" t="s">
+        <v>3551</v>
+      </c>
+      <c r="P155" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q155" s="3"/>
-      <c r="R155" s="3"/>
-      <c r="S155" s="3"/>
-      <c r="T155" s="3">
+      <c r="Q155" s="2"/>
+      <c r="R155" s="2"/>
+      <c r="S155" s="2"/>
+      <c r="T155" s="2">
         <v>0</v>
       </c>
-      <c r="U155" s="3" t="s">
+      <c r="U155" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V155" s="3" t="str">
+      <c r="V155" s="2" t="str">
         <f>VLOOKUP(U155,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W155" s="3" t="s">
+      <c r="W155" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X155" s="3" t="str">
+      <c r="X155" s="2" t="str">
         <f>VLOOKUP(W155,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y155" s="3">
+      <c r="Y155" s="2">
         <v>63</v>
       </c>
-      <c r="Z155" s="3" t="s">
-        <v>3566</v>
-      </c>
-      <c r="AA155" s="3">
+      <c r="Z155" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA155" s="2">
         <v>1913.38</v>
       </c>
-      <c r="AB155" s="4">
+      <c r="AB155" s="3">
         <v>45714.69734953704</v>
       </c>
     </row>
     <row r="156" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A156" s="3" t="s">
+      <c r="A156" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B156" s="3">
+      <c r="B156" s="2">
         <v>526</v>
       </c>
-      <c r="C156" s="3"/>
-      <c r="D156" s="3" t="s">
+      <c r="C156" s="2"/>
+      <c r="D156" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E156" s="3"/>
-      <c r="F156" s="3"/>
-      <c r="G156" s="3" t="s">
+      <c r="E156" s="2"/>
+      <c r="F156" s="2"/>
+      <c r="G156" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H156" s="3" t="s">
+      <c r="H156" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I156" s="3">
+      <c r="I156" s="2">
         <v>362</v>
       </c>
-      <c r="J156" s="3" t="s">
-        <v>3538</v>
-      </c>
-      <c r="K156" s="3"/>
-      <c r="L156" s="3"/>
-      <c r="M156" s="3"/>
-      <c r="N156" s="3"/>
-      <c r="O156" s="3" t="s">
-        <v>3553</v>
-      </c>
-      <c r="P156" s="3" t="s">
+      <c r="J156" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K156" s="2"/>
+      <c r="L156" s="2"/>
+      <c r="M156" s="2"/>
+      <c r="N156" s="2"/>
+      <c r="O156" s="2" t="s">
+        <v>3552</v>
+      </c>
+      <c r="P156" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q156" s="3"/>
-      <c r="R156" s="3"/>
-      <c r="S156" s="3"/>
-      <c r="T156" s="3">
+      <c r="Q156" s="2"/>
+      <c r="R156" s="2"/>
+      <c r="S156" s="2"/>
+      <c r="T156" s="2">
         <v>0</v>
       </c>
-      <c r="U156" s="3" t="s">
+      <c r="U156" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V156" s="3" t="str">
+      <c r="V156" s="2" t="str">
         <f>VLOOKUP(U156,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W156" s="3" t="s">
+      <c r="W156" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X156" s="3" t="str">
+      <c r="X156" s="2" t="str">
         <f>VLOOKUP(W156,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y156" s="3">
+      <c r="Y156" s="2">
         <v>63</v>
       </c>
-      <c r="Z156" s="3" t="s">
-        <v>3566</v>
-      </c>
-      <c r="AA156" s="3">
+      <c r="Z156" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA156" s="2">
         <v>5266.27</v>
       </c>
-      <c r="AB156" s="4">
+      <c r="AB156" s="3">
         <v>45714.69734953704</v>
       </c>
     </row>
     <row r="157" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A157" s="3" t="s">
+      <c r="A157" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B157" s="3">
+      <c r="B157" s="2">
         <v>526</v>
       </c>
-      <c r="C157" s="3"/>
-      <c r="D157" s="3" t="s">
+      <c r="C157" s="2"/>
+      <c r="D157" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E157" s="3"/>
-      <c r="F157" s="3"/>
-      <c r="G157" s="3" t="s">
+      <c r="E157" s="2"/>
+      <c r="F157" s="2"/>
+      <c r="G157" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H157" s="3" t="s">
+      <c r="H157" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I157" s="3">
+      <c r="I157" s="2">
         <v>362</v>
       </c>
-      <c r="J157" s="3" t="s">
-        <v>3538</v>
-      </c>
-      <c r="K157" s="3"/>
-      <c r="L157" s="3"/>
-      <c r="M157" s="3"/>
-      <c r="N157" s="3"/>
-      <c r="O157" s="3" t="s">
-        <v>3553</v>
-      </c>
-      <c r="P157" s="3" t="s">
+      <c r="J157" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K157" s="2"/>
+      <c r="L157" s="2"/>
+      <c r="M157" s="2"/>
+      <c r="N157" s="2"/>
+      <c r="O157" s="2" t="s">
+        <v>3552</v>
+      </c>
+      <c r="P157" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q157" s="3"/>
-      <c r="R157" s="3"/>
-      <c r="S157" s="3"/>
-      <c r="T157" s="3">
+      <c r="Q157" s="2"/>
+      <c r="R157" s="2"/>
+      <c r="S157" s="2"/>
+      <c r="T157" s="2">
         <v>0</v>
       </c>
-      <c r="U157" s="3" t="s">
+      <c r="U157" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V157" s="3" t="str">
+      <c r="V157" s="2" t="str">
         <f>VLOOKUP(U157,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W157" s="3" t="s">
+      <c r="W157" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X157" s="3" t="str">
+      <c r="X157" s="2" t="str">
         <f>VLOOKUP(W157,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y157" s="3">
+      <c r="Y157" s="2">
         <v>63</v>
       </c>
-      <c r="Z157" s="3" t="s">
-        <v>3566</v>
-      </c>
-      <c r="AA157" s="3">
+      <c r="Z157" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA157" s="2">
         <v>9807.02</v>
       </c>
-      <c r="AB157" s="4">
+      <c r="AB157" s="3">
         <v>45714.69734953704</v>
       </c>
     </row>
     <row r="158" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A158" s="3" t="s">
+      <c r="A158" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B158" s="3">
+      <c r="B158" s="2">
         <v>571</v>
       </c>
-      <c r="C158" s="3"/>
-      <c r="D158" s="3" t="s">
+      <c r="C158" s="2"/>
+      <c r="D158" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E158" s="3"/>
-      <c r="F158" s="3"/>
-      <c r="G158" s="3" t="s">
+      <c r="E158" s="2"/>
+      <c r="F158" s="2"/>
+      <c r="G158" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H158" s="3" t="s">
+      <c r="H158" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I158" s="3">
+      <c r="I158" s="2">
         <v>362</v>
       </c>
-      <c r="J158" s="3" t="s">
-        <v>3538</v>
-      </c>
-      <c r="K158" s="3"/>
-      <c r="L158" s="3"/>
-      <c r="M158" s="3"/>
-      <c r="N158" s="3"/>
-      <c r="O158" s="3" t="s">
-        <v>3554</v>
-      </c>
-      <c r="P158" s="3" t="s">
+      <c r="J158" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K158" s="2"/>
+      <c r="L158" s="2"/>
+      <c r="M158" s="2"/>
+      <c r="N158" s="2"/>
+      <c r="O158" s="2" t="s">
+        <v>3553</v>
+      </c>
+      <c r="P158" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q158" s="3"/>
-      <c r="R158" s="3"/>
-      <c r="S158" s="3"/>
-      <c r="T158" s="3">
+      <c r="Q158" s="2"/>
+      <c r="R158" s="2"/>
+      <c r="S158" s="2"/>
+      <c r="T158" s="2">
         <v>0</v>
       </c>
-      <c r="U158" s="3" t="s">
+      <c r="U158" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V158" s="3" t="str">
+      <c r="V158" s="2" t="str">
         <f>VLOOKUP(U158,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W158" s="3" t="s">
+      <c r="W158" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X158" s="3" t="str">
+      <c r="X158" s="2" t="str">
         <f>VLOOKUP(W158,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y158" s="3">
+      <c r="Y158" s="2">
         <v>63</v>
       </c>
-      <c r="Z158" s="3" t="s">
-        <v>3566</v>
-      </c>
-      <c r="AA158" s="3">
+      <c r="Z158" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA158" s="2">
         <v>257917.62</v>
       </c>
-      <c r="AB158" s="4">
+      <c r="AB158" s="3">
         <v>45716.697349849535</v>
       </c>
     </row>
     <row r="159" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A159" s="3" t="s">
+      <c r="A159" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B159" s="3">
+      <c r="B159" s="2">
         <v>571</v>
       </c>
-      <c r="C159" s="3"/>
-      <c r="D159" s="3" t="s">
+      <c r="C159" s="2"/>
+      <c r="D159" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E159" s="3"/>
-      <c r="F159" s="3"/>
-      <c r="G159" s="3" t="s">
+      <c r="E159" s="2"/>
+      <c r="F159" s="2"/>
+      <c r="G159" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H159" s="3" t="s">
+      <c r="H159" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I159" s="3">
+      <c r="I159" s="2">
         <v>362</v>
       </c>
-      <c r="J159" s="3" t="s">
-        <v>3538</v>
-      </c>
-      <c r="K159" s="3"/>
-      <c r="L159" s="3"/>
-      <c r="M159" s="3"/>
-      <c r="N159" s="3"/>
-      <c r="O159" s="3" t="s">
-        <v>3554</v>
-      </c>
-      <c r="P159" s="3" t="s">
+      <c r="J159" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K159" s="2"/>
+      <c r="L159" s="2"/>
+      <c r="M159" s="2"/>
+      <c r="N159" s="2"/>
+      <c r="O159" s="2" t="s">
+        <v>3553</v>
+      </c>
+      <c r="P159" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q159" s="3"/>
-      <c r="R159" s="3"/>
-      <c r="S159" s="3"/>
-      <c r="T159" s="3">
+      <c r="Q159" s="2"/>
+      <c r="R159" s="2"/>
+      <c r="S159" s="2"/>
+      <c r="T159" s="2">
         <v>0</v>
       </c>
-      <c r="U159" s="3" t="s">
+      <c r="U159" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V159" s="3" t="str">
+      <c r="V159" s="2" t="str">
         <f>VLOOKUP(U159,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W159" s="3" t="s">
+      <c r="W159" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X159" s="3" t="str">
+      <c r="X159" s="2" t="str">
         <f>VLOOKUP(W159,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y159" s="3">
+      <c r="Y159" s="2">
         <v>63</v>
       </c>
-      <c r="Z159" s="3" t="s">
-        <v>3566</v>
-      </c>
-      <c r="AA159" s="3">
+      <c r="Z159" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA159" s="2">
         <v>55123.31</v>
       </c>
-      <c r="AB159" s="4">
+      <c r="AB159" s="3">
         <v>45716.697349849535</v>
       </c>
     </row>
     <row r="160" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A160" s="3" t="s">
+      <c r="A160" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B160" s="3">
+      <c r="B160" s="2">
         <v>582</v>
       </c>
-      <c r="C160" s="3"/>
-      <c r="D160" s="3" t="s">
+      <c r="C160" s="2"/>
+      <c r="D160" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E160" s="3"/>
-      <c r="F160" s="3"/>
-      <c r="G160" s="3" t="s">
+      <c r="E160" s="2"/>
+      <c r="F160" s="2"/>
+      <c r="G160" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H160" s="3" t="s">
+      <c r="H160" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I160" s="3">
+      <c r="I160" s="2">
         <v>362</v>
       </c>
-      <c r="J160" s="3" t="s">
-        <v>3538</v>
-      </c>
-      <c r="K160" s="3"/>
-      <c r="L160" s="3"/>
-      <c r="M160" s="3"/>
-      <c r="N160" s="3"/>
-      <c r="O160" s="3" t="s">
-        <v>3555</v>
-      </c>
-      <c r="P160" s="3" t="s">
+      <c r="J160" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K160" s="2"/>
+      <c r="L160" s="2"/>
+      <c r="M160" s="2"/>
+      <c r="N160" s="2"/>
+      <c r="O160" s="2" t="s">
+        <v>3554</v>
+      </c>
+      <c r="P160" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q160" s="3"/>
-      <c r="R160" s="3"/>
-      <c r="S160" s="3"/>
-      <c r="T160" s="3">
+      <c r="Q160" s="2"/>
+      <c r="R160" s="2"/>
+      <c r="S160" s="2"/>
+      <c r="T160" s="2">
         <v>0</v>
       </c>
-      <c r="U160" s="3" t="s">
+      <c r="U160" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V160" s="3" t="str">
+      <c r="V160" s="2" t="str">
         <f>VLOOKUP(U160,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W160" s="3" t="s">
+      <c r="W160" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X160" s="3" t="str">
+      <c r="X160" s="2" t="str">
         <f>VLOOKUP(W160,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y160" s="3">
+      <c r="Y160" s="2">
         <v>63</v>
       </c>
-      <c r="Z160" s="3" t="s">
-        <v>3566</v>
-      </c>
-      <c r="AA160" s="3">
+      <c r="Z160" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA160" s="2">
         <v>67617.5</v>
       </c>
-      <c r="AB160" s="4">
+      <c r="AB160" s="3">
         <v>45716.697349849535</v>
       </c>
     </row>
     <row r="161" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A161" s="3" t="s">
+      <c r="A161" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B161" s="3">
+      <c r="B161" s="2">
         <v>582</v>
       </c>
-      <c r="C161" s="3"/>
-      <c r="D161" s="3" t="s">
+      <c r="C161" s="2"/>
+      <c r="D161" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E161" s="3"/>
-      <c r="F161" s="3"/>
-      <c r="G161" s="3" t="s">
+      <c r="E161" s="2"/>
+      <c r="F161" s="2"/>
+      <c r="G161" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H161" s="3" t="s">
+      <c r="H161" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I161" s="3">
+      <c r="I161" s="2">
         <v>362</v>
       </c>
-      <c r="J161" s="3" t="s">
-        <v>3538</v>
-      </c>
-      <c r="K161" s="3"/>
-      <c r="L161" s="3"/>
-      <c r="M161" s="3"/>
-      <c r="N161" s="3"/>
-      <c r="O161" s="3" t="s">
-        <v>3555</v>
-      </c>
-      <c r="P161" s="3" t="s">
+      <c r="J161" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="K161" s="2"/>
+      <c r="L161" s="2"/>
+      <c r="M161" s="2"/>
+      <c r="N161" s="2"/>
+      <c r="O161" s="2" t="s">
+        <v>3554</v>
+      </c>
+      <c r="P161" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q161" s="3"/>
-      <c r="R161" s="3"/>
-      <c r="S161" s="3"/>
-      <c r="T161" s="3">
+      <c r="Q161" s="2"/>
+      <c r="R161" s="2"/>
+      <c r="S161" s="2"/>
+      <c r="T161" s="2">
         <v>0</v>
       </c>
-      <c r="U161" s="3" t="s">
+      <c r="U161" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V161" s="3" t="str">
+      <c r="V161" s="2" t="str">
         <f>VLOOKUP(U161,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W161" s="3" t="s">
+      <c r="W161" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X161" s="3" t="str">
+      <c r="X161" s="2" t="str">
         <f>VLOOKUP(W161,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y161" s="3">
+      <c r="Y161" s="2">
         <v>63</v>
       </c>
-      <c r="Z161" s="3" t="s">
-        <v>3566</v>
-      </c>
-      <c r="AA161" s="3">
+      <c r="Z161" s="2" t="s">
+        <v>3565</v>
+      </c>
+      <c r="AA161" s="2">
         <v>15767.5</v>
       </c>
-      <c r="AB161" s="4">
+      <c r="AB161" s="3">
         <v>45716.697349849535</v>
       </c>
     </row>
     <row r="162" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A162" s="3" t="s">
+      <c r="A162" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B162" s="3">
+      <c r="B162" s="2">
         <v>225</v>
       </c>
-      <c r="C162" s="3"/>
-      <c r="D162" s="3" t="s">
+      <c r="C162" s="2"/>
+      <c r="D162" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E162" s="3"/>
-      <c r="F162" s="3"/>
-      <c r="G162" s="3" t="s">
+      <c r="E162" s="2"/>
+      <c r="F162" s="2"/>
+      <c r="G162" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H162" s="3" t="s">
+      <c r="H162" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I162" s="3">
+      <c r="I162" s="2">
         <v>362</v>
       </c>
-      <c r="J162" s="3" t="s">
-        <v>3535</v>
-      </c>
-      <c r="K162" s="3"/>
-      <c r="L162" s="3"/>
-      <c r="M162" s="3"/>
-      <c r="N162" s="3"/>
-      <c r="O162" s="3" t="s">
-        <v>3556</v>
-      </c>
-      <c r="P162" s="3" t="s">
+      <c r="J162" s="2" t="s">
+        <v>3534</v>
+      </c>
+      <c r="K162" s="2"/>
+      <c r="L162" s="2"/>
+      <c r="M162" s="2"/>
+      <c r="N162" s="2"/>
+      <c r="O162" s="2" t="s">
+        <v>3555</v>
+      </c>
+      <c r="P162" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q162" s="3"/>
-      <c r="R162" s="3"/>
-      <c r="S162" s="3"/>
-      <c r="T162" s="3">
+      <c r="Q162" s="2"/>
+      <c r="R162" s="2"/>
+      <c r="S162" s="2"/>
+      <c r="T162" s="2">
         <v>0</v>
       </c>
-      <c r="U162" s="3" t="s">
+      <c r="U162" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V162" s="3" t="str">
+      <c r="V162" s="2" t="str">
         <f>VLOOKUP(U162,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W162" s="3" t="s">
+      <c r="W162" s="2" t="s">
         <v>2679</v>
       </c>
-      <c r="X162" s="3" t="str">
+      <c r="X162" s="2" t="str">
         <f>VLOOKUP(W162,clasificador!A$1:B$1635,2,0)</f>
         <v>2.5. 4  1. 3  1: MULTAS</v>
       </c>
-      <c r="Y162" s="3">
+      <c r="Y162" s="2">
         <v>31</v>
       </c>
-      <c r="Z162" s="3" t="s">
+      <c r="Z162" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AA162" s="3">
+      <c r="AA162" s="2">
         <v>1162.79</v>
       </c>
-      <c r="AB162" s="4">
+      <c r="AB162" s="3">
         <v>45693.428518518522</v>
       </c>
     </row>
     <row r="163" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A163" s="3" t="s">
+      <c r="A163" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B163" s="3">
+      <c r="B163" s="2">
         <v>247</v>
       </c>
-      <c r="C163" s="3"/>
-      <c r="D163" s="3" t="s">
+      <c r="C163" s="2"/>
+      <c r="D163" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E163" s="3"/>
-      <c r="F163" s="3"/>
-      <c r="G163" s="3" t="s">
+      <c r="E163" s="2"/>
+      <c r="F163" s="2"/>
+      <c r="G163" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H163" s="3" t="s">
+      <c r="H163" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I163" s="3"/>
-      <c r="J163" s="3" t="s">
-        <v>3539</v>
-      </c>
-      <c r="K163" s="3"/>
-      <c r="L163" s="3"/>
-      <c r="M163" s="3"/>
-      <c r="N163" s="3"/>
-      <c r="O163" s="3" t="s">
-        <v>3557</v>
-      </c>
-      <c r="P163" s="3" t="s">
+      <c r="I163" s="2"/>
+      <c r="J163" s="2" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K163" s="2"/>
+      <c r="L163" s="2"/>
+      <c r="M163" s="2"/>
+      <c r="N163" s="2"/>
+      <c r="O163" s="2" t="s">
+        <v>3556</v>
+      </c>
+      <c r="P163" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q163" s="3"/>
-      <c r="R163" s="3"/>
-      <c r="S163" s="3"/>
-      <c r="T163" s="3">
+      <c r="Q163" s="2"/>
+      <c r="R163" s="2"/>
+      <c r="S163" s="2"/>
+      <c r="T163" s="2">
         <v>9</v>
       </c>
-      <c r="U163" s="3" t="s">
+      <c r="U163" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="V163" s="3" t="str">
+      <c r="V163" s="2" t="str">
         <f>VLOOKUP(U163,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">09: RECURSOS DIRECTAMENTE RECAUDADOS                                                                                                                      </v>
       </c>
-      <c r="W163" s="3" t="s">
+      <c r="W163" s="2" t="s">
         <v>2135</v>
       </c>
-      <c r="X163" s="3" t="str">
+      <c r="X163" s="2" t="str">
         <f>VLOOKUP(W163,clasificador!A$1:B$1635,2,0)</f>
         <v>2.3. 2  1. 2 99: OTROS GASTOS</v>
       </c>
-      <c r="Y163" s="3">
+      <c r="Y163" s="2">
         <v>24</v>
       </c>
-      <c r="Z163" s="3" t="s">
+      <c r="Z163" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AA163" s="3">
+      <c r="AA163" s="2">
         <v>221931.16</v>
       </c>
-      <c r="AB163" s="4">
+      <c r="AB163" s="3">
         <v>45695.428518518522</v>
       </c>
     </row>
     <row r="164" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A164" s="3" t="s">
+      <c r="A164" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B164" s="3">
+      <c r="B164" s="2">
         <v>247</v>
       </c>
-      <c r="C164" s="3"/>
-      <c r="D164" s="3" t="s">
+      <c r="C164" s="2"/>
+      <c r="D164" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E164" s="3"/>
-      <c r="F164" s="3"/>
-      <c r="G164" s="3" t="s">
+      <c r="E164" s="2"/>
+      <c r="F164" s="2"/>
+      <c r="G164" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H164" s="3" t="s">
+      <c r="H164" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I164" s="3"/>
-      <c r="J164" s="3" t="s">
-        <v>3539</v>
-      </c>
-      <c r="K164" s="3"/>
-      <c r="L164" s="3"/>
-      <c r="M164" s="3"/>
-      <c r="N164" s="3"/>
-      <c r="O164" s="3" t="s">
-        <v>3557</v>
-      </c>
-      <c r="P164" s="3" t="s">
+      <c r="I164" s="2"/>
+      <c r="J164" s="2" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K164" s="2"/>
+      <c r="L164" s="2"/>
+      <c r="M164" s="2"/>
+      <c r="N164" s="2"/>
+      <c r="O164" s="2" t="s">
+        <v>3556</v>
+      </c>
+      <c r="P164" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q164" s="3"/>
-      <c r="R164" s="3"/>
-      <c r="S164" s="3"/>
-      <c r="T164" s="3">
+      <c r="Q164" s="2"/>
+      <c r="R164" s="2"/>
+      <c r="S164" s="2"/>
+      <c r="T164" s="2">
         <v>9</v>
       </c>
-      <c r="U164" s="3" t="s">
+      <c r="U164" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="V164" s="3" t="str">
+      <c r="V164" s="2" t="str">
         <f>VLOOKUP(U164,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">09: RECURSOS DIRECTAMENTE RECAUDADOS                                                                                                                      </v>
       </c>
-      <c r="W164" s="3" t="s">
+      <c r="W164" s="2" t="s">
         <v>2135</v>
       </c>
-      <c r="X164" s="3" t="str">
+      <c r="X164" s="2" t="str">
         <f>VLOOKUP(W164,clasificador!A$1:B$1635,2,0)</f>
         <v>2.3. 2  1. 2 99: OTROS GASTOS</v>
       </c>
-      <c r="Y164" s="3">
+      <c r="Y164" s="2">
         <v>24</v>
       </c>
-      <c r="Z164" s="3" t="s">
+      <c r="Z164" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AA164" s="3">
+      <c r="AA164" s="2">
         <v>2161.84</v>
       </c>
-      <c r="AB164" s="4">
+      <c r="AB164" s="3">
         <v>45695.428518518522</v>
       </c>
     </row>
     <row r="165" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A165" s="3" t="s">
+      <c r="A165" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B165" s="3">
+      <c r="B165" s="2">
         <v>507</v>
       </c>
-      <c r="C165" s="3"/>
-      <c r="D165" s="3" t="s">
+      <c r="C165" s="2"/>
+      <c r="D165" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E165" s="3"/>
-      <c r="F165" s="3"/>
-      <c r="G165" s="3" t="s">
+      <c r="E165" s="2"/>
+      <c r="F165" s="2"/>
+      <c r="G165" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H165" s="3" t="s">
+      <c r="H165" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I165" s="3"/>
-      <c r="J165" s="3" t="s">
-        <v>3539</v>
-      </c>
-      <c r="K165" s="3"/>
-      <c r="L165" s="3"/>
-      <c r="M165" s="3"/>
-      <c r="N165" s="3"/>
-      <c r="O165" s="3" t="s">
-        <v>3558</v>
-      </c>
-      <c r="P165" s="3" t="s">
+      <c r="I165" s="2"/>
+      <c r="J165" s="2" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K165" s="2"/>
+      <c r="L165" s="2"/>
+      <c r="M165" s="2"/>
+      <c r="N165" s="2"/>
+      <c r="O165" s="2" t="s">
+        <v>3557</v>
+      </c>
+      <c r="P165" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q165" s="3"/>
-      <c r="R165" s="3"/>
-      <c r="S165" s="3"/>
-      <c r="T165" s="3">
+      <c r="Q165" s="2"/>
+      <c r="R165" s="2"/>
+      <c r="S165" s="2"/>
+      <c r="T165" s="2">
         <v>9</v>
       </c>
-      <c r="U165" s="3" t="s">
+      <c r="U165" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="V165" s="3" t="str">
+      <c r="V165" s="2" t="str">
         <f>VLOOKUP(U165,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">09: RECURSOS DIRECTAMENTE RECAUDADOS                                                                                                                      </v>
       </c>
-      <c r="W165" s="3" t="s">
+      <c r="W165" s="2" t="s">
         <v>2135</v>
       </c>
-      <c r="X165" s="3" t="str">
+      <c r="X165" s="2" t="str">
         <f>VLOOKUP(W165,clasificador!A$1:B$1635,2,0)</f>
         <v>2.3. 2  1. 2 99: OTROS GASTOS</v>
       </c>
-      <c r="Y165" s="3">
+      <c r="Y165" s="2">
         <v>24</v>
       </c>
-      <c r="Z165" s="3" t="s">
+      <c r="Z165" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AA165" s="3">
+      <c r="AA165" s="2">
         <v>221743.31</v>
       </c>
-      <c r="AB165" s="4">
+      <c r="AB165" s="3">
         <v>45715.42851597222</v>
       </c>
     </row>
     <row r="166" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A166" s="3" t="s">
+      <c r="A166" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B166" s="3">
+      <c r="B166" s="2">
         <v>507</v>
       </c>
-      <c r="C166" s="3"/>
-      <c r="D166" s="3" t="s">
+      <c r="C166" s="2"/>
+      <c r="D166" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E166" s="3"/>
-      <c r="F166" s="3"/>
-      <c r="G166" s="3" t="s">
+      <c r="E166" s="2"/>
+      <c r="F166" s="2"/>
+      <c r="G166" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H166" s="3" t="s">
+      <c r="H166" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I166" s="3"/>
-      <c r="J166" s="3" t="s">
-        <v>3539</v>
-      </c>
-      <c r="K166" s="3"/>
-      <c r="L166" s="3"/>
-      <c r="M166" s="3"/>
-      <c r="N166" s="3"/>
-      <c r="O166" s="3" t="s">
-        <v>3558</v>
-      </c>
-      <c r="P166" s="3" t="s">
+      <c r="I166" s="2"/>
+      <c r="J166" s="2" t="s">
+        <v>3538</v>
+      </c>
+      <c r="K166" s="2"/>
+      <c r="L166" s="2"/>
+      <c r="M166" s="2"/>
+      <c r="N166" s="2"/>
+      <c r="O166" s="2" t="s">
+        <v>3557</v>
+      </c>
+      <c r="P166" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q166" s="3"/>
-      <c r="R166" s="3"/>
-      <c r="S166" s="3"/>
-      <c r="T166" s="3">
+      <c r="Q166" s="2"/>
+      <c r="R166" s="2"/>
+      <c r="S166" s="2"/>
+      <c r="T166" s="2">
         <v>9</v>
       </c>
-      <c r="U166" s="3" t="s">
+      <c r="U166" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="V166" s="3" t="str">
+      <c r="V166" s="2" t="str">
         <f>VLOOKUP(U166,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">09: RECURSOS DIRECTAMENTE RECAUDADOS                                                                                                                      </v>
       </c>
-      <c r="W166" s="3" t="s">
+      <c r="W166" s="2" t="s">
         <v>2135</v>
       </c>
-      <c r="X166" s="3" t="str">
+      <c r="X166" s="2" t="str">
         <f>VLOOKUP(W166,clasificador!A$1:B$1635,2,0)</f>
         <v>2.3. 2  1. 2 99: OTROS GASTOS</v>
       </c>
-      <c r="Y166" s="3">
+      <c r="Y166" s="2">
         <v>24</v>
       </c>
-      <c r="Z166" s="3" t="s">
+      <c r="Z166" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AA166" s="3">
+      <c r="AA166" s="2">
         <v>2419.69</v>
       </c>
-      <c r="AB166" s="4">
+      <c r="AB166" s="3">
         <v>45715.42851597222</v>
       </c>
     </row>
     <row r="167" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A167" s="3" t="s">
+      <c r="A167" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B167" s="3">
+      <c r="B167" s="2">
         <v>327</v>
       </c>
-      <c r="C167" s="3"/>
-      <c r="D167" s="3" t="s">
+      <c r="C167" s="2"/>
+      <c r="D167" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E167" s="3"/>
-      <c r="F167" s="3"/>
-      <c r="G167" s="3" t="s">
+      <c r="E167" s="2"/>
+      <c r="F167" s="2"/>
+      <c r="G167" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H167" s="3" t="s">
+      <c r="H167" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I167" s="3">
+      <c r="I167" s="2">
         <v>196</v>
       </c>
-      <c r="J167" s="3" t="s">
-        <v>3540</v>
-      </c>
-      <c r="K167" s="3"/>
-      <c r="L167" s="3"/>
-      <c r="M167" s="3"/>
-      <c r="N167" s="3"/>
-      <c r="O167" s="3" t="s">
-        <v>3559</v>
-      </c>
-      <c r="P167" s="3" t="s">
+      <c r="J167" s="2" t="s">
+        <v>3539</v>
+      </c>
+      <c r="K167" s="2"/>
+      <c r="L167" s="2"/>
+      <c r="M167" s="2"/>
+      <c r="N167" s="2"/>
+      <c r="O167" s="2" t="s">
+        <v>3558</v>
+      </c>
+      <c r="P167" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q167" s="3"/>
-      <c r="R167" s="3"/>
-      <c r="S167" s="3"/>
-      <c r="T167" s="3">
+      <c r="Q167" s="2"/>
+      <c r="R167" s="2"/>
+      <c r="S167" s="2"/>
+      <c r="T167" s="2">
         <v>0</v>
       </c>
-      <c r="U167" s="3" t="s">
+      <c r="U167" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V167" s="3" t="str">
+      <c r="V167" s="2" t="str">
         <f>VLOOKUP(U167,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W167" s="3" t="s">
+      <c r="W167" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="X167" s="3" t="str">
+      <c r="X167" s="2" t="str">
         <f>VLOOKUP(W167,clasificador!A$1:B$1635,2,0)</f>
         <v>2.3. 2  1. 2  1: PASAJES Y GASTOS DE TRANSPORTE</v>
       </c>
-      <c r="Y167" s="3">
+      <c r="Y167" s="2">
         <v>22</v>
       </c>
-      <c r="Z167" s="3" t="s">
+      <c r="Z167" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AA167" s="3">
+      <c r="AA167" s="2">
         <v>90</v>
       </c>
-      <c r="AB167" s="4">
+      <c r="AB167" s="3">
         <v>45702.520452280092</v>
       </c>
     </row>
     <row r="168" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A168" s="3" t="s">
+      <c r="A168" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B168" s="3">
+      <c r="B168" s="2">
         <v>346</v>
       </c>
-      <c r="C168" s="3"/>
-      <c r="D168" s="3" t="s">
+      <c r="C168" s="2"/>
+      <c r="D168" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E168" s="3"/>
-      <c r="F168" s="3"/>
-      <c r="G168" s="3" t="s">
+      <c r="E168" s="2"/>
+      <c r="F168" s="2"/>
+      <c r="G168" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H168" s="3" t="s">
+      <c r="H168" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I168" s="3"/>
-      <c r="J168" s="3" t="s">
-        <v>3541</v>
-      </c>
-      <c r="K168" s="3"/>
-      <c r="L168" s="3"/>
-      <c r="M168" s="3"/>
-      <c r="N168" s="3"/>
-      <c r="O168" s="3" t="s">
-        <v>3560</v>
-      </c>
-      <c r="P168" s="3" t="s">
+      <c r="I168" s="2"/>
+      <c r="J168" s="2" t="s">
+        <v>3540</v>
+      </c>
+      <c r="K168" s="2"/>
+      <c r="L168" s="2"/>
+      <c r="M168" s="2"/>
+      <c r="N168" s="2"/>
+      <c r="O168" s="2" t="s">
+        <v>3559</v>
+      </c>
+      <c r="P168" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q168" s="3"/>
-      <c r="R168" s="3"/>
-      <c r="S168" s="3"/>
-      <c r="T168" s="3">
+      <c r="Q168" s="2"/>
+      <c r="R168" s="2"/>
+      <c r="S168" s="2"/>
+      <c r="T168" s="2">
         <v>0</v>
       </c>
-      <c r="U168" s="3" t="s">
+      <c r="U168" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V168" s="3" t="str">
+      <c r="V168" s="2" t="str">
         <f>VLOOKUP(U168,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W168" s="3" t="s">
+      <c r="W168" s="2" t="s">
         <v>2517</v>
       </c>
-      <c r="X168" s="3" t="str">
+      <c r="X168" s="2" t="str">
         <f>VLOOKUP(W168,clasificador!A$1:B$1635,2,0)</f>
         <v>2.4. 1  3. 1  1: A OTRAS UNIDADES DEL GOBIERNO NACIONAL</v>
       </c>
-      <c r="Y168" s="3">
+      <c r="Y168" s="2">
         <v>39</v>
       </c>
-      <c r="Z168" s="3" t="s">
+      <c r="Z168" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AA168" s="3">
+      <c r="AA168" s="2">
         <v>68270</v>
       </c>
-      <c r="AB168" s="4">
+      <c r="AB168" s="3">
         <v>45702.520452280092</v>
       </c>
     </row>
     <row r="169" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A169" s="3" t="s">
+      <c r="A169" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B169" s="3">
+      <c r="B169" s="2">
         <v>347</v>
       </c>
-      <c r="C169" s="3"/>
-      <c r="D169" s="3" t="s">
+      <c r="C169" s="2"/>
+      <c r="D169" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E169" s="3"/>
-      <c r="F169" s="3"/>
-      <c r="G169" s="3" t="s">
+      <c r="E169" s="2"/>
+      <c r="F169" s="2"/>
+      <c r="G169" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H169" s="3" t="s">
+      <c r="H169" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I169" s="3">
+      <c r="I169" s="2">
         <v>284</v>
       </c>
-      <c r="J169" s="3" t="s">
+      <c r="J169" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K169" s="3"/>
-      <c r="L169" s="3"/>
-      <c r="M169" s="3"/>
-      <c r="N169" s="3"/>
-      <c r="O169" s="3" t="s">
-        <v>3561</v>
-      </c>
-      <c r="P169" s="3" t="s">
+      <c r="K169" s="2"/>
+      <c r="L169" s="2"/>
+      <c r="M169" s="2"/>
+      <c r="N169" s="2"/>
+      <c r="O169" s="2" t="s">
+        <v>3560</v>
+      </c>
+      <c r="P169" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q169" s="3"/>
-      <c r="R169" s="3"/>
-      <c r="S169" s="3"/>
-      <c r="T169" s="3">
+      <c r="Q169" s="2"/>
+      <c r="R169" s="2"/>
+      <c r="S169" s="2"/>
+      <c r="T169" s="2">
         <v>0</v>
       </c>
-      <c r="U169" s="3" t="s">
+      <c r="U169" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V169" s="3" t="str">
+      <c r="V169" s="2" t="str">
         <f>VLOOKUP(U169,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W169" s="3" t="s">
+      <c r="W169" s="2" t="s">
         <v>2695</v>
       </c>
-      <c r="X169" s="3" t="str">
+      <c r="X169" s="2" t="str">
         <f>VLOOKUP(W169,clasificador!A$1:B$1635,2,0)</f>
         <v>2.5. 4  3. 1  1: IMPUESTOS</v>
       </c>
-      <c r="Y169" s="3">
+      <c r="Y169" s="2">
         <v>31</v>
       </c>
-      <c r="Z169" s="3" t="s">
+      <c r="Z169" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AA169" s="3">
+      <c r="AA169" s="2">
         <v>7.5</v>
       </c>
-      <c r="AB169" s="4">
+      <c r="AB169" s="3">
         <v>45702.520452280092</v>
       </c>
     </row>
     <row r="170" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A170" s="3" t="s">
+      <c r="A170" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B170" s="3">
+      <c r="B170" s="2">
         <v>347</v>
       </c>
-      <c r="C170" s="3"/>
-      <c r="D170" s="3" t="s">
+      <c r="C170" s="2"/>
+      <c r="D170" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E170" s="3"/>
-      <c r="F170" s="3"/>
-      <c r="G170" s="3" t="s">
+      <c r="E170" s="2"/>
+      <c r="F170" s="2"/>
+      <c r="G170" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H170" s="3" t="s">
+      <c r="H170" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I170" s="3">
+      <c r="I170" s="2">
         <v>284</v>
       </c>
-      <c r="J170" s="3" t="s">
+      <c r="J170" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K170" s="3"/>
-      <c r="L170" s="3"/>
-      <c r="M170" s="3"/>
-      <c r="N170" s="3"/>
-      <c r="O170" s="3" t="s">
-        <v>3561</v>
-      </c>
-      <c r="P170" s="3" t="s">
+      <c r="K170" s="2"/>
+      <c r="L170" s="2"/>
+      <c r="M170" s="2"/>
+      <c r="N170" s="2"/>
+      <c r="O170" s="2" t="s">
+        <v>3560</v>
+      </c>
+      <c r="P170" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q170" s="3"/>
-      <c r="R170" s="3"/>
-      <c r="S170" s="3"/>
-      <c r="T170" s="3">
+      <c r="Q170" s="2"/>
+      <c r="R170" s="2"/>
+      <c r="S170" s="2"/>
+      <c r="T170" s="2">
         <v>0</v>
       </c>
-      <c r="U170" s="3" t="s">
+      <c r="U170" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V170" s="3" t="str">
+      <c r="V170" s="2" t="str">
         <f>VLOOKUP(U170,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W170" s="3" t="s">
+      <c r="W170" s="2" t="s">
         <v>2699</v>
       </c>
-      <c r="X170" s="3" t="str">
+      <c r="X170" s="2" t="str">
         <f>VLOOKUP(W170,clasificador!A$1:B$1635,2,0)</f>
         <v>2.5. 4  3. 2  1: DERECHOS ADMINISTRATIVOS</v>
       </c>
-      <c r="Y170" s="3">
+      <c r="Y170" s="2">
         <v>31</v>
       </c>
-      <c r="Z170" s="3" t="s">
+      <c r="Z170" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AA170" s="3">
+      <c r="AA170" s="2">
         <v>716.4</v>
       </c>
-      <c r="AB170" s="4">
+      <c r="AB170" s="3">
         <v>45702.520452280092</v>
       </c>
     </row>
     <row r="171" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A171" s="3" t="s">
+      <c r="A171" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B171" s="3">
+      <c r="B171" s="2">
         <v>431</v>
       </c>
-      <c r="C171" s="3"/>
-      <c r="D171" s="3" t="s">
+      <c r="C171" s="2"/>
+      <c r="D171" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E171" s="3"/>
-      <c r="F171" s="3"/>
-      <c r="G171" s="3" t="s">
+      <c r="E171" s="2"/>
+      <c r="F171" s="2"/>
+      <c r="G171" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H171" s="3" t="s">
-        <v>3532</v>
-      </c>
-      <c r="I171" s="3"/>
-      <c r="J171" s="3" t="s">
-        <v>3536</v>
-      </c>
-      <c r="K171" s="3"/>
-      <c r="L171" s="3"/>
-      <c r="M171" s="3"/>
-      <c r="N171" s="3"/>
-      <c r="O171" s="3" t="s">
-        <v>3562</v>
-      </c>
-      <c r="P171" s="3" t="s">
+      <c r="H171" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I171" s="2"/>
+      <c r="J171" s="2" t="s">
+        <v>3535</v>
+      </c>
+      <c r="K171" s="2"/>
+      <c r="L171" s="2"/>
+      <c r="M171" s="2"/>
+      <c r="N171" s="2"/>
+      <c r="O171" s="2" t="s">
+        <v>3561</v>
+      </c>
+      <c r="P171" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q171" s="3"/>
-      <c r="R171" s="3"/>
-      <c r="S171" s="3"/>
-      <c r="T171" s="3">
+      <c r="Q171" s="2"/>
+      <c r="R171" s="2"/>
+      <c r="S171" s="2"/>
+      <c r="T171" s="2">
         <v>0</v>
       </c>
-      <c r="U171" s="3" t="s">
+      <c r="U171" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V171" s="3" t="str">
+      <c r="V171" s="2" t="str">
         <f>VLOOKUP(U171,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v xml:space="preserve">00: RECURSOS ORDINARIOS                                                                                                                                   </v>
       </c>
-      <c r="W171" s="3" t="s">
+      <c r="W171" s="2" t="s">
         <v>2657</v>
       </c>
-      <c r="X171" s="3" t="str">
+      <c r="X171" s="2" t="str">
         <f>VLOOKUP(W171,clasificador!A$1:B$1635,2,0)</f>
         <v>2.5. 3  1. 1  1: A ESTUDIANTES</v>
       </c>
-      <c r="Y171" s="3">
+      <c r="Y171" s="2">
         <v>57</v>
       </c>
-      <c r="Z171" s="3" t="s">
-        <v>3565</v>
-      </c>
-      <c r="AA171" s="3">
+      <c r="Z171" s="2" t="s">
+        <v>3564</v>
+      </c>
+      <c r="AA171" s="2">
         <v>50000</v>
       </c>
-      <c r="AB171" s="4">
+      <c r="AB171" s="3">
         <v>45706.597614733793</v>
       </c>
     </row>
     <row r="172" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A172" s="3" t="s">
+      <c r="A172" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B172" s="3">
+      <c r="B172" s="2">
         <v>570</v>
       </c>
-      <c r="C172" s="3"/>
-      <c r="D172" s="3" t="s">
+      <c r="C172" s="2"/>
+      <c r="D172" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E172" s="3"/>
-      <c r="F172" s="3"/>
-      <c r="G172" s="3" t="s">
+      <c r="E172" s="2"/>
+      <c r="F172" s="2"/>
+      <c r="G172" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H172" s="3" t="s">
+      <c r="H172" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I172" s="3">
+      <c r="I172" s="2">
         <v>368</v>
       </c>
-      <c r="J172" s="3" t="s">
+      <c r="J172" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="K172" s="3"/>
-      <c r="L172" s="3"/>
-      <c r="M172" s="3"/>
-      <c r="N172" s="3"/>
-      <c r="O172" s="3" t="s">
-        <v>3563</v>
-      </c>
-      <c r="P172" s="3" t="s">
+      <c r="K172" s="2"/>
+      <c r="L172" s="2"/>
+      <c r="M172" s="2"/>
+      <c r="N172" s="2"/>
+      <c r="O172" s="2" t="s">
+        <v>3562</v>
+      </c>
+      <c r="P172" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q172" s="3"/>
-      <c r="R172" s="3"/>
-      <c r="S172" s="3"/>
-      <c r="T172" s="3">
+      <c r="Q172" s="2"/>
+      <c r="R172" s="2"/>
+      <c r="S172" s="2"/>
+      <c r="T172" s="2">
         <v>18</v>
       </c>
-      <c r="U172" s="3" t="s">
+      <c r="U172" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="V172" s="3" t="str">
+      <c r="V172" s="2" t="str">
         <f>VLOOKUP(U172,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v>18: CANON Y SOBRECANON, REGALIAS, RENTA DE ADUANAS Y PARTICIPACIONES</v>
       </c>
-      <c r="W172" s="3" t="s">
+      <c r="W172" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X172" s="3" t="str">
+      <c r="X172" s="2" t="str">
         <f>VLOOKUP(W172,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y172" s="3">
+      <c r="Y172" s="2">
         <v>64</v>
       </c>
-      <c r="Z172" s="3" t="s">
+      <c r="Z172" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="AA172" s="3">
+      <c r="AA172" s="2">
         <v>28595.64</v>
       </c>
-      <c r="AB172" s="4">
+      <c r="AB172" s="3">
         <v>45716.697349849535</v>
       </c>
     </row>
     <row r="173" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A173" s="3" t="s">
+      <c r="A173" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B173" s="3">
+      <c r="B173" s="2">
         <v>570</v>
       </c>
-      <c r="C173" s="3"/>
-      <c r="D173" s="3" t="s">
+      <c r="C173" s="2"/>
+      <c r="D173" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E173" s="3"/>
-      <c r="F173" s="3"/>
-      <c r="G173" s="3" t="s">
+      <c r="E173" s="2"/>
+      <c r="F173" s="2"/>
+      <c r="G173" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H173" s="3" t="s">
+      <c r="H173" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I173" s="3">
+      <c r="I173" s="2">
         <v>368</v>
       </c>
-      <c r="J173" s="3" t="s">
+      <c r="J173" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="K173" s="3"/>
-      <c r="L173" s="3"/>
-      <c r="M173" s="3"/>
-      <c r="N173" s="3"/>
-      <c r="O173" s="3" t="s">
-        <v>3563</v>
-      </c>
-      <c r="P173" s="3" t="s">
+      <c r="K173" s="2"/>
+      <c r="L173" s="2"/>
+      <c r="M173" s="2"/>
+      <c r="N173" s="2"/>
+      <c r="O173" s="2" t="s">
+        <v>3562</v>
+      </c>
+      <c r="P173" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q173" s="3"/>
-      <c r="R173" s="3"/>
-      <c r="S173" s="3"/>
-      <c r="T173" s="3">
+      <c r="Q173" s="2"/>
+      <c r="R173" s="2"/>
+      <c r="S173" s="2"/>
+      <c r="T173" s="2">
         <v>18</v>
       </c>
-      <c r="U173" s="3" t="s">
+      <c r="U173" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="V173" s="3" t="str">
+      <c r="V173" s="2" t="str">
         <f>VLOOKUP(U173,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v>18: CANON Y SOBRECANON, REGALIAS, RENTA DE ADUANAS Y PARTICIPACIONES</v>
       </c>
-      <c r="W173" s="3" t="s">
+      <c r="W173" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X173" s="3" t="str">
+      <c r="X173" s="2" t="str">
         <f>VLOOKUP(W173,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y173" s="3">
+      <c r="Y173" s="2">
         <v>64</v>
       </c>
-      <c r="Z173" s="3" t="s">
+      <c r="Z173" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="AA173" s="3">
+      <c r="AA173" s="2">
         <v>6766.9</v>
       </c>
-      <c r="AB173" s="4">
+      <c r="AB173" s="3">
         <v>45716.697349849535</v>
       </c>
     </row>
     <row r="174" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A174" s="3" t="s">
+      <c r="A174" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B174" s="3">
+      <c r="B174" s="2">
         <v>569</v>
       </c>
-      <c r="C174" s="3"/>
-      <c r="D174" s="3" t="s">
+      <c r="C174" s="2"/>
+      <c r="D174" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E174" s="3"/>
-      <c r="F174" s="3"/>
-      <c r="G174" s="3" t="s">
+      <c r="E174" s="2"/>
+      <c r="F174" s="2"/>
+      <c r="G174" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H174" s="3" t="s">
+      <c r="H174" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I174" s="3">
+      <c r="I174" s="2">
         <v>368</v>
       </c>
-      <c r="J174" s="3" t="s">
+      <c r="J174" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="K174" s="3"/>
-      <c r="L174" s="3"/>
-      <c r="M174" s="3"/>
-      <c r="N174" s="3"/>
-      <c r="O174" s="3" t="s">
-        <v>3564</v>
-      </c>
-      <c r="P174" s="3" t="s">
+      <c r="K174" s="2"/>
+      <c r="L174" s="2"/>
+      <c r="M174" s="2"/>
+      <c r="N174" s="2"/>
+      <c r="O174" s="2" t="s">
+        <v>3563</v>
+      </c>
+      <c r="P174" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q174" s="3"/>
-      <c r="R174" s="3"/>
-      <c r="S174" s="3"/>
-      <c r="T174" s="3">
+      <c r="Q174" s="2"/>
+      <c r="R174" s="2"/>
+      <c r="S174" s="2"/>
+      <c r="T174" s="2">
         <v>18</v>
       </c>
-      <c r="U174" s="3" t="s">
+      <c r="U174" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="V174" s="3" t="str">
+      <c r="V174" s="2" t="str">
         <f>VLOOKUP(U174,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v>18: CANON Y SOBRECANON, REGALIAS, RENTA DE ADUANAS Y PARTICIPACIONES</v>
       </c>
-      <c r="W174" s="3" t="s">
+      <c r="W174" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X174" s="3" t="str">
+      <c r="X174" s="2" t="str">
         <f>VLOOKUP(W174,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y174" s="3">
+      <c r="Y174" s="2">
         <v>69</v>
       </c>
-      <c r="Z174" s="3" t="s">
+      <c r="Z174" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="AA174" s="3">
+      <c r="AA174" s="2">
         <v>19012.62</v>
       </c>
-      <c r="AB174" s="4">
+      <c r="AB174" s="3">
         <v>45716.697349849535</v>
       </c>
     </row>
     <row r="175" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A175" s="3" t="s">
+      <c r="A175" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B175" s="3">
+      <c r="B175" s="2">
         <v>569</v>
       </c>
-      <c r="C175" s="3"/>
-      <c r="D175" s="3" t="s">
+      <c r="C175" s="2"/>
+      <c r="D175" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E175" s="3"/>
-      <c r="F175" s="3"/>
-      <c r="G175" s="3" t="s">
+      <c r="E175" s="2"/>
+      <c r="F175" s="2"/>
+      <c r="G175" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H175" s="3" t="s">
+      <c r="H175" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I175" s="3">
+      <c r="I175" s="2">
         <v>368</v>
       </c>
-      <c r="J175" s="3" t="s">
+      <c r="J175" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="K175" s="3"/>
-      <c r="L175" s="3"/>
-      <c r="M175" s="3"/>
-      <c r="N175" s="3"/>
-      <c r="O175" s="3" t="s">
-        <v>3564</v>
-      </c>
-      <c r="P175" s="3" t="s">
+      <c r="K175" s="2"/>
+      <c r="L175" s="2"/>
+      <c r="M175" s="2"/>
+      <c r="N175" s="2"/>
+      <c r="O175" s="2" t="s">
+        <v>3563</v>
+      </c>
+      <c r="P175" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q175" s="3"/>
-      <c r="R175" s="3"/>
-      <c r="S175" s="3"/>
-      <c r="T175" s="3">
+      <c r="Q175" s="2"/>
+      <c r="R175" s="2"/>
+      <c r="S175" s="2"/>
+      <c r="T175" s="2">
         <v>18</v>
       </c>
-      <c r="U175" s="3" t="s">
+      <c r="U175" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="V175" s="3" t="str">
+      <c r="V175" s="2" t="str">
         <f>VLOOKUP(U175,fuente_financiamiento!A$1:B$4,2,0)</f>
         <v>18: CANON Y SOBRECANON, REGALIAS, RENTA DE ADUANAS Y PARTICIPACIONES</v>
       </c>
-      <c r="W175" s="3" t="s">
+      <c r="W175" s="2" t="s">
         <v>2817</v>
       </c>
-      <c r="X175" s="3" t="str">
+      <c r="X175" s="2" t="str">
         <f>VLOOKUP(W175,clasificador!A$1:B$1635,2,0)</f>
         <v>2.6. 2  2. 2  3: COSTO DE CONSTRUCCION POR ADMINISTRACION DIRECTA - PERSONAL</v>
       </c>
-      <c r="Y175" s="3">
+      <c r="Y175" s="2">
         <v>69</v>
       </c>
-      <c r="Z175" s="3" t="s">
+      <c r="Z175" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="AA175" s="3">
+      <c r="AA175" s="2">
         <v>4537.21</v>
       </c>
-      <c r="AB175" s="4">
+      <c r="AB175" s="3">
         <v>45716.697349849535</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB136" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -25706,219 +25700,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FF48C4-0B42-4380-95AC-0257E17CBFC1}">
-  <dimension ref="A1:A39"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
-        <v>45671</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>45681</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>45687</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>45687</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>45694</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>45694</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>45716</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>45716</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>45698</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>45699</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>45699</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>45714</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>45714</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>45714</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>45714</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>45714</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>45714</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>45714</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>45714</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>45714</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>45714</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>45716</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>45716</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>45716</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>45716</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>45693</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>45695</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>45695</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>45715</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>45715</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>45702</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>45702</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>45702</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>45702</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>45706</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>45716</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>45716</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>45716</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>45716</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6221D2DB-799F-4324-BBD2-ADABBC53D541}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -25968,7 +25749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5195F7-D3C3-4C49-8E44-49F942F20CCF}">
   <dimension ref="A1:B1635"/>
   <sheetViews>

</xml_diff>

<commit_message>
actualizacion de data siaf de opp
</commit_message>
<xml_diff>
--- a/data/ep_mes_2025.xlsx
+++ b/data/ep_mes_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6. Código\seguimiento_presupuestal_unsch_streamlit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D373BD79-3B53-4936-8211-F6E8E915143A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F7D877-62A9-45C7-B045-EFBA7850883F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5209" uniqueCount="3566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5209" uniqueCount="3565">
   <si>
     <t>ano_eje</t>
   </si>
@@ -10656,9 +10656,6 @@
   </si>
   <si>
     <t>ASIGNACIÓN EXTRAORDINARIA POR MOVILIDAD AL PERSONAL ADMINISTRATIVO</t>
-  </si>
-  <si>
-    <t>IMPLEMENTACION Y DESARROLLO DE ACTIVIDADES ADMINISTRATIVAS DE PLANIFICACION</t>
   </si>
   <si>
     <t>REALIZACIÓN DE LA TRANSFERENCIA A LA CONTRALORIA GENERAL DE LA REPÚBLICA PARA ACCIONES DE CONTROL</t>
@@ -11079,7 +11076,7 @@
   <cols>
     <col min="7" max="7" width="22.42578125" customWidth="1"/>
     <col min="8" max="8" width="78.42578125" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="82.7109375" customWidth="1"/>
     <col min="11" max="11" width="15.28515625" customWidth="1"/>
     <col min="15" max="15" width="43.85546875" customWidth="1"/>
     <col min="16" max="16" width="14" customWidth="1"/>
@@ -23088,7 +23085,7 @@
       <c r="M137" s="2"/>
       <c r="N137" s="2"/>
       <c r="O137" s="2" t="s">
-        <v>3541</v>
+        <v>3540</v>
       </c>
       <c r="P137" s="2" t="s">
         <v>32</v>
@@ -23154,7 +23151,7 @@
       <c r="M138" s="2"/>
       <c r="N138" s="2"/>
       <c r="O138" s="2" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
       <c r="P138" s="2" t="s">
         <v>32</v>
@@ -23183,7 +23180,7 @@
         <v>57</v>
       </c>
       <c r="Z138" s="2" t="s">
-        <v>3564</v>
+        <v>3563</v>
       </c>
       <c r="AA138" s="2">
         <v>40000</v>
@@ -23220,7 +23217,7 @@
       <c r="M139" s="2"/>
       <c r="N139" s="2"/>
       <c r="O139" s="2" t="s">
-        <v>3543</v>
+        <v>3542</v>
       </c>
       <c r="P139" s="2" t="s">
         <v>32</v>
@@ -23288,7 +23285,7 @@
       <c r="M140" s="2"/>
       <c r="N140" s="2"/>
       <c r="O140" s="2" t="s">
-        <v>3543</v>
+        <v>3542</v>
       </c>
       <c r="P140" s="2" t="s">
         <v>32</v>
@@ -23356,7 +23353,7 @@
       <c r="M141" s="2"/>
       <c r="N141" s="2"/>
       <c r="O141" s="2" t="s">
-        <v>3544</v>
+        <v>3543</v>
       </c>
       <c r="P141" s="2" t="s">
         <v>32</v>
@@ -23424,7 +23421,7 @@
       <c r="M142" s="2"/>
       <c r="N142" s="2"/>
       <c r="O142" s="2" t="s">
-        <v>3544</v>
+        <v>3543</v>
       </c>
       <c r="P142" s="2" t="s">
         <v>32</v>
@@ -23492,7 +23489,7 @@
       <c r="M143" s="2"/>
       <c r="N143" s="2"/>
       <c r="O143" s="2" t="s">
-        <v>3545</v>
+        <v>3544</v>
       </c>
       <c r="P143" s="2" t="s">
         <v>32</v>
@@ -23560,7 +23557,7 @@
       <c r="M144" s="2"/>
       <c r="N144" s="2"/>
       <c r="O144" s="2" t="s">
-        <v>3545</v>
+        <v>3544</v>
       </c>
       <c r="P144" s="2" t="s">
         <v>32</v>
@@ -23626,7 +23623,7 @@
       <c r="M145" s="2"/>
       <c r="N145" s="2"/>
       <c r="O145" s="2" t="s">
-        <v>3546</v>
+        <v>3545</v>
       </c>
       <c r="P145" s="2" t="s">
         <v>32</v>
@@ -23694,7 +23691,7 @@
       <c r="M146" s="2"/>
       <c r="N146" s="2"/>
       <c r="O146" s="2" t="s">
-        <v>3547</v>
+        <v>3546</v>
       </c>
       <c r="P146" s="2" t="s">
         <v>32</v>
@@ -23723,7 +23720,7 @@
         <v>63</v>
       </c>
       <c r="Z146" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="AA146" s="2">
         <v>54892.11</v>
@@ -23762,7 +23759,7 @@
       <c r="M147" s="2"/>
       <c r="N147" s="2"/>
       <c r="O147" s="2" t="s">
-        <v>3547</v>
+        <v>3546</v>
       </c>
       <c r="P147" s="2" t="s">
         <v>32</v>
@@ -23791,7 +23788,7 @@
         <v>63</v>
       </c>
       <c r="Z147" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="AA147" s="2">
         <v>12871.08</v>
@@ -23830,7 +23827,7 @@
       <c r="M148" s="2"/>
       <c r="N148" s="2"/>
       <c r="O148" s="2" t="s">
-        <v>3548</v>
+        <v>3547</v>
       </c>
       <c r="P148" s="2" t="s">
         <v>32</v>
@@ -23859,7 +23856,7 @@
         <v>63</v>
       </c>
       <c r="Z148" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="AA148" s="2">
         <v>5201.99</v>
@@ -23898,7 +23895,7 @@
       <c r="M149" s="2"/>
       <c r="N149" s="2"/>
       <c r="O149" s="2" t="s">
-        <v>3548</v>
+        <v>3547</v>
       </c>
       <c r="P149" s="2" t="s">
         <v>32</v>
@@ -23927,7 +23924,7 @@
         <v>63</v>
       </c>
       <c r="Z149" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="AA149" s="2">
         <v>446.69</v>
@@ -23966,7 +23963,7 @@
       <c r="M150" s="2"/>
       <c r="N150" s="2"/>
       <c r="O150" s="2" t="s">
-        <v>3549</v>
+        <v>3548</v>
       </c>
       <c r="P150" s="2" t="s">
         <v>32</v>
@@ -23995,7 +23992,7 @@
         <v>63</v>
       </c>
       <c r="Z150" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="AA150" s="2">
         <v>10286.459999999999</v>
@@ -24034,7 +24031,7 @@
       <c r="M151" s="2"/>
       <c r="N151" s="2"/>
       <c r="O151" s="2" t="s">
-        <v>3549</v>
+        <v>3548</v>
       </c>
       <c r="P151" s="2" t="s">
         <v>32</v>
@@ -24063,7 +24060,7 @@
         <v>63</v>
       </c>
       <c r="Z151" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="AA151" s="2">
         <v>312.25</v>
@@ -24102,7 +24099,7 @@
       <c r="M152" s="2"/>
       <c r="N152" s="2"/>
       <c r="O152" s="2" t="s">
-        <v>3550</v>
+        <v>3549</v>
       </c>
       <c r="P152" s="2" t="s">
         <v>32</v>
@@ -24131,7 +24128,7 @@
         <v>63</v>
       </c>
       <c r="Z152" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="AA152" s="2">
         <v>1163.76</v>
@@ -24170,7 +24167,7 @@
       <c r="M153" s="2"/>
       <c r="N153" s="2"/>
       <c r="O153" s="2" t="s">
-        <v>3550</v>
+        <v>3549</v>
       </c>
       <c r="P153" s="2" t="s">
         <v>32</v>
@@ -24199,7 +24196,7 @@
         <v>63</v>
       </c>
       <c r="Z153" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="AA153" s="2">
         <v>112.7</v>
@@ -24238,7 +24235,7 @@
       <c r="M154" s="2"/>
       <c r="N154" s="2"/>
       <c r="O154" s="2" t="s">
-        <v>3551</v>
+        <v>3550</v>
       </c>
       <c r="P154" s="2" t="s">
         <v>32</v>
@@ -24267,7 +24264,7 @@
         <v>63</v>
       </c>
       <c r="Z154" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="AA154" s="2">
         <v>7663.6</v>
@@ -24306,7 +24303,7 @@
       <c r="M155" s="2"/>
       <c r="N155" s="2"/>
       <c r="O155" s="2" t="s">
-        <v>3551</v>
+        <v>3550</v>
       </c>
       <c r="P155" s="2" t="s">
         <v>32</v>
@@ -24335,7 +24332,7 @@
         <v>63</v>
       </c>
       <c r="Z155" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="AA155" s="2">
         <v>1913.38</v>
@@ -24374,7 +24371,7 @@
       <c r="M156" s="2"/>
       <c r="N156" s="2"/>
       <c r="O156" s="2" t="s">
-        <v>3552</v>
+        <v>3551</v>
       </c>
       <c r="P156" s="2" t="s">
         <v>32</v>
@@ -24403,7 +24400,7 @@
         <v>63</v>
       </c>
       <c r="Z156" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="AA156" s="2">
         <v>5266.27</v>
@@ -24442,7 +24439,7 @@
       <c r="M157" s="2"/>
       <c r="N157" s="2"/>
       <c r="O157" s="2" t="s">
-        <v>3552</v>
+        <v>3551</v>
       </c>
       <c r="P157" s="2" t="s">
         <v>32</v>
@@ -24471,7 +24468,7 @@
         <v>63</v>
       </c>
       <c r="Z157" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="AA157" s="2">
         <v>9807.02</v>
@@ -24510,7 +24507,7 @@
       <c r="M158" s="2"/>
       <c r="N158" s="2"/>
       <c r="O158" s="2" t="s">
-        <v>3553</v>
+        <v>3552</v>
       </c>
       <c r="P158" s="2" t="s">
         <v>32</v>
@@ -24539,7 +24536,7 @@
         <v>63</v>
       </c>
       <c r="Z158" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="AA158" s="2">
         <v>257917.62</v>
@@ -24578,7 +24575,7 @@
       <c r="M159" s="2"/>
       <c r="N159" s="2"/>
       <c r="O159" s="2" t="s">
-        <v>3553</v>
+        <v>3552</v>
       </c>
       <c r="P159" s="2" t="s">
         <v>32</v>
@@ -24607,7 +24604,7 @@
         <v>63</v>
       </c>
       <c r="Z159" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="AA159" s="2">
         <v>55123.31</v>
@@ -24646,7 +24643,7 @@
       <c r="M160" s="2"/>
       <c r="N160" s="2"/>
       <c r="O160" s="2" t="s">
-        <v>3554</v>
+        <v>3553</v>
       </c>
       <c r="P160" s="2" t="s">
         <v>32</v>
@@ -24675,7 +24672,7 @@
         <v>63</v>
       </c>
       <c r="Z160" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="AA160" s="2">
         <v>67617.5</v>
@@ -24714,7 +24711,7 @@
       <c r="M161" s="2"/>
       <c r="N161" s="2"/>
       <c r="O161" s="2" t="s">
-        <v>3554</v>
+        <v>3553</v>
       </c>
       <c r="P161" s="2" t="s">
         <v>32</v>
@@ -24743,7 +24740,7 @@
         <v>63</v>
       </c>
       <c r="Z161" s="2" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="AA161" s="2">
         <v>15767.5</v>
@@ -24782,7 +24779,7 @@
       <c r="M162" s="2"/>
       <c r="N162" s="2"/>
       <c r="O162" s="2" t="s">
-        <v>3555</v>
+        <v>3554</v>
       </c>
       <c r="P162" s="2" t="s">
         <v>32</v>
@@ -24848,7 +24845,7 @@
       <c r="M163" s="2"/>
       <c r="N163" s="2"/>
       <c r="O163" s="2" t="s">
-        <v>3556</v>
+        <v>3555</v>
       </c>
       <c r="P163" s="2" t="s">
         <v>32</v>
@@ -24914,7 +24911,7 @@
       <c r="M164" s="2"/>
       <c r="N164" s="2"/>
       <c r="O164" s="2" t="s">
-        <v>3556</v>
+        <v>3555</v>
       </c>
       <c r="P164" s="2" t="s">
         <v>32</v>
@@ -24980,7 +24977,7 @@
       <c r="M165" s="2"/>
       <c r="N165" s="2"/>
       <c r="O165" s="2" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
       <c r="P165" s="2" t="s">
         <v>32</v>
@@ -25046,7 +25043,7 @@
       <c r="M166" s="2"/>
       <c r="N166" s="2"/>
       <c r="O166" s="2" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
       <c r="P166" s="2" t="s">
         <v>32</v>
@@ -25107,14 +25104,14 @@
         <v>196</v>
       </c>
       <c r="J167" s="2" t="s">
-        <v>3539</v>
+        <v>209</v>
       </c>
       <c r="K167" s="2"/>
       <c r="L167" s="2"/>
       <c r="M167" s="2"/>
       <c r="N167" s="2"/>
       <c r="O167" s="2" t="s">
-        <v>3558</v>
+        <v>3557</v>
       </c>
       <c r="P167" s="2" t="s">
         <v>32</v>
@@ -25173,14 +25170,14 @@
       </c>
       <c r="I168" s="2"/>
       <c r="J168" s="2" t="s">
-        <v>3540</v>
+        <v>3539</v>
       </c>
       <c r="K168" s="2"/>
       <c r="L168" s="2"/>
       <c r="M168" s="2"/>
       <c r="N168" s="2"/>
       <c r="O168" s="2" t="s">
-        <v>3559</v>
+        <v>3558</v>
       </c>
       <c r="P168" s="2" t="s">
         <v>32</v>
@@ -25248,7 +25245,7 @@
       <c r="M169" s="2"/>
       <c r="N169" s="2"/>
       <c r="O169" s="2" t="s">
-        <v>3560</v>
+        <v>3559</v>
       </c>
       <c r="P169" s="2" t="s">
         <v>32</v>
@@ -25316,7 +25313,7 @@
       <c r="M170" s="2"/>
       <c r="N170" s="2"/>
       <c r="O170" s="2" t="s">
-        <v>3560</v>
+        <v>3559</v>
       </c>
       <c r="P170" s="2" t="s">
         <v>32</v>
@@ -25382,7 +25379,7 @@
       <c r="M171" s="2"/>
       <c r="N171" s="2"/>
       <c r="O171" s="2" t="s">
-        <v>3561</v>
+        <v>3560</v>
       </c>
       <c r="P171" s="2" t="s">
         <v>32</v>
@@ -25411,7 +25408,7 @@
         <v>57</v>
       </c>
       <c r="Z171" s="2" t="s">
-        <v>3564</v>
+        <v>3563</v>
       </c>
       <c r="AA171" s="2">
         <v>50000</v>
@@ -25450,7 +25447,7 @@
       <c r="M172" s="2"/>
       <c r="N172" s="2"/>
       <c r="O172" s="2" t="s">
-        <v>3562</v>
+        <v>3561</v>
       </c>
       <c r="P172" s="2" t="s">
         <v>32</v>
@@ -25518,7 +25515,7 @@
       <c r="M173" s="2"/>
       <c r="N173" s="2"/>
       <c r="O173" s="2" t="s">
-        <v>3562</v>
+        <v>3561</v>
       </c>
       <c r="P173" s="2" t="s">
         <v>32</v>
@@ -25586,7 +25583,7 @@
       <c r="M174" s="2"/>
       <c r="N174" s="2"/>
       <c r="O174" s="2" t="s">
-        <v>3563</v>
+        <v>3562</v>
       </c>
       <c r="P174" s="2" t="s">
         <v>32</v>
@@ -25654,7 +25651,7 @@
       <c r="M175" s="2"/>
       <c r="N175" s="2"/>
       <c r="O175" s="2" t="s">
-        <v>3563</v>
+        <v>3562</v>
       </c>
       <c r="P175" s="2" t="s">
         <v>32</v>

</xml_diff>